<commit_message>
update file sau khi review
</commit_message>
<xml_diff>
--- a/Document/Design/SDD_UserManager.xlsx
+++ b/Document/Design/SDD_UserManager.xlsx
@@ -1072,7 +1072,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="130">
   <si>
     <t>&lt;Project Name&gt;</t>
   </si>
@@ -1401,15 +1401,9 @@
     <t>Display</t>
   </si>
   <si>
-    <t>checkbox ( tick chọn User trong bảng danh sách User)</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
-    <t>All(Tất cả column)</t>
-  </si>
-  <si>
     <t>cboSelectGroup(chọn user theo group)</t>
   </si>
   <si>
@@ -1465,6 +1459,9 @@
   </si>
   <si>
     <t>UserManager</t>
+  </si>
+  <si>
+    <t>21/10/2011</t>
   </si>
 </sst>
 </file>
@@ -2595,40 +2592,215 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2640,181 +2812,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3182,14 +3179,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="33">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1" t="s">
@@ -3409,12 +3406,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="33">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
     </row>
     <row r="5" spans="2:5" ht="15.75">
       <c r="B5" s="21" t="s">
@@ -3476,16 +3473,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="33">
-      <c r="B2" s="89" t="s">
+      <c r="B2" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
     </row>
     <row r="4" spans="2:4" ht="15">
       <c r="B4" s="22"/>
-      <c r="C4" s="162" t="s">
-        <v>130</v>
+      <c r="C4" s="89" t="s">
+        <v>128</v>
       </c>
       <c r="D4" s="23"/>
     </row>
@@ -3657,7 +3654,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="BB5" sqref="BB5:BE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="12.75"/>
@@ -3681,307 +3678,311 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:57">
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97" t="s">
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97"/>
-      <c r="M2" s="97"/>
-      <c r="N2" s="97"/>
-      <c r="O2" s="97"/>
-      <c r="P2" s="97"/>
-      <c r="Q2" s="97"/>
-      <c r="R2" s="97"/>
-      <c r="S2" s="97"/>
-      <c r="T2" s="97"/>
-      <c r="U2" s="97"/>
-      <c r="V2" s="97"/>
-      <c r="W2" s="97"/>
-      <c r="X2" s="97"/>
-      <c r="Y2" s="97"/>
-      <c r="Z2" s="97"/>
-      <c r="AA2" s="97"/>
-      <c r="AB2" s="97"/>
-      <c r="AC2" s="97"/>
-      <c r="AD2" s="97"/>
-      <c r="AE2" s="97"/>
-      <c r="AF2" s="97"/>
-      <c r="AG2" s="97"/>
-      <c r="AH2" s="97"/>
-      <c r="AI2" s="97"/>
-      <c r="AJ2" s="97"/>
-      <c r="AK2" s="97"/>
-      <c r="AL2" s="97"/>
-      <c r="AM2" s="97"/>
-      <c r="AN2" s="97"/>
-      <c r="AO2" s="97"/>
-      <c r="AP2" s="97"/>
-      <c r="AQ2" s="99" t="s">
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="92"/>
+      <c r="L2" s="92"/>
+      <c r="M2" s="92"/>
+      <c r="N2" s="92"/>
+      <c r="O2" s="92"/>
+      <c r="P2" s="92"/>
+      <c r="Q2" s="92"/>
+      <c r="R2" s="92"/>
+      <c r="S2" s="92"/>
+      <c r="T2" s="92"/>
+      <c r="U2" s="92"/>
+      <c r="V2" s="92"/>
+      <c r="W2" s="92"/>
+      <c r="X2" s="92"/>
+      <c r="Y2" s="92"/>
+      <c r="Z2" s="92"/>
+      <c r="AA2" s="92"/>
+      <c r="AB2" s="92"/>
+      <c r="AC2" s="92"/>
+      <c r="AD2" s="92"/>
+      <c r="AE2" s="92"/>
+      <c r="AF2" s="92"/>
+      <c r="AG2" s="92"/>
+      <c r="AH2" s="92"/>
+      <c r="AI2" s="92"/>
+      <c r="AJ2" s="92"/>
+      <c r="AK2" s="92"/>
+      <c r="AL2" s="92"/>
+      <c r="AM2" s="92"/>
+      <c r="AN2" s="92"/>
+      <c r="AO2" s="92"/>
+      <c r="AP2" s="92"/>
+      <c r="AQ2" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="AR2" s="99"/>
-      <c r="AS2" s="99"/>
-      <c r="AT2" s="99"/>
-      <c r="AU2" s="99"/>
-      <c r="AV2" s="99"/>
-      <c r="AW2" s="99"/>
-      <c r="AX2" s="99" t="s">
+      <c r="AR2" s="93"/>
+      <c r="AS2" s="93"/>
+      <c r="AT2" s="93"/>
+      <c r="AU2" s="93"/>
+      <c r="AV2" s="93"/>
+      <c r="AW2" s="93"/>
+      <c r="AX2" s="93" t="s">
         <v>22</v>
       </c>
-      <c r="AY2" s="99"/>
-      <c r="AZ2" s="99"/>
-      <c r="BA2" s="99"/>
-      <c r="BB2" s="99"/>
-      <c r="BC2" s="99"/>
-      <c r="BD2" s="99"/>
-      <c r="BE2" s="99"/>
+      <c r="AY2" s="93"/>
+      <c r="AZ2" s="93"/>
+      <c r="BA2" s="93"/>
+      <c r="BB2" s="93"/>
+      <c r="BC2" s="93"/>
+      <c r="BD2" s="93"/>
+      <c r="BE2" s="93"/>
     </row>
     <row r="3" spans="2:57">
-      <c r="B3" s="96"/>
-      <c r="C3" s="96"/>
-      <c r="D3" s="96"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97"/>
-      <c r="H3" s="97"/>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="97"/>
-      <c r="N3" s="97"/>
-      <c r="O3" s="97"/>
-      <c r="P3" s="97"/>
-      <c r="Q3" s="97"/>
-      <c r="R3" s="97"/>
-      <c r="S3" s="97"/>
-      <c r="T3" s="97"/>
-      <c r="U3" s="97"/>
-      <c r="V3" s="97"/>
-      <c r="W3" s="97"/>
-      <c r="X3" s="97"/>
-      <c r="Y3" s="97"/>
-      <c r="Z3" s="97"/>
-      <c r="AA3" s="97"/>
-      <c r="AB3" s="97"/>
-      <c r="AC3" s="97"/>
-      <c r="AD3" s="97"/>
-      <c r="AE3" s="97"/>
-      <c r="AF3" s="97"/>
-      <c r="AG3" s="97"/>
-      <c r="AH3" s="97"/>
-      <c r="AI3" s="97"/>
-      <c r="AJ3" s="97"/>
-      <c r="AK3" s="97"/>
-      <c r="AL3" s="97"/>
-      <c r="AM3" s="97"/>
-      <c r="AN3" s="97"/>
-      <c r="AO3" s="97"/>
-      <c r="AP3" s="97"/>
-      <c r="AQ3" s="100" t="s">
+      <c r="B3" s="91"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="92"/>
+      <c r="R3" s="92"/>
+      <c r="S3" s="92"/>
+      <c r="T3" s="92"/>
+      <c r="U3" s="92"/>
+      <c r="V3" s="92"/>
+      <c r="W3" s="92"/>
+      <c r="X3" s="92"/>
+      <c r="Y3" s="92"/>
+      <c r="Z3" s="92"/>
+      <c r="AA3" s="92"/>
+      <c r="AB3" s="92"/>
+      <c r="AC3" s="92"/>
+      <c r="AD3" s="92"/>
+      <c r="AE3" s="92"/>
+      <c r="AF3" s="92"/>
+      <c r="AG3" s="92"/>
+      <c r="AH3" s="92"/>
+      <c r="AI3" s="92"/>
+      <c r="AJ3" s="92"/>
+      <c r="AK3" s="92"/>
+      <c r="AL3" s="92"/>
+      <c r="AM3" s="92"/>
+      <c r="AN3" s="92"/>
+      <c r="AO3" s="92"/>
+      <c r="AP3" s="92"/>
+      <c r="AQ3" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="AR3" s="100"/>
-      <c r="AS3" s="100"/>
-      <c r="AT3" s="100"/>
-      <c r="AU3" s="100"/>
-      <c r="AV3" s="100"/>
-      <c r="AW3" s="100"/>
-      <c r="AX3" s="100" t="s">
-        <v>128</v>
-      </c>
-      <c r="AY3" s="100"/>
-      <c r="AZ3" s="100"/>
-      <c r="BA3" s="100"/>
-      <c r="BB3" s="100"/>
-      <c r="BC3" s="100"/>
-      <c r="BD3" s="100"/>
-      <c r="BE3" s="100"/>
+      <c r="AR3" s="94"/>
+      <c r="AS3" s="94"/>
+      <c r="AT3" s="94"/>
+      <c r="AU3" s="94"/>
+      <c r="AV3" s="94"/>
+      <c r="AW3" s="94"/>
+      <c r="AX3" s="94" t="s">
+        <v>126</v>
+      </c>
+      <c r="AY3" s="94"/>
+      <c r="AZ3" s="94"/>
+      <c r="BA3" s="94"/>
+      <c r="BB3" s="94"/>
+      <c r="BC3" s="94"/>
+      <c r="BD3" s="94"/>
+      <c r="BE3" s="94"/>
     </row>
     <row r="4" spans="2:57">
-      <c r="B4" s="139" t="s">
+      <c r="B4" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="139"/>
-      <c r="D4" s="139"/>
-      <c r="E4" s="140"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
-      <c r="L4" s="98"/>
-      <c r="M4" s="98"/>
-      <c r="N4" s="98"/>
-      <c r="O4" s="143" t="s">
+      <c r="C4" s="146"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="147"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="95"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="95"/>
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="99" t="s">
         <v>27</v>
       </c>
-      <c r="P4" s="141"/>
-      <c r="Q4" s="141"/>
-      <c r="R4" s="141"/>
-      <c r="S4" s="141"/>
-      <c r="T4" s="142"/>
-      <c r="U4" s="98" t="s">
+      <c r="P4" s="100"/>
+      <c r="Q4" s="100"/>
+      <c r="R4" s="100"/>
+      <c r="S4" s="100"/>
+      <c r="T4" s="101"/>
+      <c r="U4" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="V4" s="98"/>
-      <c r="W4" s="98"/>
-      <c r="X4" s="98"/>
-      <c r="Y4" s="98"/>
-      <c r="Z4" s="98"/>
-      <c r="AA4" s="98"/>
-      <c r="AB4" s="98"/>
-      <c r="AC4" s="98"/>
-      <c r="AD4" s="98"/>
-      <c r="AE4" s="98"/>
-      <c r="AF4" s="98"/>
-      <c r="AG4" s="98"/>
-      <c r="AH4" s="98"/>
-      <c r="AI4" s="98"/>
-      <c r="AJ4" s="98"/>
-      <c r="AK4" s="98"/>
-      <c r="AL4" s="98"/>
-      <c r="AM4" s="98"/>
-      <c r="AN4" s="98"/>
-      <c r="AO4" s="98"/>
-      <c r="AP4" s="98"/>
-      <c r="AQ4" s="144" t="s">
+      <c r="V4" s="95"/>
+      <c r="W4" s="95"/>
+      <c r="X4" s="95"/>
+      <c r="Y4" s="95"/>
+      <c r="Z4" s="95"/>
+      <c r="AA4" s="95"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="95"/>
+      <c r="AD4" s="95"/>
+      <c r="AE4" s="95"/>
+      <c r="AF4" s="95"/>
+      <c r="AG4" s="95"/>
+      <c r="AH4" s="95"/>
+      <c r="AI4" s="95"/>
+      <c r="AJ4" s="95"/>
+      <c r="AK4" s="95"/>
+      <c r="AL4" s="95"/>
+      <c r="AM4" s="95"/>
+      <c r="AN4" s="95"/>
+      <c r="AO4" s="95"/>
+      <c r="AP4" s="95"/>
+      <c r="AQ4" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="AR4" s="145"/>
-      <c r="AS4" s="146"/>
-      <c r="AT4" s="98" t="s">
+      <c r="AR4" s="97"/>
+      <c r="AS4" s="98"/>
+      <c r="AT4" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="AU4" s="98"/>
-      <c r="AV4" s="98"/>
-      <c r="AW4" s="98"/>
-      <c r="AX4" s="144" t="s">
+      <c r="AU4" s="95"/>
+      <c r="AV4" s="95"/>
+      <c r="AW4" s="95"/>
+      <c r="AX4" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="AY4" s="145"/>
-      <c r="AZ4" s="145"/>
-      <c r="BA4" s="146"/>
-      <c r="BB4" s="98" t="s">
+      <c r="AY4" s="97"/>
+      <c r="AZ4" s="97"/>
+      <c r="BA4" s="98"/>
+      <c r="BB4" s="95" t="s">
+        <v>127</v>
+      </c>
+      <c r="BC4" s="95"/>
+      <c r="BD4" s="95"/>
+      <c r="BE4" s="95"/>
+    </row>
+    <row r="5" spans="2:57">
+      <c r="B5" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="95"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="95"/>
+      <c r="O5" s="99" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="100"/>
+      <c r="Q5" s="100"/>
+      <c r="R5" s="100"/>
+      <c r="S5" s="100"/>
+      <c r="T5" s="101"/>
+      <c r="U5" s="95"/>
+      <c r="V5" s="95"/>
+      <c r="W5" s="95"/>
+      <c r="X5" s="95"/>
+      <c r="Y5" s="95"/>
+      <c r="Z5" s="95"/>
+      <c r="AA5" s="95"/>
+      <c r="AB5" s="95"/>
+      <c r="AC5" s="95"/>
+      <c r="AD5" s="95"/>
+      <c r="AE5" s="95"/>
+      <c r="AF5" s="95"/>
+      <c r="AG5" s="95"/>
+      <c r="AH5" s="95"/>
+      <c r="AI5" s="95"/>
+      <c r="AJ5" s="95"/>
+      <c r="AK5" s="95"/>
+      <c r="AL5" s="95"/>
+      <c r="AM5" s="95"/>
+      <c r="AN5" s="95"/>
+      <c r="AO5" s="95"/>
+      <c r="AP5" s="95"/>
+      <c r="AQ5" s="99" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR5" s="148"/>
+      <c r="AS5" s="101"/>
+      <c r="AT5" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU5" s="95"/>
+      <c r="AV5" s="95"/>
+      <c r="AW5" s="95"/>
+      <c r="AX5" s="99" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY5" s="100"/>
+      <c r="AZ5" s="100"/>
+      <c r="BA5" s="101"/>
+      <c r="BB5" s="95" t="s">
         <v>129</v>
       </c>
-      <c r="BC4" s="98"/>
-      <c r="BD4" s="98"/>
-      <c r="BE4" s="98"/>
-    </row>
-    <row r="5" spans="2:57">
-      <c r="B5" s="141" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141"/>
-      <c r="E5" s="142"/>
-      <c r="F5" s="98"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="98"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
-      <c r="L5" s="98"/>
-      <c r="M5" s="98"/>
-      <c r="N5" s="98"/>
-      <c r="O5" s="143" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="141"/>
-      <c r="Q5" s="141"/>
-      <c r="R5" s="141"/>
-      <c r="S5" s="141"/>
-      <c r="T5" s="142"/>
-      <c r="U5" s="98"/>
-      <c r="V5" s="98"/>
-      <c r="W5" s="98"/>
-      <c r="X5" s="98"/>
-      <c r="Y5" s="98"/>
-      <c r="Z5" s="98"/>
-      <c r="AA5" s="98"/>
-      <c r="AB5" s="98"/>
-      <c r="AC5" s="98"/>
-      <c r="AD5" s="98"/>
-      <c r="AE5" s="98"/>
-      <c r="AF5" s="98"/>
-      <c r="AG5" s="98"/>
-      <c r="AH5" s="98"/>
-      <c r="AI5" s="98"/>
-      <c r="AJ5" s="98"/>
-      <c r="AK5" s="98"/>
-      <c r="AL5" s="98"/>
-      <c r="AM5" s="98"/>
-      <c r="AN5" s="98"/>
-      <c r="AO5" s="98"/>
-      <c r="AP5" s="98"/>
-      <c r="AQ5" s="143" t="s">
-        <v>23</v>
-      </c>
-      <c r="AR5" s="147"/>
-      <c r="AS5" s="142"/>
-      <c r="AT5" s="98"/>
-      <c r="AU5" s="98"/>
-      <c r="AV5" s="98"/>
-      <c r="AW5" s="98"/>
-      <c r="AX5" s="143" t="s">
-        <v>24</v>
-      </c>
-      <c r="AY5" s="141"/>
-      <c r="AZ5" s="141"/>
-      <c r="BA5" s="142"/>
-      <c r="BB5" s="98"/>
-      <c r="BC5" s="98"/>
-      <c r="BD5" s="98"/>
-      <c r="BE5" s="98"/>
+      <c r="BC5" s="95"/>
+      <c r="BD5" s="95"/>
+      <c r="BE5" s="95"/>
     </row>
     <row r="7" spans="2:57">
-      <c r="C7" s="148" t="s">
+      <c r="C7" s="144" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="148"/>
-      <c r="E7" s="148"/>
-      <c r="F7" s="148"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="148"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="144"/>
+      <c r="H7" s="144"/>
     </row>
     <row r="9" spans="2:57" ht="13.5" thickBot="1">
       <c r="C9" s="32"/>
     </row>
     <row r="10" spans="2:57" ht="15" customHeight="1">
-      <c r="D10" s="127" t="s">
+      <c r="D10" s="110" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="128"/>
-      <c r="F10" s="128"/>
-      <c r="G10" s="129"/>
-      <c r="H10" s="153" t="s">
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
+      <c r="G10" s="112"/>
+      <c r="H10" s="128" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="153"/>
-      <c r="J10" s="153"/>
-      <c r="K10" s="153"/>
-      <c r="L10" s="153"/>
-      <c r="M10" s="153"/>
-      <c r="N10" s="153"/>
-      <c r="O10" s="153"/>
-      <c r="P10" s="153"/>
-      <c r="Q10" s="153"/>
-      <c r="R10" s="153"/>
-      <c r="S10" s="153"/>
-      <c r="T10" s="153"/>
-      <c r="U10" s="153"/>
+      <c r="I10" s="128"/>
+      <c r="J10" s="128"/>
+      <c r="K10" s="128"/>
+      <c r="L10" s="128"/>
+      <c r="M10" s="128"/>
+      <c r="N10" s="128"/>
+      <c r="O10" s="128"/>
+      <c r="P10" s="128"/>
+      <c r="Q10" s="128"/>
+      <c r="R10" s="128"/>
+      <c r="S10" s="128"/>
+      <c r="T10" s="128"/>
+      <c r="U10" s="128"/>
       <c r="V10" s="70"/>
       <c r="W10" s="70"/>
       <c r="X10" s="70"/>
@@ -4018,24 +4019,24 @@
       <c r="BC10" s="71"/>
     </row>
     <row r="11" spans="2:57" ht="13.5" thickBot="1">
-      <c r="D11" s="150"/>
-      <c r="E11" s="151"/>
-      <c r="F11" s="151"/>
-      <c r="G11" s="152"/>
-      <c r="H11" s="154"/>
-      <c r="I11" s="154"/>
-      <c r="J11" s="154"/>
-      <c r="K11" s="154"/>
-      <c r="L11" s="154"/>
-      <c r="M11" s="154"/>
-      <c r="N11" s="154"/>
-      <c r="O11" s="154"/>
-      <c r="P11" s="154"/>
-      <c r="Q11" s="154"/>
-      <c r="R11" s="154"/>
-      <c r="S11" s="154"/>
-      <c r="T11" s="154"/>
-      <c r="U11" s="154"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="126"/>
+      <c r="F11" s="126"/>
+      <c r="G11" s="127"/>
+      <c r="H11" s="129"/>
+      <c r="I11" s="129"/>
+      <c r="J11" s="129"/>
+      <c r="K11" s="129"/>
+      <c r="L11" s="129"/>
+      <c r="M11" s="129"/>
+      <c r="N11" s="129"/>
+      <c r="O11" s="129"/>
+      <c r="P11" s="129"/>
+      <c r="Q11" s="129"/>
+      <c r="R11" s="129"/>
+      <c r="S11" s="129"/>
+      <c r="T11" s="129"/>
+      <c r="U11" s="129"/>
       <c r="V11" s="72"/>
       <c r="W11" s="72"/>
       <c r="X11" s="72"/>
@@ -4072,24 +4073,24 @@
       <c r="BC11" s="73"/>
     </row>
     <row r="12" spans="2:57" ht="15" customHeight="1">
-      <c r="D12" s="150"/>
-      <c r="E12" s="151"/>
-      <c r="F12" s="151"/>
-      <c r="G12" s="152"/>
-      <c r="H12" s="154"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="154"/>
-      <c r="K12" s="154"/>
-      <c r="L12" s="154"/>
-      <c r="M12" s="154"/>
-      <c r="N12" s="154"/>
-      <c r="O12" s="154"/>
-      <c r="P12" s="154"/>
-      <c r="Q12" s="154"/>
-      <c r="R12" s="154"/>
-      <c r="S12" s="154"/>
-      <c r="T12" s="154"/>
-      <c r="U12" s="154"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="126"/>
+      <c r="F12" s="126"/>
+      <c r="G12" s="127"/>
+      <c r="H12" s="129"/>
+      <c r="I12" s="129"/>
+      <c r="J12" s="129"/>
+      <c r="K12" s="129"/>
+      <c r="L12" s="129"/>
+      <c r="M12" s="129"/>
+      <c r="N12" s="129"/>
+      <c r="O12" s="129"/>
+      <c r="P12" s="129"/>
+      <c r="Q12" s="129"/>
+      <c r="R12" s="129"/>
+      <c r="S12" s="129"/>
+      <c r="T12" s="129"/>
+      <c r="U12" s="129"/>
       <c r="V12" s="72"/>
       <c r="W12" s="72"/>
       <c r="X12" s="72"/>
@@ -4101,59 +4102,59 @@
       <c r="AD12" s="72"/>
       <c r="AE12" s="72"/>
       <c r="AF12" s="72"/>
-      <c r="AG12" s="133" t="s">
+      <c r="AG12" s="149" t="s">
         <v>88</v>
       </c>
-      <c r="AH12" s="134"/>
-      <c r="AI12" s="134"/>
-      <c r="AJ12" s="135"/>
+      <c r="AH12" s="150"/>
+      <c r="AI12" s="150"/>
+      <c r="AJ12" s="151"/>
       <c r="AK12" s="72"/>
-      <c r="AL12" s="127" t="s">
+      <c r="AL12" s="110" t="s">
         <v>89</v>
       </c>
-      <c r="AM12" s="128"/>
-      <c r="AN12" s="129"/>
+      <c r="AM12" s="111"/>
+      <c r="AN12" s="112"/>
       <c r="AO12" s="72"/>
-      <c r="AP12" s="127" t="s">
+      <c r="AP12" s="110" t="s">
         <v>90</v>
       </c>
-      <c r="AQ12" s="128"/>
-      <c r="AR12" s="129"/>
+      <c r="AQ12" s="111"/>
+      <c r="AR12" s="112"/>
       <c r="AS12" s="72"/>
-      <c r="AT12" s="127" t="s">
+      <c r="AT12" s="110" t="s">
         <v>91</v>
       </c>
-      <c r="AU12" s="128"/>
-      <c r="AV12" s="129"/>
+      <c r="AU12" s="111"/>
+      <c r="AV12" s="112"/>
       <c r="AW12" s="75"/>
-      <c r="AX12" s="127" t="s">
+      <c r="AX12" s="110" t="s">
         <v>92</v>
       </c>
-      <c r="AY12" s="128"/>
-      <c r="AZ12" s="129"/>
+      <c r="AY12" s="111"/>
+      <c r="AZ12" s="112"/>
       <c r="BA12" s="72"/>
       <c r="BB12" s="72"/>
       <c r="BC12" s="73"/>
     </row>
     <row r="13" spans="2:57" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D13" s="150"/>
-      <c r="E13" s="151"/>
-      <c r="F13" s="151"/>
-      <c r="G13" s="152"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
-      <c r="L13" s="154"/>
-      <c r="M13" s="154"/>
-      <c r="N13" s="154"/>
-      <c r="O13" s="154"/>
-      <c r="P13" s="154"/>
-      <c r="Q13" s="154"/>
-      <c r="R13" s="154"/>
-      <c r="S13" s="154"/>
-      <c r="T13" s="154"/>
-      <c r="U13" s="154"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="126"/>
+      <c r="F13" s="126"/>
+      <c r="G13" s="127"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="129"/>
+      <c r="J13" s="129"/>
+      <c r="K13" s="129"/>
+      <c r="L13" s="129"/>
+      <c r="M13" s="129"/>
+      <c r="N13" s="129"/>
+      <c r="O13" s="129"/>
+      <c r="P13" s="129"/>
+      <c r="Q13" s="129"/>
+      <c r="R13" s="129"/>
+      <c r="S13" s="129"/>
+      <c r="T13" s="129"/>
+      <c r="U13" s="129"/>
       <c r="V13" s="72"/>
       <c r="W13" s="72"/>
       <c r="X13" s="72"/>
@@ -4165,49 +4166,49 @@
       <c r="AD13" s="72"/>
       <c r="AE13" s="72"/>
       <c r="AF13" s="72"/>
-      <c r="AG13" s="136"/>
-      <c r="AH13" s="137"/>
-      <c r="AI13" s="137"/>
-      <c r="AJ13" s="138"/>
+      <c r="AG13" s="152"/>
+      <c r="AH13" s="153"/>
+      <c r="AI13" s="153"/>
+      <c r="AJ13" s="154"/>
       <c r="AK13" s="72"/>
-      <c r="AL13" s="130"/>
-      <c r="AM13" s="131"/>
-      <c r="AN13" s="132"/>
+      <c r="AL13" s="113"/>
+      <c r="AM13" s="114"/>
+      <c r="AN13" s="115"/>
       <c r="AO13" s="72"/>
-      <c r="AP13" s="130"/>
-      <c r="AQ13" s="131"/>
-      <c r="AR13" s="132"/>
+      <c r="AP13" s="113"/>
+      <c r="AQ13" s="114"/>
+      <c r="AR13" s="115"/>
       <c r="AS13" s="72"/>
-      <c r="AT13" s="130"/>
-      <c r="AU13" s="131"/>
-      <c r="AV13" s="132"/>
+      <c r="AT13" s="113"/>
+      <c r="AU13" s="114"/>
+      <c r="AV13" s="115"/>
       <c r="AW13" s="75"/>
-      <c r="AX13" s="130"/>
-      <c r="AY13" s="131"/>
-      <c r="AZ13" s="132"/>
+      <c r="AX13" s="113"/>
+      <c r="AY13" s="114"/>
+      <c r="AZ13" s="115"/>
       <c r="BA13" s="72"/>
       <c r="BB13" s="72"/>
       <c r="BC13" s="73"/>
     </row>
     <row r="14" spans="2:57">
-      <c r="D14" s="150"/>
-      <c r="E14" s="151"/>
-      <c r="F14" s="151"/>
-      <c r="G14" s="152"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
-      <c r="L14" s="154"/>
-      <c r="M14" s="154"/>
-      <c r="N14" s="154"/>
-      <c r="O14" s="154"/>
-      <c r="P14" s="154"/>
-      <c r="Q14" s="154"/>
-      <c r="R14" s="154"/>
-      <c r="S14" s="154"/>
-      <c r="T14" s="154"/>
-      <c r="U14" s="154"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="127"/>
+      <c r="H14" s="129"/>
+      <c r="I14" s="129"/>
+      <c r="J14" s="129"/>
+      <c r="K14" s="129"/>
+      <c r="L14" s="129"/>
+      <c r="M14" s="129"/>
+      <c r="N14" s="129"/>
+      <c r="O14" s="129"/>
+      <c r="P14" s="129"/>
+      <c r="Q14" s="129"/>
+      <c r="R14" s="129"/>
+      <c r="S14" s="129"/>
+      <c r="T14" s="129"/>
+      <c r="U14" s="129"/>
       <c r="V14" s="72"/>
       <c r="W14" s="72"/>
       <c r="X14" s="72"/>
@@ -4244,24 +4245,24 @@
       <c r="BC14" s="73"/>
     </row>
     <row r="15" spans="2:57">
-      <c r="D15" s="150"/>
-      <c r="E15" s="151"/>
-      <c r="F15" s="151"/>
-      <c r="G15" s="152"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
-      <c r="L15" s="154"/>
-      <c r="M15" s="154"/>
-      <c r="N15" s="154"/>
-      <c r="O15" s="154"/>
-      <c r="P15" s="154"/>
-      <c r="Q15" s="154"/>
-      <c r="R15" s="154"/>
-      <c r="S15" s="154"/>
-      <c r="T15" s="154"/>
-      <c r="U15" s="154"/>
+      <c r="D15" s="125"/>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126"/>
+      <c r="G15" s="127"/>
+      <c r="H15" s="129"/>
+      <c r="I15" s="129"/>
+      <c r="J15" s="129"/>
+      <c r="K15" s="129"/>
+      <c r="L15" s="129"/>
+      <c r="M15" s="129"/>
+      <c r="N15" s="129"/>
+      <c r="O15" s="129"/>
+      <c r="P15" s="129"/>
+      <c r="Q15" s="129"/>
+      <c r="R15" s="129"/>
+      <c r="S15" s="129"/>
+      <c r="T15" s="129"/>
+      <c r="U15" s="129"/>
       <c r="V15" s="72"/>
       <c r="W15" s="72"/>
       <c r="X15" s="72"/>
@@ -4520,19 +4521,19 @@
         <v>93</v>
       </c>
       <c r="G20" s="44"/>
-      <c r="H20" s="124"/>
-      <c r="I20" s="125"/>
-      <c r="J20" s="126"/>
+      <c r="H20" s="116"/>
+      <c r="I20" s="117"/>
+      <c r="J20" s="118"/>
       <c r="K20" s="44"/>
-      <c r="L20" s="124" t="s">
+      <c r="L20" s="116" t="s">
         <v>94</v>
       </c>
-      <c r="M20" s="126"/>
+      <c r="M20" s="118"/>
       <c r="N20" s="44"/>
-      <c r="O20" s="124" t="s">
+      <c r="O20" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="P20" s="126"/>
+      <c r="P20" s="118"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="44"/>
       <c r="S20" s="44"/>
@@ -4556,25 +4557,25 @@
       <c r="AK20" s="44"/>
       <c r="AL20" s="44"/>
       <c r="AM20" s="44"/>
-      <c r="AN20" s="124" t="s">
+      <c r="AN20" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="AO20" s="125"/>
-      <c r="AP20" s="125"/>
-      <c r="AQ20" s="125"/>
-      <c r="AR20" s="126"/>
+      <c r="AO20" s="117"/>
+      <c r="AP20" s="117"/>
+      <c r="AQ20" s="117"/>
+      <c r="AR20" s="118"/>
       <c r="AS20" s="78" t="s">
         <v>85</v>
       </c>
       <c r="AT20" s="44"/>
       <c r="AU20" s="44"/>
-      <c r="AV20" s="124" t="s">
+      <c r="AV20" s="116" t="s">
         <v>97</v>
       </c>
-      <c r="AW20" s="125"/>
-      <c r="AX20" s="125"/>
-      <c r="AY20" s="125"/>
-      <c r="AZ20" s="126"/>
+      <c r="AW20" s="117"/>
+      <c r="AX20" s="117"/>
+      <c r="AY20" s="117"/>
+      <c r="AZ20" s="118"/>
       <c r="BA20" s="78" t="s">
         <v>85</v>
       </c>
@@ -4640,13 +4641,13 @@
       <c r="E22" s="60"/>
       <c r="F22" s="44"/>
       <c r="G22" s="44"/>
-      <c r="H22" s="155" t="s">
+      <c r="H22" s="137" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="155"/>
-      <c r="J22" s="155"/>
-      <c r="K22" s="155"/>
-      <c r="L22" s="155"/>
+      <c r="I22" s="137"/>
+      <c r="J22" s="137"/>
+      <c r="K22" s="137"/>
+      <c r="L22" s="137"/>
       <c r="M22" s="44"/>
       <c r="N22" s="44"/>
       <c r="O22" s="44"/>
@@ -4694,72 +4695,72 @@
     <row r="23" spans="4:55">
       <c r="D23" s="65"/>
       <c r="E23" s="60"/>
-      <c r="F23" s="156" t="s">
+      <c r="F23" s="138" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="118"/>
-      <c r="H23" s="158" t="s">
+      <c r="G23" s="133"/>
+      <c r="H23" s="140" t="s">
         <v>99</v>
       </c>
-      <c r="I23" s="159"/>
-      <c r="J23" s="119" t="s">
+      <c r="I23" s="141"/>
+      <c r="J23" s="134" t="s">
         <v>100</v>
       </c>
-      <c r="K23" s="120"/>
-      <c r="L23" s="120"/>
-      <c r="M23" s="120"/>
-      <c r="N23" s="120"/>
-      <c r="O23" s="120"/>
-      <c r="P23" s="121"/>
-      <c r="Q23" s="116" t="s">
+      <c r="K23" s="135"/>
+      <c r="L23" s="135"/>
+      <c r="M23" s="135"/>
+      <c r="N23" s="135"/>
+      <c r="O23" s="135"/>
+      <c r="P23" s="136"/>
+      <c r="Q23" s="131" t="s">
         <v>101</v>
       </c>
-      <c r="R23" s="117"/>
-      <c r="S23" s="117"/>
-      <c r="T23" s="117"/>
-      <c r="U23" s="117"/>
-      <c r="V23" s="117"/>
-      <c r="W23" s="118"/>
-      <c r="X23" s="116" t="s">
+      <c r="R23" s="132"/>
+      <c r="S23" s="132"/>
+      <c r="T23" s="132"/>
+      <c r="U23" s="132"/>
+      <c r="V23" s="132"/>
+      <c r="W23" s="133"/>
+      <c r="X23" s="131" t="s">
         <v>102</v>
       </c>
-      <c r="Y23" s="117"/>
-      <c r="Z23" s="117"/>
-      <c r="AA23" s="118"/>
-      <c r="AB23" s="116" t="s">
+      <c r="Y23" s="132"/>
+      <c r="Z23" s="132"/>
+      <c r="AA23" s="133"/>
+      <c r="AB23" s="131" t="s">
         <v>103</v>
       </c>
-      <c r="AC23" s="117"/>
-      <c r="AD23" s="117"/>
-      <c r="AE23" s="118"/>
-      <c r="AF23" s="116" t="s">
+      <c r="AC23" s="132"/>
+      <c r="AD23" s="132"/>
+      <c r="AE23" s="133"/>
+      <c r="AF23" s="131" t="s">
         <v>104</v>
       </c>
-      <c r="AG23" s="117"/>
-      <c r="AH23" s="117"/>
-      <c r="AI23" s="117"/>
-      <c r="AJ23" s="117"/>
-      <c r="AK23" s="117"/>
-      <c r="AL23" s="117"/>
+      <c r="AG23" s="132"/>
+      <c r="AH23" s="132"/>
+      <c r="AI23" s="132"/>
+      <c r="AJ23" s="132"/>
+      <c r="AK23" s="132"/>
+      <c r="AL23" s="132"/>
       <c r="AM23" s="79"/>
-      <c r="AN23" s="116" t="s">
+      <c r="AN23" s="131" t="s">
         <v>105</v>
       </c>
-      <c r="AO23" s="117"/>
-      <c r="AP23" s="117"/>
-      <c r="AQ23" s="117"/>
-      <c r="AR23" s="117"/>
-      <c r="AS23" s="117"/>
-      <c r="AT23" s="118"/>
-      <c r="AU23" s="116" t="s">
+      <c r="AO23" s="132"/>
+      <c r="AP23" s="132"/>
+      <c r="AQ23" s="132"/>
+      <c r="AR23" s="132"/>
+      <c r="AS23" s="132"/>
+      <c r="AT23" s="133"/>
+      <c r="AU23" s="131" t="s">
         <v>107</v>
       </c>
-      <c r="AV23" s="117"/>
-      <c r="AW23" s="117"/>
-      <c r="AX23" s="117"/>
-      <c r="AY23" s="117"/>
-      <c r="AZ23" s="118"/>
-      <c r="BA23" s="122" t="s">
+      <c r="AV23" s="132"/>
+      <c r="AW23" s="132"/>
+      <c r="AX23" s="132"/>
+      <c r="AY23" s="132"/>
+      <c r="AZ23" s="133"/>
+      <c r="BA23" s="155" t="s">
         <v>106</v>
       </c>
       <c r="BB23" s="61"/>
@@ -4768,54 +4769,54 @@
     <row r="24" spans="4:55">
       <c r="D24" s="65"/>
       <c r="E24" s="60"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="121"/>
-      <c r="H24" s="160"/>
-      <c r="I24" s="161"/>
-      <c r="J24" s="119"/>
-      <c r="K24" s="120"/>
-      <c r="L24" s="120"/>
-      <c r="M24" s="120"/>
-      <c r="N24" s="120"/>
-      <c r="O24" s="120"/>
-      <c r="P24" s="121"/>
-      <c r="Q24" s="119"/>
-      <c r="R24" s="120"/>
-      <c r="S24" s="120"/>
-      <c r="T24" s="120"/>
-      <c r="U24" s="120"/>
-      <c r="V24" s="120"/>
-      <c r="W24" s="121"/>
-      <c r="X24" s="119"/>
-      <c r="Y24" s="120"/>
-      <c r="Z24" s="120"/>
-      <c r="AA24" s="121"/>
-      <c r="AB24" s="119"/>
-      <c r="AC24" s="120"/>
-      <c r="AD24" s="120"/>
-      <c r="AE24" s="121"/>
-      <c r="AF24" s="119"/>
-      <c r="AG24" s="120"/>
-      <c r="AH24" s="120"/>
-      <c r="AI24" s="120"/>
-      <c r="AJ24" s="120"/>
-      <c r="AK24" s="120"/>
-      <c r="AL24" s="120"/>
+      <c r="F24" s="139"/>
+      <c r="G24" s="136"/>
+      <c r="H24" s="142"/>
+      <c r="I24" s="143"/>
+      <c r="J24" s="134"/>
+      <c r="K24" s="135"/>
+      <c r="L24" s="135"/>
+      <c r="M24" s="135"/>
+      <c r="N24" s="135"/>
+      <c r="O24" s="135"/>
+      <c r="P24" s="136"/>
+      <c r="Q24" s="134"/>
+      <c r="R24" s="135"/>
+      <c r="S24" s="135"/>
+      <c r="T24" s="135"/>
+      <c r="U24" s="135"/>
+      <c r="V24" s="135"/>
+      <c r="W24" s="136"/>
+      <c r="X24" s="134"/>
+      <c r="Y24" s="135"/>
+      <c r="Z24" s="135"/>
+      <c r="AA24" s="136"/>
+      <c r="AB24" s="134"/>
+      <c r="AC24" s="135"/>
+      <c r="AD24" s="135"/>
+      <c r="AE24" s="136"/>
+      <c r="AF24" s="134"/>
+      <c r="AG24" s="135"/>
+      <c r="AH24" s="135"/>
+      <c r="AI24" s="135"/>
+      <c r="AJ24" s="135"/>
+      <c r="AK24" s="135"/>
+      <c r="AL24" s="135"/>
       <c r="AM24" s="72"/>
-      <c r="AN24" s="119"/>
-      <c r="AO24" s="120"/>
-      <c r="AP24" s="120"/>
-      <c r="AQ24" s="120"/>
-      <c r="AR24" s="120"/>
-      <c r="AS24" s="120"/>
-      <c r="AT24" s="121"/>
-      <c r="AU24" s="119"/>
-      <c r="AV24" s="120"/>
-      <c r="AW24" s="120"/>
-      <c r="AX24" s="120"/>
-      <c r="AY24" s="120"/>
-      <c r="AZ24" s="121"/>
-      <c r="BA24" s="123"/>
+      <c r="AN24" s="134"/>
+      <c r="AO24" s="135"/>
+      <c r="AP24" s="135"/>
+      <c r="AQ24" s="135"/>
+      <c r="AR24" s="135"/>
+      <c r="AS24" s="135"/>
+      <c r="AT24" s="136"/>
+      <c r="AU24" s="134"/>
+      <c r="AV24" s="135"/>
+      <c r="AW24" s="135"/>
+      <c r="AX24" s="135"/>
+      <c r="AY24" s="135"/>
+      <c r="AZ24" s="136"/>
+      <c r="BA24" s="156"/>
       <c r="BB24" s="61"/>
       <c r="BC24" s="66"/>
     </row>
@@ -5580,94 +5581,94 @@
       <c r="BC38" s="69"/>
     </row>
     <row r="41" spans="3:56">
-      <c r="C41" s="149" t="s">
+      <c r="C41" s="145" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="149"/>
-      <c r="E41" s="149"/>
-      <c r="F41" s="149"/>
-      <c r="G41" s="149"/>
+      <c r="D41" s="145"/>
+      <c r="E41" s="145"/>
+      <c r="F41" s="145"/>
+      <c r="G41" s="145"/>
     </row>
     <row r="42" spans="3:56">
       <c r="C42" s="31"/>
     </row>
     <row r="43" spans="3:56" ht="15">
-      <c r="C43" s="95" t="s">
+      <c r="C43" s="119" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="93"/>
-      <c r="E43" s="93" t="s">
+      <c r="D43" s="120"/>
+      <c r="E43" s="120" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="93"/>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="93"/>
-      <c r="K43" s="93"/>
-      <c r="L43" s="93"/>
-      <c r="M43" s="93"/>
-      <c r="N43" s="93" t="s">
+      <c r="F43" s="120"/>
+      <c r="G43" s="120"/>
+      <c r="H43" s="120"/>
+      <c r="I43" s="120"/>
+      <c r="J43" s="120"/>
+      <c r="K43" s="120"/>
+      <c r="L43" s="120"/>
+      <c r="M43" s="120"/>
+      <c r="N43" s="120" t="s">
         <v>36</v>
       </c>
-      <c r="O43" s="93"/>
-      <c r="P43" s="93"/>
-      <c r="Q43" s="93"/>
-      <c r="R43" s="93" t="s">
+      <c r="O43" s="120"/>
+      <c r="P43" s="120"/>
+      <c r="Q43" s="120"/>
+      <c r="R43" s="120" t="s">
         <v>37</v>
       </c>
-      <c r="S43" s="93"/>
-      <c r="T43" s="93"/>
-      <c r="U43" s="93" t="s">
+      <c r="S43" s="120"/>
+      <c r="T43" s="120"/>
+      <c r="U43" s="120" t="s">
         <v>38</v>
       </c>
-      <c r="V43" s="93"/>
-      <c r="W43" s="93"/>
-      <c r="X43" s="93" t="s">
+      <c r="V43" s="120"/>
+      <c r="W43" s="120"/>
+      <c r="X43" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="Y43" s="93"/>
-      <c r="Z43" s="93"/>
-      <c r="AA43" s="93"/>
-      <c r="AB43" s="93"/>
-      <c r="AC43" s="93"/>
-      <c r="AD43" s="93"/>
-      <c r="AE43" s="93" t="s">
+      <c r="Y43" s="120"/>
+      <c r="Z43" s="120"/>
+      <c r="AA43" s="120"/>
+      <c r="AB43" s="120"/>
+      <c r="AC43" s="120"/>
+      <c r="AD43" s="120"/>
+      <c r="AE43" s="120" t="s">
         <v>40</v>
       </c>
-      <c r="AF43" s="93"/>
-      <c r="AG43" s="93"/>
-      <c r="AH43" s="93"/>
-      <c r="AI43" s="93"/>
-      <c r="AJ43" s="93" t="s">
+      <c r="AF43" s="120"/>
+      <c r="AG43" s="120"/>
+      <c r="AH43" s="120"/>
+      <c r="AI43" s="120"/>
+      <c r="AJ43" s="120" t="s">
         <v>41</v>
       </c>
-      <c r="AK43" s="93"/>
-      <c r="AL43" s="93"/>
-      <c r="AM43" s="93"/>
-      <c r="AN43" s="93" t="s">
+      <c r="AK43" s="120"/>
+      <c r="AL43" s="120"/>
+      <c r="AM43" s="120"/>
+      <c r="AN43" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="AO43" s="93"/>
-      <c r="AP43" s="93"/>
-      <c r="AQ43" s="93" t="s">
+      <c r="AO43" s="120"/>
+      <c r="AP43" s="120"/>
+      <c r="AQ43" s="120" t="s">
         <v>43</v>
       </c>
-      <c r="AR43" s="93"/>
-      <c r="AS43" s="93"/>
-      <c r="AT43" s="93"/>
-      <c r="AU43" s="93"/>
-      <c r="AV43" s="93"/>
-      <c r="AW43" s="93" t="s">
+      <c r="AR43" s="120"/>
+      <c r="AS43" s="120"/>
+      <c r="AT43" s="120"/>
+      <c r="AU43" s="120"/>
+      <c r="AV43" s="120"/>
+      <c r="AW43" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="AX43" s="93"/>
-      <c r="AY43" s="93"/>
-      <c r="AZ43" s="93"/>
-      <c r="BA43" s="93"/>
-      <c r="BB43" s="93"/>
-      <c r="BC43" s="93"/>
-      <c r="BD43" s="94"/>
+      <c r="AX43" s="120"/>
+      <c r="AY43" s="120"/>
+      <c r="AZ43" s="120"/>
+      <c r="BA43" s="120"/>
+      <c r="BB43" s="120"/>
+      <c r="BC43" s="120"/>
+      <c r="BD43" s="130"/>
     </row>
     <row r="44" spans="3:56">
       <c r="C44" s="33"/>
@@ -5878,14 +5879,14 @@
         <v>53</v>
       </c>
       <c r="AP46" s="38"/>
-      <c r="AQ46" s="107" t="s">
+      <c r="AQ46" s="122" t="s">
         <v>84</v>
       </c>
-      <c r="AR46" s="108"/>
-      <c r="AS46" s="108"/>
-      <c r="AT46" s="108"/>
-      <c r="AU46" s="108"/>
-      <c r="AV46" s="109"/>
+      <c r="AR46" s="123"/>
+      <c r="AS46" s="123"/>
+      <c r="AT46" s="123"/>
+      <c r="AU46" s="123"/>
+      <c r="AV46" s="124"/>
       <c r="AW46" s="39" t="s">
         <v>58</v>
       </c>
@@ -6100,8 +6101,8 @@
       </c>
       <c r="AM49" s="38"/>
       <c r="AN49" s="39"/>
-      <c r="AO49" s="35" t="s">
-        <v>53</v>
+      <c r="AO49" s="35">
+        <v>20</v>
       </c>
       <c r="AP49" s="38"/>
       <c r="AQ49" s="39"/>
@@ -7214,132 +7215,124 @@
       <c r="BD66" s="44"/>
     </row>
     <row r="67" spans="3:56">
-      <c r="C67" s="149" t="s">
+      <c r="C67" s="145" t="s">
         <v>32</v>
       </c>
-      <c r="D67" s="149"/>
-      <c r="E67" s="149"/>
-      <c r="F67" s="149"/>
-      <c r="G67" s="149"/>
-      <c r="H67" s="149"/>
-      <c r="I67" s="149"/>
-      <c r="J67" s="149"/>
+      <c r="D67" s="145"/>
+      <c r="E67" s="145"/>
+      <c r="F67" s="145"/>
+      <c r="G67" s="145"/>
+      <c r="H67" s="145"/>
+      <c r="I67" s="145"/>
+      <c r="J67" s="145"/>
     </row>
     <row r="68" spans="3:56">
       <c r="C68" s="31"/>
     </row>
     <row r="69" spans="3:56" ht="15">
-      <c r="C69" s="92" t="s">
+      <c r="C69" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="D69" s="90"/>
-      <c r="E69" s="90" t="s">
+      <c r="D69" s="103"/>
+      <c r="E69" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="F69" s="90"/>
-      <c r="G69" s="90"/>
-      <c r="H69" s="90"/>
-      <c r="I69" s="90"/>
-      <c r="J69" s="90"/>
-      <c r="K69" s="90"/>
-      <c r="L69" s="90"/>
-      <c r="M69" s="90"/>
-      <c r="N69" s="90"/>
-      <c r="O69" s="90"/>
-      <c r="P69" s="90"/>
-      <c r="Q69" s="90"/>
-      <c r="R69" s="90" t="s">
+      <c r="F69" s="103"/>
+      <c r="G69" s="103"/>
+      <c r="H69" s="103"/>
+      <c r="I69" s="103"/>
+      <c r="J69" s="103"/>
+      <c r="K69" s="103"/>
+      <c r="L69" s="103"/>
+      <c r="M69" s="103"/>
+      <c r="N69" s="103"/>
+      <c r="O69" s="103"/>
+      <c r="P69" s="103"/>
+      <c r="Q69" s="103"/>
+      <c r="R69" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="S69" s="90"/>
-      <c r="T69" s="90"/>
-      <c r="U69" s="90"/>
-      <c r="V69" s="90"/>
-      <c r="W69" s="90"/>
-      <c r="X69" s="90" t="s">
+      <c r="S69" s="103"/>
+      <c r="T69" s="103"/>
+      <c r="U69" s="103"/>
+      <c r="V69" s="103"/>
+      <c r="W69" s="103"/>
+      <c r="X69" s="103" t="s">
         <v>45</v>
       </c>
-      <c r="Y69" s="90"/>
-      <c r="Z69" s="90"/>
-      <c r="AA69" s="90"/>
-      <c r="AB69" s="90"/>
-      <c r="AC69" s="90"/>
-      <c r="AD69" s="90"/>
-      <c r="AE69" s="90" t="s">
+      <c r="Y69" s="103"/>
+      <c r="Z69" s="103"/>
+      <c r="AA69" s="103"/>
+      <c r="AB69" s="103"/>
+      <c r="AC69" s="103"/>
+      <c r="AD69" s="103"/>
+      <c r="AE69" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="AF69" s="90"/>
-      <c r="AG69" s="90"/>
-      <c r="AH69" s="90"/>
-      <c r="AI69" s="90"/>
-      <c r="AJ69" s="90"/>
-      <c r="AK69" s="90"/>
-      <c r="AL69" s="90" t="s">
+      <c r="AF69" s="103"/>
+      <c r="AG69" s="103"/>
+      <c r="AH69" s="103"/>
+      <c r="AI69" s="103"/>
+      <c r="AJ69" s="103"/>
+      <c r="AK69" s="103"/>
+      <c r="AL69" s="103" t="s">
         <v>44</v>
       </c>
-      <c r="AM69" s="90"/>
-      <c r="AN69" s="90"/>
-      <c r="AO69" s="90"/>
-      <c r="AP69" s="90"/>
-      <c r="AQ69" s="90"/>
-      <c r="AR69" s="90"/>
-      <c r="AS69" s="90"/>
-      <c r="AT69" s="90"/>
-      <c r="AU69" s="90"/>
-      <c r="AV69" s="90"/>
-      <c r="AW69" s="90"/>
-      <c r="AX69" s="90"/>
-      <c r="AY69" s="90"/>
-      <c r="AZ69" s="90"/>
-      <c r="BA69" s="90"/>
-      <c r="BB69" s="90"/>
-      <c r="BC69" s="90"/>
-      <c r="BD69" s="91"/>
+      <c r="AM69" s="103"/>
+      <c r="AN69" s="103"/>
+      <c r="AO69" s="103"/>
+      <c r="AP69" s="103"/>
+      <c r="AQ69" s="103"/>
+      <c r="AR69" s="103"/>
+      <c r="AS69" s="103"/>
+      <c r="AT69" s="103"/>
+      <c r="AU69" s="103"/>
+      <c r="AV69" s="103"/>
+      <c r="AW69" s="103"/>
+      <c r="AX69" s="103"/>
+      <c r="AY69" s="103"/>
+      <c r="AZ69" s="103"/>
+      <c r="BA69" s="103"/>
+      <c r="BB69" s="103"/>
+      <c r="BC69" s="103"/>
+      <c r="BD69" s="121"/>
     </row>
     <row r="70" spans="3:56" ht="15" customHeight="1">
       <c r="C70" s="45"/>
-      <c r="D70" s="37">
-        <v>1</v>
-      </c>
-      <c r="E70" s="110" t="s">
-        <v>109</v>
-      </c>
-      <c r="F70" s="111"/>
-      <c r="G70" s="111"/>
-      <c r="H70" s="111"/>
-      <c r="I70" s="111"/>
-      <c r="J70" s="111"/>
-      <c r="K70" s="111"/>
-      <c r="L70" s="111"/>
-      <c r="M70" s="111"/>
-      <c r="N70" s="111"/>
-      <c r="O70" s="111"/>
-      <c r="P70" s="111"/>
-      <c r="Q70" s="112"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="104"/>
+      <c r="F70" s="105"/>
+      <c r="G70" s="105"/>
+      <c r="H70" s="105"/>
+      <c r="I70" s="105"/>
+      <c r="J70" s="105"/>
+      <c r="K70" s="105"/>
+      <c r="L70" s="105"/>
+      <c r="M70" s="105"/>
+      <c r="N70" s="105"/>
+      <c r="O70" s="105"/>
+      <c r="P70" s="105"/>
+      <c r="Q70" s="106"/>
       <c r="R70" s="34"/>
       <c r="S70" s="34"/>
       <c r="T70" s="34"/>
       <c r="U70" s="34"/>
       <c r="V70" s="34"/>
       <c r="W70" s="37"/>
-      <c r="X70" s="113" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y70" s="114"/>
-      <c r="Z70" s="114"/>
-      <c r="AA70" s="114"/>
-      <c r="AB70" s="114"/>
-      <c r="AC70" s="114"/>
-      <c r="AD70" s="115"/>
-      <c r="AE70" s="110" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF70" s="111"/>
-      <c r="AG70" s="111"/>
-      <c r="AH70" s="111"/>
-      <c r="AI70" s="111"/>
-      <c r="AJ70" s="111"/>
-      <c r="AK70" s="112"/>
+      <c r="X70" s="157"/>
+      <c r="Y70" s="158"/>
+      <c r="Z70" s="158"/>
+      <c r="AA70" s="158"/>
+      <c r="AB70" s="158"/>
+      <c r="AC70" s="158"/>
+      <c r="AD70" s="159"/>
+      <c r="AE70" s="104"/>
+      <c r="AF70" s="105"/>
+      <c r="AG70" s="105"/>
+      <c r="AH70" s="105"/>
+      <c r="AI70" s="105"/>
+      <c r="AJ70" s="105"/>
+      <c r="AK70" s="106"/>
       <c r="AL70" s="34"/>
       <c r="AM70" s="34"/>
       <c r="AN70" s="34"/>
@@ -7363,47 +7356,47 @@
     <row r="71" spans="3:56" ht="15" customHeight="1">
       <c r="C71" s="46"/>
       <c r="D71" s="40">
-        <v>2</v>
-      </c>
-      <c r="E71" s="104" t="s">
-        <v>112</v>
-      </c>
-      <c r="F71" s="105"/>
-      <c r="G71" s="105"/>
-      <c r="H71" s="105"/>
-      <c r="I71" s="105"/>
-      <c r="J71" s="105"/>
-      <c r="K71" s="105"/>
-      <c r="L71" s="105"/>
-      <c r="M71" s="105"/>
-      <c r="N71" s="105"/>
-      <c r="O71" s="105"/>
-      <c r="P71" s="105"/>
-      <c r="Q71" s="106"/>
+        <v>1</v>
+      </c>
+      <c r="E71" s="107" t="s">
+        <v>110</v>
+      </c>
+      <c r="F71" s="108"/>
+      <c r="G71" s="108"/>
+      <c r="H71" s="108"/>
+      <c r="I71" s="108"/>
+      <c r="J71" s="108"/>
+      <c r="K71" s="108"/>
+      <c r="L71" s="108"/>
+      <c r="M71" s="108"/>
+      <c r="N71" s="108"/>
+      <c r="O71" s="108"/>
+      <c r="P71" s="108"/>
+      <c r="Q71" s="109"/>
       <c r="R71" s="38"/>
       <c r="S71" s="38"/>
       <c r="T71" s="38"/>
       <c r="U71" s="38"/>
       <c r="V71" s="38"/>
       <c r="W71" s="40"/>
-      <c r="X71" s="107" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y71" s="108"/>
-      <c r="Z71" s="108"/>
-      <c r="AA71" s="108"/>
-      <c r="AB71" s="108"/>
-      <c r="AC71" s="108"/>
-      <c r="AD71" s="109"/>
-      <c r="AE71" s="104" t="s">
+      <c r="X71" s="122" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y71" s="123"/>
+      <c r="Z71" s="123"/>
+      <c r="AA71" s="123"/>
+      <c r="AB71" s="123"/>
+      <c r="AC71" s="123"/>
+      <c r="AD71" s="124"/>
+      <c r="AE71" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="AF71" s="105"/>
-      <c r="AG71" s="105"/>
-      <c r="AH71" s="105"/>
-      <c r="AI71" s="105"/>
-      <c r="AJ71" s="105"/>
-      <c r="AK71" s="106"/>
+      <c r="AF71" s="108"/>
+      <c r="AG71" s="108"/>
+      <c r="AH71" s="108"/>
+      <c r="AI71" s="108"/>
+      <c r="AJ71" s="108"/>
+      <c r="AK71" s="109"/>
       <c r="AL71" s="38"/>
       <c r="AM71" s="38"/>
       <c r="AN71" s="38"/>
@@ -7427,47 +7420,47 @@
     <row r="72" spans="3:56" ht="15" customHeight="1">
       <c r="C72" s="46"/>
       <c r="D72" s="40">
-        <v>3</v>
-      </c>
-      <c r="E72" s="104" t="s">
-        <v>113</v>
-      </c>
-      <c r="F72" s="105"/>
-      <c r="G72" s="105"/>
-      <c r="H72" s="105"/>
-      <c r="I72" s="105"/>
-      <c r="J72" s="105"/>
-      <c r="K72" s="105"/>
-      <c r="L72" s="105"/>
-      <c r="M72" s="105"/>
-      <c r="N72" s="105"/>
-      <c r="O72" s="105"/>
-      <c r="P72" s="105"/>
-      <c r="Q72" s="106"/>
+        <v>2</v>
+      </c>
+      <c r="E72" s="107" t="s">
+        <v>111</v>
+      </c>
+      <c r="F72" s="108"/>
+      <c r="G72" s="108"/>
+      <c r="H72" s="108"/>
+      <c r="I72" s="108"/>
+      <c r="J72" s="108"/>
+      <c r="K72" s="108"/>
+      <c r="L72" s="108"/>
+      <c r="M72" s="108"/>
+      <c r="N72" s="108"/>
+      <c r="O72" s="108"/>
+      <c r="P72" s="108"/>
+      <c r="Q72" s="109"/>
       <c r="R72" s="38"/>
       <c r="S72" s="38"/>
       <c r="T72" s="38"/>
       <c r="U72" s="38"/>
       <c r="V72" s="38"/>
       <c r="W72" s="40"/>
-      <c r="X72" s="107" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y72" s="108"/>
-      <c r="Z72" s="108"/>
-      <c r="AA72" s="108"/>
-      <c r="AB72" s="108"/>
-      <c r="AC72" s="108"/>
-      <c r="AD72" s="109"/>
-      <c r="AE72" s="104" t="s">
-        <v>114</v>
-      </c>
-      <c r="AF72" s="105"/>
-      <c r="AG72" s="105"/>
-      <c r="AH72" s="105"/>
-      <c r="AI72" s="105"/>
-      <c r="AJ72" s="105"/>
-      <c r="AK72" s="106"/>
+      <c r="X72" s="122" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y72" s="123"/>
+      <c r="Z72" s="123"/>
+      <c r="AA72" s="123"/>
+      <c r="AB72" s="123"/>
+      <c r="AC72" s="123"/>
+      <c r="AD72" s="124"/>
+      <c r="AE72" s="107" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF72" s="108"/>
+      <c r="AG72" s="108"/>
+      <c r="AH72" s="108"/>
+      <c r="AI72" s="108"/>
+      <c r="AJ72" s="108"/>
+      <c r="AK72" s="109"/>
       <c r="AL72" s="38"/>
       <c r="AM72" s="38"/>
       <c r="AN72" s="38"/>
@@ -8166,68 +8159,68 @@
       </c>
     </row>
     <row r="88" spans="3:56" ht="15">
-      <c r="C88" s="92" t="s">
+      <c r="C88" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="D88" s="90"/>
-      <c r="E88" s="90" t="s">
+      <c r="D88" s="103"/>
+      <c r="E88" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="F88" s="90"/>
-      <c r="G88" s="90"/>
-      <c r="H88" s="90"/>
-      <c r="I88" s="90"/>
-      <c r="J88" s="90"/>
-      <c r="K88" s="90"/>
-      <c r="L88" s="90"/>
-      <c r="M88" s="90"/>
-      <c r="N88" s="90"/>
-      <c r="O88" s="90"/>
-      <c r="P88" s="90"/>
-      <c r="Q88" s="90"/>
-      <c r="R88" s="90" t="s">
+      <c r="F88" s="103"/>
+      <c r="G88" s="103"/>
+      <c r="H88" s="103"/>
+      <c r="I88" s="103"/>
+      <c r="J88" s="103"/>
+      <c r="K88" s="103"/>
+      <c r="L88" s="103"/>
+      <c r="M88" s="103"/>
+      <c r="N88" s="103"/>
+      <c r="O88" s="103"/>
+      <c r="P88" s="103"/>
+      <c r="Q88" s="103"/>
+      <c r="R88" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="S88" s="90"/>
-      <c r="T88" s="90"/>
-      <c r="U88" s="90"/>
-      <c r="V88" s="90"/>
-      <c r="W88" s="90"/>
-      <c r="X88" s="90" t="s">
+      <c r="S88" s="103"/>
+      <c r="T88" s="103"/>
+      <c r="U88" s="103"/>
+      <c r="V88" s="103"/>
+      <c r="W88" s="103"/>
+      <c r="X88" s="103" t="s">
         <v>49</v>
       </c>
-      <c r="Y88" s="90"/>
-      <c r="Z88" s="90"/>
-      <c r="AA88" s="90"/>
-      <c r="AB88" s="90"/>
-      <c r="AC88" s="90"/>
-      <c r="AD88" s="90"/>
-      <c r="AE88" s="90"/>
-      <c r="AF88" s="90"/>
-      <c r="AG88" s="90"/>
-      <c r="AH88" s="90"/>
-      <c r="AI88" s="90"/>
-      <c r="AJ88" s="90"/>
-      <c r="AK88" s="90"/>
-      <c r="AL88" s="90"/>
-      <c r="AM88" s="90"/>
-      <c r="AN88" s="90"/>
-      <c r="AO88" s="90"/>
-      <c r="AP88" s="90"/>
-      <c r="AQ88" s="90"/>
-      <c r="AR88" s="90"/>
-      <c r="AS88" s="90"/>
-      <c r="AT88" s="90"/>
-      <c r="AU88" s="90"/>
-      <c r="AV88" s="90"/>
-      <c r="AW88" s="90"/>
-      <c r="AX88" s="90"/>
-      <c r="AY88" s="90"/>
-      <c r="AZ88" s="90"/>
-      <c r="BA88" s="90"/>
-      <c r="BB88" s="90"/>
-      <c r="BC88" s="90"/>
-      <c r="BD88" s="91"/>
+      <c r="Y88" s="103"/>
+      <c r="Z88" s="103"/>
+      <c r="AA88" s="103"/>
+      <c r="AB88" s="103"/>
+      <c r="AC88" s="103"/>
+      <c r="AD88" s="103"/>
+      <c r="AE88" s="103"/>
+      <c r="AF88" s="103"/>
+      <c r="AG88" s="103"/>
+      <c r="AH88" s="103"/>
+      <c r="AI88" s="103"/>
+      <c r="AJ88" s="103"/>
+      <c r="AK88" s="103"/>
+      <c r="AL88" s="103"/>
+      <c r="AM88" s="103"/>
+      <c r="AN88" s="103"/>
+      <c r="AO88" s="103"/>
+      <c r="AP88" s="103"/>
+      <c r="AQ88" s="103"/>
+      <c r="AR88" s="103"/>
+      <c r="AS88" s="103"/>
+      <c r="AT88" s="103"/>
+      <c r="AU88" s="103"/>
+      <c r="AV88" s="103"/>
+      <c r="AW88" s="103"/>
+      <c r="AX88" s="103"/>
+      <c r="AY88" s="103"/>
+      <c r="AZ88" s="103"/>
+      <c r="BA88" s="103"/>
+      <c r="BB88" s="103"/>
+      <c r="BC88" s="103"/>
+      <c r="BD88" s="121"/>
     </row>
     <row r="89" spans="3:56" ht="15" customHeight="1">
       <c r="C89" s="33"/>
@@ -8252,46 +8245,46 @@
       <c r="R89" s="34"/>
       <c r="S89" s="34"/>
       <c r="T89" s="34" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U89" s="34"/>
       <c r="V89" s="34"/>
       <c r="W89" s="37"/>
-      <c r="X89" s="110" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y89" s="111"/>
-      <c r="Z89" s="111"/>
-      <c r="AA89" s="111"/>
-      <c r="AB89" s="111"/>
-      <c r="AC89" s="111"/>
-      <c r="AD89" s="111"/>
-      <c r="AE89" s="111"/>
-      <c r="AF89" s="111"/>
-      <c r="AG89" s="111"/>
-      <c r="AH89" s="111"/>
-      <c r="AI89" s="111"/>
-      <c r="AJ89" s="111"/>
-      <c r="AK89" s="111"/>
-      <c r="AL89" s="111"/>
-      <c r="AM89" s="111"/>
-      <c r="AN89" s="111"/>
-      <c r="AO89" s="111"/>
-      <c r="AP89" s="111"/>
-      <c r="AQ89" s="111"/>
-      <c r="AR89" s="111"/>
-      <c r="AS89" s="111"/>
-      <c r="AT89" s="111"/>
-      <c r="AU89" s="111"/>
-      <c r="AV89" s="111"/>
-      <c r="AW89" s="111"/>
-      <c r="AX89" s="111"/>
-      <c r="AY89" s="111"/>
-      <c r="AZ89" s="111"/>
-      <c r="BA89" s="111"/>
-      <c r="BB89" s="111"/>
-      <c r="BC89" s="111"/>
-      <c r="BD89" s="112"/>
+      <c r="X89" s="104" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y89" s="105"/>
+      <c r="Z89" s="105"/>
+      <c r="AA89" s="105"/>
+      <c r="AB89" s="105"/>
+      <c r="AC89" s="105"/>
+      <c r="AD89" s="105"/>
+      <c r="AE89" s="105"/>
+      <c r="AF89" s="105"/>
+      <c r="AG89" s="105"/>
+      <c r="AH89" s="105"/>
+      <c r="AI89" s="105"/>
+      <c r="AJ89" s="105"/>
+      <c r="AK89" s="105"/>
+      <c r="AL89" s="105"/>
+      <c r="AM89" s="105"/>
+      <c r="AN89" s="105"/>
+      <c r="AO89" s="105"/>
+      <c r="AP89" s="105"/>
+      <c r="AQ89" s="105"/>
+      <c r="AR89" s="105"/>
+      <c r="AS89" s="105"/>
+      <c r="AT89" s="105"/>
+      <c r="AU89" s="105"/>
+      <c r="AV89" s="105"/>
+      <c r="AW89" s="105"/>
+      <c r="AX89" s="105"/>
+      <c r="AY89" s="105"/>
+      <c r="AZ89" s="105"/>
+      <c r="BA89" s="105"/>
+      <c r="BB89" s="105"/>
+      <c r="BC89" s="105"/>
+      <c r="BD89" s="106"/>
     </row>
     <row r="90" spans="3:56" ht="15" customHeight="1">
       <c r="C90" s="39"/>
@@ -8316,46 +8309,46 @@
       <c r="R90" s="38"/>
       <c r="S90" s="38"/>
       <c r="T90" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U90" s="38"/>
       <c r="V90" s="38"/>
       <c r="W90" s="40"/>
-      <c r="X90" s="104" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y90" s="105"/>
-      <c r="Z90" s="105"/>
-      <c r="AA90" s="105"/>
-      <c r="AB90" s="105"/>
-      <c r="AC90" s="105"/>
-      <c r="AD90" s="105"/>
-      <c r="AE90" s="105"/>
-      <c r="AF90" s="105"/>
-      <c r="AG90" s="105"/>
-      <c r="AH90" s="105"/>
-      <c r="AI90" s="105"/>
-      <c r="AJ90" s="105"/>
-      <c r="AK90" s="105"/>
-      <c r="AL90" s="105"/>
-      <c r="AM90" s="105"/>
-      <c r="AN90" s="105"/>
-      <c r="AO90" s="105"/>
-      <c r="AP90" s="105"/>
-      <c r="AQ90" s="105"/>
-      <c r="AR90" s="105"/>
-      <c r="AS90" s="105"/>
-      <c r="AT90" s="105"/>
-      <c r="AU90" s="105"/>
-      <c r="AV90" s="105"/>
-      <c r="AW90" s="105"/>
-      <c r="AX90" s="105"/>
-      <c r="AY90" s="105"/>
-      <c r="AZ90" s="105"/>
-      <c r="BA90" s="105"/>
-      <c r="BB90" s="105"/>
-      <c r="BC90" s="105"/>
-      <c r="BD90" s="106"/>
+      <c r="X90" s="107" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y90" s="108"/>
+      <c r="Z90" s="108"/>
+      <c r="AA90" s="108"/>
+      <c r="AB90" s="108"/>
+      <c r="AC90" s="108"/>
+      <c r="AD90" s="108"/>
+      <c r="AE90" s="108"/>
+      <c r="AF90" s="108"/>
+      <c r="AG90" s="108"/>
+      <c r="AH90" s="108"/>
+      <c r="AI90" s="108"/>
+      <c r="AJ90" s="108"/>
+      <c r="AK90" s="108"/>
+      <c r="AL90" s="108"/>
+      <c r="AM90" s="108"/>
+      <c r="AN90" s="108"/>
+      <c r="AO90" s="108"/>
+      <c r="AP90" s="108"/>
+      <c r="AQ90" s="108"/>
+      <c r="AR90" s="108"/>
+      <c r="AS90" s="108"/>
+      <c r="AT90" s="108"/>
+      <c r="AU90" s="108"/>
+      <c r="AV90" s="108"/>
+      <c r="AW90" s="108"/>
+      <c r="AX90" s="108"/>
+      <c r="AY90" s="108"/>
+      <c r="AZ90" s="108"/>
+      <c r="BA90" s="108"/>
+      <c r="BB90" s="108"/>
+      <c r="BC90" s="108"/>
+      <c r="BD90" s="109"/>
     </row>
     <row r="91" spans="3:56" ht="15" customHeight="1">
       <c r="C91" s="39"/>
@@ -8380,46 +8373,46 @@
       <c r="R91" s="38"/>
       <c r="S91" s="38"/>
       <c r="T91" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U91" s="38"/>
       <c r="V91" s="38"/>
       <c r="W91" s="40"/>
-      <c r="X91" s="104" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y91" s="105"/>
-      <c r="Z91" s="105"/>
-      <c r="AA91" s="105"/>
-      <c r="AB91" s="105"/>
-      <c r="AC91" s="105"/>
-      <c r="AD91" s="105"/>
-      <c r="AE91" s="105"/>
-      <c r="AF91" s="105"/>
-      <c r="AG91" s="105"/>
-      <c r="AH91" s="105"/>
-      <c r="AI91" s="105"/>
-      <c r="AJ91" s="105"/>
-      <c r="AK91" s="105"/>
-      <c r="AL91" s="105"/>
-      <c r="AM91" s="105"/>
-      <c r="AN91" s="105"/>
-      <c r="AO91" s="105"/>
-      <c r="AP91" s="105"/>
-      <c r="AQ91" s="105"/>
-      <c r="AR91" s="105"/>
-      <c r="AS91" s="105"/>
-      <c r="AT91" s="105"/>
-      <c r="AU91" s="105"/>
-      <c r="AV91" s="105"/>
-      <c r="AW91" s="105"/>
-      <c r="AX91" s="105"/>
-      <c r="AY91" s="105"/>
-      <c r="AZ91" s="105"/>
-      <c r="BA91" s="105"/>
-      <c r="BB91" s="105"/>
-      <c r="BC91" s="105"/>
-      <c r="BD91" s="106"/>
+      <c r="X91" s="107" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y91" s="108"/>
+      <c r="Z91" s="108"/>
+      <c r="AA91" s="108"/>
+      <c r="AB91" s="108"/>
+      <c r="AC91" s="108"/>
+      <c r="AD91" s="108"/>
+      <c r="AE91" s="108"/>
+      <c r="AF91" s="108"/>
+      <c r="AG91" s="108"/>
+      <c r="AH91" s="108"/>
+      <c r="AI91" s="108"/>
+      <c r="AJ91" s="108"/>
+      <c r="AK91" s="108"/>
+      <c r="AL91" s="108"/>
+      <c r="AM91" s="108"/>
+      <c r="AN91" s="108"/>
+      <c r="AO91" s="108"/>
+      <c r="AP91" s="108"/>
+      <c r="AQ91" s="108"/>
+      <c r="AR91" s="108"/>
+      <c r="AS91" s="108"/>
+      <c r="AT91" s="108"/>
+      <c r="AU91" s="108"/>
+      <c r="AV91" s="108"/>
+      <c r="AW91" s="108"/>
+      <c r="AX91" s="108"/>
+      <c r="AY91" s="108"/>
+      <c r="AZ91" s="108"/>
+      <c r="BA91" s="108"/>
+      <c r="BB91" s="108"/>
+      <c r="BC91" s="108"/>
+      <c r="BD91" s="109"/>
     </row>
     <row r="92" spans="3:56" ht="15" customHeight="1">
       <c r="C92" s="39"/>
@@ -8444,46 +8437,46 @@
       <c r="R92" s="38"/>
       <c r="S92" s="38"/>
       <c r="T92" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U92" s="38"/>
       <c r="V92" s="38"/>
       <c r="W92" s="40"/>
-      <c r="X92" s="104" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y92" s="105"/>
-      <c r="Z92" s="105"/>
-      <c r="AA92" s="105"/>
-      <c r="AB92" s="105"/>
-      <c r="AC92" s="105"/>
-      <c r="AD92" s="105"/>
-      <c r="AE92" s="105"/>
-      <c r="AF92" s="105"/>
-      <c r="AG92" s="105"/>
-      <c r="AH92" s="105"/>
-      <c r="AI92" s="105"/>
-      <c r="AJ92" s="105"/>
-      <c r="AK92" s="105"/>
-      <c r="AL92" s="105"/>
-      <c r="AM92" s="105"/>
-      <c r="AN92" s="105"/>
-      <c r="AO92" s="105"/>
-      <c r="AP92" s="105"/>
-      <c r="AQ92" s="105"/>
-      <c r="AR92" s="105"/>
-      <c r="AS92" s="105"/>
-      <c r="AT92" s="105"/>
-      <c r="AU92" s="105"/>
-      <c r="AV92" s="105"/>
-      <c r="AW92" s="105"/>
-      <c r="AX92" s="105"/>
-      <c r="AY92" s="105"/>
-      <c r="AZ92" s="105"/>
-      <c r="BA92" s="105"/>
-      <c r="BB92" s="105"/>
-      <c r="BC92" s="105"/>
-      <c r="BD92" s="106"/>
+      <c r="X92" s="107" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y92" s="108"/>
+      <c r="Z92" s="108"/>
+      <c r="AA92" s="108"/>
+      <c r="AB92" s="108"/>
+      <c r="AC92" s="108"/>
+      <c r="AD92" s="108"/>
+      <c r="AE92" s="108"/>
+      <c r="AF92" s="108"/>
+      <c r="AG92" s="108"/>
+      <c r="AH92" s="108"/>
+      <c r="AI92" s="108"/>
+      <c r="AJ92" s="108"/>
+      <c r="AK92" s="108"/>
+      <c r="AL92" s="108"/>
+      <c r="AM92" s="108"/>
+      <c r="AN92" s="108"/>
+      <c r="AO92" s="108"/>
+      <c r="AP92" s="108"/>
+      <c r="AQ92" s="108"/>
+      <c r="AR92" s="108"/>
+      <c r="AS92" s="108"/>
+      <c r="AT92" s="108"/>
+      <c r="AU92" s="108"/>
+      <c r="AV92" s="108"/>
+      <c r="AW92" s="108"/>
+      <c r="AX92" s="108"/>
+      <c r="AY92" s="108"/>
+      <c r="AZ92" s="108"/>
+      <c r="BA92" s="108"/>
+      <c r="BB92" s="108"/>
+      <c r="BC92" s="108"/>
+      <c r="BD92" s="109"/>
     </row>
     <row r="93" spans="3:56" ht="15" customHeight="1">
       <c r="C93" s="39"/>
@@ -8508,46 +8501,46 @@
       <c r="R93" s="38"/>
       <c r="S93" s="38"/>
       <c r="T93" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U93" s="38"/>
       <c r="V93" s="38"/>
       <c r="W93" s="40"/>
-      <c r="X93" s="101" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y93" s="102"/>
-      <c r="Z93" s="102"/>
-      <c r="AA93" s="102"/>
-      <c r="AB93" s="102"/>
-      <c r="AC93" s="102"/>
-      <c r="AD93" s="102"/>
-      <c r="AE93" s="102"/>
-      <c r="AF93" s="102"/>
-      <c r="AG93" s="102"/>
-      <c r="AH93" s="102"/>
-      <c r="AI93" s="102"/>
-      <c r="AJ93" s="102"/>
-      <c r="AK93" s="102"/>
-      <c r="AL93" s="102"/>
-      <c r="AM93" s="102"/>
-      <c r="AN93" s="102"/>
-      <c r="AO93" s="102"/>
-      <c r="AP93" s="102"/>
-      <c r="AQ93" s="102"/>
-      <c r="AR93" s="102"/>
-      <c r="AS93" s="102"/>
-      <c r="AT93" s="102"/>
-      <c r="AU93" s="102"/>
-      <c r="AV93" s="102"/>
-      <c r="AW93" s="102"/>
-      <c r="AX93" s="102"/>
-      <c r="AY93" s="102"/>
-      <c r="AZ93" s="102"/>
-      <c r="BA93" s="102"/>
-      <c r="BB93" s="102"/>
-      <c r="BC93" s="102"/>
-      <c r="BD93" s="103"/>
+      <c r="X93" s="160" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y93" s="161"/>
+      <c r="Z93" s="161"/>
+      <c r="AA93" s="161"/>
+      <c r="AB93" s="161"/>
+      <c r="AC93" s="161"/>
+      <c r="AD93" s="161"/>
+      <c r="AE93" s="161"/>
+      <c r="AF93" s="161"/>
+      <c r="AG93" s="161"/>
+      <c r="AH93" s="161"/>
+      <c r="AI93" s="161"/>
+      <c r="AJ93" s="161"/>
+      <c r="AK93" s="161"/>
+      <c r="AL93" s="161"/>
+      <c r="AM93" s="161"/>
+      <c r="AN93" s="161"/>
+      <c r="AO93" s="161"/>
+      <c r="AP93" s="161"/>
+      <c r="AQ93" s="161"/>
+      <c r="AR93" s="161"/>
+      <c r="AS93" s="161"/>
+      <c r="AT93" s="161"/>
+      <c r="AU93" s="161"/>
+      <c r="AV93" s="161"/>
+      <c r="AW93" s="161"/>
+      <c r="AX93" s="161"/>
+      <c r="AY93" s="161"/>
+      <c r="AZ93" s="161"/>
+      <c r="BA93" s="161"/>
+      <c r="BB93" s="161"/>
+      <c r="BC93" s="161"/>
+      <c r="BD93" s="162"/>
     </row>
     <row r="94" spans="3:56" ht="15" customHeight="1">
       <c r="C94" s="39"/>
@@ -8572,46 +8565,46 @@
       <c r="R94" s="38"/>
       <c r="S94" s="38"/>
       <c r="T94" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U94" s="38"/>
       <c r="V94" s="38"/>
       <c r="W94" s="40"/>
-      <c r="X94" s="101" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y94" s="102"/>
-      <c r="Z94" s="102"/>
-      <c r="AA94" s="102"/>
-      <c r="AB94" s="102"/>
-      <c r="AC94" s="102"/>
-      <c r="AD94" s="102"/>
-      <c r="AE94" s="102"/>
-      <c r="AF94" s="102"/>
-      <c r="AG94" s="102"/>
-      <c r="AH94" s="102"/>
-      <c r="AI94" s="102"/>
-      <c r="AJ94" s="102"/>
-      <c r="AK94" s="102"/>
-      <c r="AL94" s="102"/>
-      <c r="AM94" s="102"/>
-      <c r="AN94" s="102"/>
-      <c r="AO94" s="102"/>
-      <c r="AP94" s="102"/>
-      <c r="AQ94" s="102"/>
-      <c r="AR94" s="102"/>
-      <c r="AS94" s="102"/>
-      <c r="AT94" s="102"/>
-      <c r="AU94" s="102"/>
-      <c r="AV94" s="102"/>
-      <c r="AW94" s="102"/>
-      <c r="AX94" s="102"/>
-      <c r="AY94" s="102"/>
-      <c r="AZ94" s="102"/>
-      <c r="BA94" s="102"/>
-      <c r="BB94" s="102"/>
-      <c r="BC94" s="102"/>
-      <c r="BD94" s="103"/>
+      <c r="X94" s="160" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y94" s="161"/>
+      <c r="Z94" s="161"/>
+      <c r="AA94" s="161"/>
+      <c r="AB94" s="161"/>
+      <c r="AC94" s="161"/>
+      <c r="AD94" s="161"/>
+      <c r="AE94" s="161"/>
+      <c r="AF94" s="161"/>
+      <c r="AG94" s="161"/>
+      <c r="AH94" s="161"/>
+      <c r="AI94" s="161"/>
+      <c r="AJ94" s="161"/>
+      <c r="AK94" s="161"/>
+      <c r="AL94" s="161"/>
+      <c r="AM94" s="161"/>
+      <c r="AN94" s="161"/>
+      <c r="AO94" s="161"/>
+      <c r="AP94" s="161"/>
+      <c r="AQ94" s="161"/>
+      <c r="AR94" s="161"/>
+      <c r="AS94" s="161"/>
+      <c r="AT94" s="161"/>
+      <c r="AU94" s="161"/>
+      <c r="AV94" s="161"/>
+      <c r="AW94" s="161"/>
+      <c r="AX94" s="161"/>
+      <c r="AY94" s="161"/>
+      <c r="AZ94" s="161"/>
+      <c r="BA94" s="161"/>
+      <c r="BB94" s="161"/>
+      <c r="BC94" s="161"/>
+      <c r="BD94" s="162"/>
     </row>
     <row r="95" spans="3:56" ht="15" customHeight="1">
       <c r="C95" s="39"/>
@@ -8636,46 +8629,46 @@
       <c r="R95" s="38"/>
       <c r="S95" s="38"/>
       <c r="T95" s="38" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U95" s="38"/>
       <c r="V95" s="38"/>
       <c r="W95" s="40"/>
-      <c r="X95" s="104" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y95" s="105"/>
-      <c r="Z95" s="105"/>
-      <c r="AA95" s="105"/>
-      <c r="AB95" s="105"/>
-      <c r="AC95" s="105"/>
-      <c r="AD95" s="105"/>
-      <c r="AE95" s="105"/>
-      <c r="AF95" s="105"/>
-      <c r="AG95" s="105"/>
-      <c r="AH95" s="105"/>
-      <c r="AI95" s="105"/>
-      <c r="AJ95" s="105"/>
-      <c r="AK95" s="105"/>
-      <c r="AL95" s="105"/>
-      <c r="AM95" s="105"/>
-      <c r="AN95" s="105"/>
-      <c r="AO95" s="105"/>
-      <c r="AP95" s="105"/>
-      <c r="AQ95" s="105"/>
-      <c r="AR95" s="105"/>
-      <c r="AS95" s="105"/>
-      <c r="AT95" s="105"/>
-      <c r="AU95" s="105"/>
-      <c r="AV95" s="105"/>
-      <c r="AW95" s="105"/>
-      <c r="AX95" s="105"/>
-      <c r="AY95" s="105"/>
-      <c r="AZ95" s="105"/>
-      <c r="BA95" s="105"/>
-      <c r="BB95" s="105"/>
-      <c r="BC95" s="105"/>
-      <c r="BD95" s="106"/>
+      <c r="X95" s="107" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y95" s="108"/>
+      <c r="Z95" s="108"/>
+      <c r="AA95" s="108"/>
+      <c r="AB95" s="108"/>
+      <c r="AC95" s="108"/>
+      <c r="AD95" s="108"/>
+      <c r="AE95" s="108"/>
+      <c r="AF95" s="108"/>
+      <c r="AG95" s="108"/>
+      <c r="AH95" s="108"/>
+      <c r="AI95" s="108"/>
+      <c r="AJ95" s="108"/>
+      <c r="AK95" s="108"/>
+      <c r="AL95" s="108"/>
+      <c r="AM95" s="108"/>
+      <c r="AN95" s="108"/>
+      <c r="AO95" s="108"/>
+      <c r="AP95" s="108"/>
+      <c r="AQ95" s="108"/>
+      <c r="AR95" s="108"/>
+      <c r="AS95" s="108"/>
+      <c r="AT95" s="108"/>
+      <c r="AU95" s="108"/>
+      <c r="AV95" s="108"/>
+      <c r="AW95" s="108"/>
+      <c r="AX95" s="108"/>
+      <c r="AY95" s="108"/>
+      <c r="AZ95" s="108"/>
+      <c r="BA95" s="108"/>
+      <c r="BB95" s="108"/>
+      <c r="BC95" s="108"/>
+      <c r="BD95" s="109"/>
     </row>
     <row r="96" spans="3:56" ht="15" customHeight="1">
       <c r="C96" s="39"/>
@@ -8700,46 +8693,46 @@
       <c r="R96" s="38"/>
       <c r="S96" s="38"/>
       <c r="T96" s="38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="U96" s="38"/>
       <c r="V96" s="38"/>
       <c r="W96" s="40"/>
-      <c r="X96" s="101" t="s">
-        <v>126</v>
-      </c>
-      <c r="Y96" s="102"/>
-      <c r="Z96" s="102"/>
-      <c r="AA96" s="102"/>
-      <c r="AB96" s="102"/>
-      <c r="AC96" s="102"/>
-      <c r="AD96" s="102"/>
-      <c r="AE96" s="102"/>
-      <c r="AF96" s="102"/>
-      <c r="AG96" s="102"/>
-      <c r="AH96" s="102"/>
-      <c r="AI96" s="102"/>
-      <c r="AJ96" s="102"/>
-      <c r="AK96" s="102"/>
-      <c r="AL96" s="102"/>
-      <c r="AM96" s="102"/>
-      <c r="AN96" s="102"/>
-      <c r="AO96" s="102"/>
-      <c r="AP96" s="102"/>
-      <c r="AQ96" s="102"/>
-      <c r="AR96" s="102"/>
-      <c r="AS96" s="102"/>
-      <c r="AT96" s="102"/>
-      <c r="AU96" s="102"/>
-      <c r="AV96" s="102"/>
-      <c r="AW96" s="102"/>
-      <c r="AX96" s="102"/>
-      <c r="AY96" s="102"/>
-      <c r="AZ96" s="102"/>
-      <c r="BA96" s="102"/>
-      <c r="BB96" s="102"/>
-      <c r="BC96" s="102"/>
-      <c r="BD96" s="103"/>
+      <c r="X96" s="160" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y96" s="161"/>
+      <c r="Z96" s="161"/>
+      <c r="AA96" s="161"/>
+      <c r="AB96" s="161"/>
+      <c r="AC96" s="161"/>
+      <c r="AD96" s="161"/>
+      <c r="AE96" s="161"/>
+      <c r="AF96" s="161"/>
+      <c r="AG96" s="161"/>
+      <c r="AH96" s="161"/>
+      <c r="AI96" s="161"/>
+      <c r="AJ96" s="161"/>
+      <c r="AK96" s="161"/>
+      <c r="AL96" s="161"/>
+      <c r="AM96" s="161"/>
+      <c r="AN96" s="161"/>
+      <c r="AO96" s="161"/>
+      <c r="AP96" s="161"/>
+      <c r="AQ96" s="161"/>
+      <c r="AR96" s="161"/>
+      <c r="AS96" s="161"/>
+      <c r="AT96" s="161"/>
+      <c r="AU96" s="161"/>
+      <c r="AV96" s="161"/>
+      <c r="AW96" s="161"/>
+      <c r="AX96" s="161"/>
+      <c r="AY96" s="161"/>
+      <c r="AZ96" s="161"/>
+      <c r="BA96" s="161"/>
+      <c r="BB96" s="161"/>
+      <c r="BC96" s="161"/>
+      <c r="BD96" s="162"/>
     </row>
     <row r="97" spans="3:56" ht="15" customHeight="1">
       <c r="C97" s="39"/>
@@ -8764,46 +8757,46 @@
       <c r="R97" s="38"/>
       <c r="S97" s="38"/>
       <c r="T97" s="38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="U97" s="38"/>
       <c r="V97" s="38"/>
       <c r="W97" s="40"/>
-      <c r="X97" s="101" t="s">
-        <v>127</v>
-      </c>
-      <c r="Y97" s="102"/>
-      <c r="Z97" s="102"/>
-      <c r="AA97" s="102"/>
-      <c r="AB97" s="102"/>
-      <c r="AC97" s="102"/>
-      <c r="AD97" s="102"/>
-      <c r="AE97" s="102"/>
-      <c r="AF97" s="102"/>
-      <c r="AG97" s="102"/>
-      <c r="AH97" s="102"/>
-      <c r="AI97" s="102"/>
-      <c r="AJ97" s="102"/>
-      <c r="AK97" s="102"/>
-      <c r="AL97" s="102"/>
-      <c r="AM97" s="102"/>
-      <c r="AN97" s="102"/>
-      <c r="AO97" s="102"/>
-      <c r="AP97" s="102"/>
-      <c r="AQ97" s="102"/>
-      <c r="AR97" s="102"/>
-      <c r="AS97" s="102"/>
-      <c r="AT97" s="102"/>
-      <c r="AU97" s="102"/>
-      <c r="AV97" s="102"/>
-      <c r="AW97" s="102"/>
-      <c r="AX97" s="102"/>
-      <c r="AY97" s="102"/>
-      <c r="AZ97" s="102"/>
-      <c r="BA97" s="102"/>
-      <c r="BB97" s="102"/>
-      <c r="BC97" s="102"/>
-      <c r="BD97" s="103"/>
+      <c r="X97" s="160" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y97" s="161"/>
+      <c r="Z97" s="161"/>
+      <c r="AA97" s="161"/>
+      <c r="AB97" s="161"/>
+      <c r="AC97" s="161"/>
+      <c r="AD97" s="161"/>
+      <c r="AE97" s="161"/>
+      <c r="AF97" s="161"/>
+      <c r="AG97" s="161"/>
+      <c r="AH97" s="161"/>
+      <c r="AI97" s="161"/>
+      <c r="AJ97" s="161"/>
+      <c r="AK97" s="161"/>
+      <c r="AL97" s="161"/>
+      <c r="AM97" s="161"/>
+      <c r="AN97" s="161"/>
+      <c r="AO97" s="161"/>
+      <c r="AP97" s="161"/>
+      <c r="AQ97" s="161"/>
+      <c r="AR97" s="161"/>
+      <c r="AS97" s="161"/>
+      <c r="AT97" s="161"/>
+      <c r="AU97" s="161"/>
+      <c r="AV97" s="161"/>
+      <c r="AW97" s="161"/>
+      <c r="AX97" s="161"/>
+      <c r="AY97" s="161"/>
+      <c r="AZ97" s="161"/>
+      <c r="BA97" s="161"/>
+      <c r="BB97" s="161"/>
+      <c r="BC97" s="161"/>
+      <c r="BD97" s="162"/>
     </row>
     <row r="98" spans="3:56" ht="15" customHeight="1">
       <c r="C98" s="39"/>
@@ -8828,46 +8821,46 @@
       <c r="R98" s="38"/>
       <c r="S98" s="38"/>
       <c r="T98" s="38" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="U98" s="38"/>
       <c r="V98" s="38"/>
       <c r="W98" s="40"/>
-      <c r="X98" s="101" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y98" s="102"/>
-      <c r="Z98" s="102"/>
-      <c r="AA98" s="102"/>
-      <c r="AB98" s="102"/>
-      <c r="AC98" s="102"/>
-      <c r="AD98" s="102"/>
-      <c r="AE98" s="102"/>
-      <c r="AF98" s="102"/>
-      <c r="AG98" s="102"/>
-      <c r="AH98" s="102"/>
-      <c r="AI98" s="102"/>
-      <c r="AJ98" s="102"/>
-      <c r="AK98" s="102"/>
-      <c r="AL98" s="102"/>
-      <c r="AM98" s="102"/>
-      <c r="AN98" s="102"/>
-      <c r="AO98" s="102"/>
-      <c r="AP98" s="102"/>
-      <c r="AQ98" s="102"/>
-      <c r="AR98" s="102"/>
-      <c r="AS98" s="102"/>
-      <c r="AT98" s="102"/>
-      <c r="AU98" s="102"/>
-      <c r="AV98" s="102"/>
-      <c r="AW98" s="102"/>
-      <c r="AX98" s="102"/>
-      <c r="AY98" s="102"/>
-      <c r="AZ98" s="102"/>
-      <c r="BA98" s="102"/>
-      <c r="BB98" s="102"/>
-      <c r="BC98" s="102"/>
-      <c r="BD98" s="103"/>
+      <c r="X98" s="160" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y98" s="161"/>
+      <c r="Z98" s="161"/>
+      <c r="AA98" s="161"/>
+      <c r="AB98" s="161"/>
+      <c r="AC98" s="161"/>
+      <c r="AD98" s="161"/>
+      <c r="AE98" s="161"/>
+      <c r="AF98" s="161"/>
+      <c r="AG98" s="161"/>
+      <c r="AH98" s="161"/>
+      <c r="AI98" s="161"/>
+      <c r="AJ98" s="161"/>
+      <c r="AK98" s="161"/>
+      <c r="AL98" s="161"/>
+      <c r="AM98" s="161"/>
+      <c r="AN98" s="161"/>
+      <c r="AO98" s="161"/>
+      <c r="AP98" s="161"/>
+      <c r="AQ98" s="161"/>
+      <c r="AR98" s="161"/>
+      <c r="AS98" s="161"/>
+      <c r="AT98" s="161"/>
+      <c r="AU98" s="161"/>
+      <c r="AV98" s="161"/>
+      <c r="AW98" s="161"/>
+      <c r="AX98" s="161"/>
+      <c r="AY98" s="161"/>
+      <c r="AZ98" s="161"/>
+      <c r="BA98" s="161"/>
+      <c r="BB98" s="161"/>
+      <c r="BC98" s="161"/>
+      <c r="BD98" s="162"/>
     </row>
     <row r="99" spans="3:56" ht="15" customHeight="1">
       <c r="C99" s="39"/>
@@ -8892,46 +8885,46 @@
       <c r="R99" s="38"/>
       <c r="S99" s="38"/>
       <c r="T99" s="38" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="U99" s="38"/>
       <c r="V99" s="38"/>
       <c r="W99" s="40"/>
-      <c r="X99" s="101" t="s">
+      <c r="X99" s="160" t="s">
         <v>78</v>
       </c>
-      <c r="Y99" s="102"/>
-      <c r="Z99" s="102"/>
-      <c r="AA99" s="102"/>
-      <c r="AB99" s="102"/>
-      <c r="AC99" s="102"/>
-      <c r="AD99" s="102"/>
-      <c r="AE99" s="102"/>
-      <c r="AF99" s="102"/>
-      <c r="AG99" s="102"/>
-      <c r="AH99" s="102"/>
-      <c r="AI99" s="102"/>
-      <c r="AJ99" s="102"/>
-      <c r="AK99" s="102"/>
-      <c r="AL99" s="102"/>
-      <c r="AM99" s="102"/>
-      <c r="AN99" s="102"/>
-      <c r="AO99" s="102"/>
-      <c r="AP99" s="102"/>
-      <c r="AQ99" s="102"/>
-      <c r="AR99" s="102"/>
-      <c r="AS99" s="102"/>
-      <c r="AT99" s="102"/>
-      <c r="AU99" s="102"/>
-      <c r="AV99" s="102"/>
-      <c r="AW99" s="102"/>
-      <c r="AX99" s="102"/>
-      <c r="AY99" s="102"/>
-      <c r="AZ99" s="102"/>
-      <c r="BA99" s="102"/>
-      <c r="BB99" s="102"/>
-      <c r="BC99" s="102"/>
-      <c r="BD99" s="103"/>
+      <c r="Y99" s="161"/>
+      <c r="Z99" s="161"/>
+      <c r="AA99" s="161"/>
+      <c r="AB99" s="161"/>
+      <c r="AC99" s="161"/>
+      <c r="AD99" s="161"/>
+      <c r="AE99" s="161"/>
+      <c r="AF99" s="161"/>
+      <c r="AG99" s="161"/>
+      <c r="AH99" s="161"/>
+      <c r="AI99" s="161"/>
+      <c r="AJ99" s="161"/>
+      <c r="AK99" s="161"/>
+      <c r="AL99" s="161"/>
+      <c r="AM99" s="161"/>
+      <c r="AN99" s="161"/>
+      <c r="AO99" s="161"/>
+      <c r="AP99" s="161"/>
+      <c r="AQ99" s="161"/>
+      <c r="AR99" s="161"/>
+      <c r="AS99" s="161"/>
+      <c r="AT99" s="161"/>
+      <c r="AU99" s="161"/>
+      <c r="AV99" s="161"/>
+      <c r="AW99" s="161"/>
+      <c r="AX99" s="161"/>
+      <c r="AY99" s="161"/>
+      <c r="AZ99" s="161"/>
+      <c r="BA99" s="161"/>
+      <c r="BB99" s="161"/>
+      <c r="BC99" s="161"/>
+      <c r="BD99" s="162"/>
     </row>
     <row r="100" spans="3:56">
       <c r="C100" s="39"/>
@@ -9047,25 +9040,61 @@
     </row>
   </sheetData>
   <mergeCells count="90">
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:AP3"/>
-    <mergeCell ref="AQ2:AW2"/>
-    <mergeCell ref="AX2:BE2"/>
-    <mergeCell ref="AQ3:AW3"/>
-    <mergeCell ref="AX3:BE3"/>
-    <mergeCell ref="AT4:AW4"/>
-    <mergeCell ref="BB4:BE4"/>
-    <mergeCell ref="F5:N5"/>
-    <mergeCell ref="U5:AP5"/>
-    <mergeCell ref="AT5:AW5"/>
-    <mergeCell ref="BB5:BE5"/>
-    <mergeCell ref="AX4:BA4"/>
-    <mergeCell ref="AX5:BA5"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="E88:Q88"/>
-    <mergeCell ref="R88:W88"/>
-    <mergeCell ref="E70:Q70"/>
-    <mergeCell ref="E72:Q72"/>
+    <mergeCell ref="X97:BD97"/>
+    <mergeCell ref="X98:BD98"/>
+    <mergeCell ref="X99:BD99"/>
+    <mergeCell ref="X91:BD91"/>
+    <mergeCell ref="X92:BD92"/>
+    <mergeCell ref="X93:BD93"/>
+    <mergeCell ref="X94:BD94"/>
+    <mergeCell ref="X95:BD95"/>
+    <mergeCell ref="X72:AD72"/>
+    <mergeCell ref="AE72:AK72"/>
+    <mergeCell ref="X89:BD89"/>
+    <mergeCell ref="X90:BD90"/>
+    <mergeCell ref="X96:BD96"/>
+    <mergeCell ref="X88:BD88"/>
+    <mergeCell ref="AU23:AZ24"/>
+    <mergeCell ref="BA23:BA24"/>
+    <mergeCell ref="X70:AD70"/>
+    <mergeCell ref="AE70:AK70"/>
+    <mergeCell ref="E71:Q71"/>
+    <mergeCell ref="X71:AD71"/>
+    <mergeCell ref="AE71:AK71"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="O4:T4"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="U4:AP4"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="C41:G41"/>
+    <mergeCell ref="C67:J67"/>
+    <mergeCell ref="AE43:AI43"/>
+    <mergeCell ref="AJ43:AM43"/>
+    <mergeCell ref="AL12:AN13"/>
+    <mergeCell ref="AG12:AJ13"/>
+    <mergeCell ref="AB23:AE24"/>
+    <mergeCell ref="AF23:AL24"/>
+    <mergeCell ref="AN23:AT24"/>
+    <mergeCell ref="AQ46:AV46"/>
+    <mergeCell ref="D10:G15"/>
+    <mergeCell ref="H10:U15"/>
+    <mergeCell ref="AQ43:AV43"/>
+    <mergeCell ref="AW43:BD43"/>
+    <mergeCell ref="X23:AA24"/>
+    <mergeCell ref="H22:L22"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="J23:P24"/>
+    <mergeCell ref="Q23:W24"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="AN20:AR20"/>
+    <mergeCell ref="AV20:AZ20"/>
+    <mergeCell ref="AP12:AR13"/>
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="E69:Q69"/>
     <mergeCell ref="AT12:AV13"/>
@@ -9082,61 +9111,25 @@
     <mergeCell ref="R69:W69"/>
     <mergeCell ref="X69:AD69"/>
     <mergeCell ref="AE69:AK69"/>
-    <mergeCell ref="AQ46:AV46"/>
-    <mergeCell ref="D10:G15"/>
-    <mergeCell ref="H10:U15"/>
-    <mergeCell ref="AQ43:AV43"/>
-    <mergeCell ref="AW43:BD43"/>
-    <mergeCell ref="X23:AA24"/>
-    <mergeCell ref="H22:L22"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="H23:I24"/>
-    <mergeCell ref="J23:P24"/>
-    <mergeCell ref="Q23:W24"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C41:G41"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="AE43:AI43"/>
-    <mergeCell ref="AJ43:AM43"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="O4:T4"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="F4:N4"/>
-    <mergeCell ref="U4:AP4"/>
-    <mergeCell ref="AN20:AR20"/>
-    <mergeCell ref="AV20:AZ20"/>
-    <mergeCell ref="AL12:AN13"/>
-    <mergeCell ref="AP12:AR13"/>
-    <mergeCell ref="AG12:AJ13"/>
-    <mergeCell ref="AB23:AE24"/>
-    <mergeCell ref="AF23:AL24"/>
-    <mergeCell ref="AN23:AT24"/>
-    <mergeCell ref="AU23:AZ24"/>
-    <mergeCell ref="BA23:BA24"/>
-    <mergeCell ref="X70:AD70"/>
-    <mergeCell ref="AE70:AK70"/>
-    <mergeCell ref="E71:Q71"/>
-    <mergeCell ref="X71:AD71"/>
-    <mergeCell ref="AE71:AK71"/>
-    <mergeCell ref="X72:AD72"/>
-    <mergeCell ref="AE72:AK72"/>
-    <mergeCell ref="X89:BD89"/>
-    <mergeCell ref="X90:BD90"/>
-    <mergeCell ref="X96:BD96"/>
-    <mergeCell ref="X88:BD88"/>
-    <mergeCell ref="X97:BD97"/>
-    <mergeCell ref="X98:BD98"/>
-    <mergeCell ref="X99:BD99"/>
-    <mergeCell ref="X91:BD91"/>
-    <mergeCell ref="X92:BD92"/>
-    <mergeCell ref="X93:BD93"/>
-    <mergeCell ref="X94:BD94"/>
-    <mergeCell ref="X95:BD95"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="E88:Q88"/>
+    <mergeCell ref="R88:W88"/>
+    <mergeCell ref="E70:Q70"/>
+    <mergeCell ref="E72:Q72"/>
+    <mergeCell ref="AT4:AW4"/>
+    <mergeCell ref="BB4:BE4"/>
+    <mergeCell ref="F5:N5"/>
+    <mergeCell ref="U5:AP5"/>
+    <mergeCell ref="AT5:AW5"/>
+    <mergeCell ref="BB5:BE5"/>
+    <mergeCell ref="AX4:BA4"/>
+    <mergeCell ref="AX5:BA5"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:AP3"/>
+    <mergeCell ref="AQ2:AW2"/>
+    <mergeCell ref="AX2:BE2"/>
+    <mergeCell ref="AQ3:AW3"/>
+    <mergeCell ref="AX3:BE3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="87" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update sau khi fix review
</commit_message>
<xml_diff>
--- a/Document/Design/SDD_UserManager.xlsx
+++ b/Document/Design/SDD_UserManager.xlsx
@@ -1072,7 +1072,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="133">
   <si>
     <t>&lt;Project Name&gt;</t>
   </si>
@@ -1410,9 +1410,6 @@
     <t>cboSelectLogStatus(chọn user theo trạng thái login)</t>
   </si>
   <si>
-    <t>LogStatus</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
@@ -1462,6 +1459,18 @@
   </si>
   <si>
     <t>21/10/2011</t>
+  </si>
+  <si>
+    <t>btnDelete(xóa user)</t>
+  </si>
+  <si>
+    <t>All column</t>
+  </si>
+  <si>
+    <t>btnLogout(đăng xuất user)</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -2368,7 +2377,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2586,9 +2595,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2653,6 +2659,39 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2689,13 +2728,46 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2713,30 +2785,36 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2755,54 +2833,6 @@
     <xf numFmtId="0" fontId="18" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2811,6 +2841,21 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3179,14 +3224,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="33">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="1" t="s">
@@ -3406,12 +3451,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="33">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
     </row>
     <row r="5" spans="2:5" ht="15.75">
       <c r="B5" s="21" t="s">
@@ -3473,16 +3518,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="33">
-      <c r="B2" s="90" t="s">
+      <c r="B2" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="90"/>
-      <c r="D2" s="90"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
     </row>
     <row r="4" spans="2:4" ht="15">
       <c r="B4" s="22"/>
-      <c r="C4" s="89" t="s">
-        <v>128</v>
+      <c r="C4" s="88" t="s">
+        <v>127</v>
       </c>
       <c r="D4" s="23"/>
     </row>
@@ -3653,8 +3698,8 @@
   <dimension ref="B2:BE101"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BB5" sqref="BB5:BE5"/>
+      <pane ySplit="5" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R79" sqref="R79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.140625" defaultRowHeight="12.75"/>
@@ -3678,311 +3723,311 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:57">
-      <c r="B2" s="91" t="s">
+      <c r="B2" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="92" t="s">
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="92"/>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="92"/>
-      <c r="V2" s="92"/>
-      <c r="W2" s="92"/>
-      <c r="X2" s="92"/>
-      <c r="Y2" s="92"/>
-      <c r="Z2" s="92"/>
-      <c r="AA2" s="92"/>
-      <c r="AB2" s="92"/>
-      <c r="AC2" s="92"/>
-      <c r="AD2" s="92"/>
-      <c r="AE2" s="92"/>
-      <c r="AF2" s="92"/>
-      <c r="AG2" s="92"/>
-      <c r="AH2" s="92"/>
-      <c r="AI2" s="92"/>
-      <c r="AJ2" s="92"/>
-      <c r="AK2" s="92"/>
-      <c r="AL2" s="92"/>
-      <c r="AM2" s="92"/>
-      <c r="AN2" s="92"/>
-      <c r="AO2" s="92"/>
-      <c r="AP2" s="92"/>
-      <c r="AQ2" s="93" t="s">
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="91"/>
+      <c r="Q2" s="91"/>
+      <c r="R2" s="91"/>
+      <c r="S2" s="91"/>
+      <c r="T2" s="91"/>
+      <c r="U2" s="91"/>
+      <c r="V2" s="91"/>
+      <c r="W2" s="91"/>
+      <c r="X2" s="91"/>
+      <c r="Y2" s="91"/>
+      <c r="Z2" s="91"/>
+      <c r="AA2" s="91"/>
+      <c r="AB2" s="91"/>
+      <c r="AC2" s="91"/>
+      <c r="AD2" s="91"/>
+      <c r="AE2" s="91"/>
+      <c r="AF2" s="91"/>
+      <c r="AG2" s="91"/>
+      <c r="AH2" s="91"/>
+      <c r="AI2" s="91"/>
+      <c r="AJ2" s="91"/>
+      <c r="AK2" s="91"/>
+      <c r="AL2" s="91"/>
+      <c r="AM2" s="91"/>
+      <c r="AN2" s="91"/>
+      <c r="AO2" s="91"/>
+      <c r="AP2" s="91"/>
+      <c r="AQ2" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="AR2" s="93"/>
-      <c r="AS2" s="93"/>
-      <c r="AT2" s="93"/>
-      <c r="AU2" s="93"/>
-      <c r="AV2" s="93"/>
-      <c r="AW2" s="93"/>
-      <c r="AX2" s="93" t="s">
+      <c r="AR2" s="92"/>
+      <c r="AS2" s="92"/>
+      <c r="AT2" s="92"/>
+      <c r="AU2" s="92"/>
+      <c r="AV2" s="92"/>
+      <c r="AW2" s="92"/>
+      <c r="AX2" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="AY2" s="93"/>
-      <c r="AZ2" s="93"/>
-      <c r="BA2" s="93"/>
-      <c r="BB2" s="93"/>
-      <c r="BC2" s="93"/>
-      <c r="BD2" s="93"/>
-      <c r="BE2" s="93"/>
+      <c r="AY2" s="92"/>
+      <c r="AZ2" s="92"/>
+      <c r="BA2" s="92"/>
+      <c r="BB2" s="92"/>
+      <c r="BC2" s="92"/>
+      <c r="BD2" s="92"/>
+      <c r="BE2" s="92"/>
     </row>
     <row r="3" spans="2:57">
-      <c r="B3" s="91"/>
-      <c r="C3" s="91"/>
-      <c r="D3" s="91"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="92"/>
-      <c r="T3" s="92"/>
-      <c r="U3" s="92"/>
-      <c r="V3" s="92"/>
-      <c r="W3" s="92"/>
-      <c r="X3" s="92"/>
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="92"/>
-      <c r="AB3" s="92"/>
-      <c r="AC3" s="92"/>
-      <c r="AD3" s="92"/>
-      <c r="AE3" s="92"/>
-      <c r="AF3" s="92"/>
-      <c r="AG3" s="92"/>
-      <c r="AH3" s="92"/>
-      <c r="AI3" s="92"/>
-      <c r="AJ3" s="92"/>
-      <c r="AK3" s="92"/>
-      <c r="AL3" s="92"/>
-      <c r="AM3" s="92"/>
-      <c r="AN3" s="92"/>
-      <c r="AO3" s="92"/>
-      <c r="AP3" s="92"/>
-      <c r="AQ3" s="94" t="s">
+      <c r="B3" s="90"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="91"/>
+      <c r="Q3" s="91"/>
+      <c r="R3" s="91"/>
+      <c r="S3" s="91"/>
+      <c r="T3" s="91"/>
+      <c r="U3" s="91"/>
+      <c r="V3" s="91"/>
+      <c r="W3" s="91"/>
+      <c r="X3" s="91"/>
+      <c r="Y3" s="91"/>
+      <c r="Z3" s="91"/>
+      <c r="AA3" s="91"/>
+      <c r="AB3" s="91"/>
+      <c r="AC3" s="91"/>
+      <c r="AD3" s="91"/>
+      <c r="AE3" s="91"/>
+      <c r="AF3" s="91"/>
+      <c r="AG3" s="91"/>
+      <c r="AH3" s="91"/>
+      <c r="AI3" s="91"/>
+      <c r="AJ3" s="91"/>
+      <c r="AK3" s="91"/>
+      <c r="AL3" s="91"/>
+      <c r="AM3" s="91"/>
+      <c r="AN3" s="91"/>
+      <c r="AO3" s="91"/>
+      <c r="AP3" s="91"/>
+      <c r="AQ3" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="AR3" s="94"/>
-      <c r="AS3" s="94"/>
-      <c r="AT3" s="94"/>
-      <c r="AU3" s="94"/>
-      <c r="AV3" s="94"/>
-      <c r="AW3" s="94"/>
-      <c r="AX3" s="94" t="s">
+      <c r="AR3" s="93"/>
+      <c r="AS3" s="93"/>
+      <c r="AT3" s="93"/>
+      <c r="AU3" s="93"/>
+      <c r="AV3" s="93"/>
+      <c r="AW3" s="93"/>
+      <c r="AX3" s="93" t="s">
+        <v>125</v>
+      </c>
+      <c r="AY3" s="93"/>
+      <c r="AZ3" s="93"/>
+      <c r="BA3" s="93"/>
+      <c r="BB3" s="93"/>
+      <c r="BC3" s="93"/>
+      <c r="BD3" s="93"/>
+      <c r="BE3" s="93"/>
+    </row>
+    <row r="4" spans="2:57">
+      <c r="B4" s="152" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="153"/>
+      <c r="F4" s="94"/>
+      <c r="G4" s="94"/>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
+      <c r="M4" s="94"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="98" t="s">
+        <v>27</v>
+      </c>
+      <c r="P4" s="99"/>
+      <c r="Q4" s="99"/>
+      <c r="R4" s="99"/>
+      <c r="S4" s="99"/>
+      <c r="T4" s="100"/>
+      <c r="U4" s="94" t="s">
+        <v>82</v>
+      </c>
+      <c r="V4" s="94"/>
+      <c r="W4" s="94"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="94"/>
+      <c r="AD4" s="94"/>
+      <c r="AE4" s="94"/>
+      <c r="AF4" s="94"/>
+      <c r="AG4" s="94"/>
+      <c r="AH4" s="94"/>
+      <c r="AI4" s="94"/>
+      <c r="AJ4" s="94"/>
+      <c r="AK4" s="94"/>
+      <c r="AL4" s="94"/>
+      <c r="AM4" s="94"/>
+      <c r="AN4" s="94"/>
+      <c r="AO4" s="94"/>
+      <c r="AP4" s="94"/>
+      <c r="AQ4" s="95" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR4" s="96"/>
+      <c r="AS4" s="97"/>
+      <c r="AT4" s="94" t="s">
+        <v>83</v>
+      </c>
+      <c r="AU4" s="94"/>
+      <c r="AV4" s="94"/>
+      <c r="AW4" s="94"/>
+      <c r="AX4" s="95" t="s">
+        <v>24</v>
+      </c>
+      <c r="AY4" s="96"/>
+      <c r="AZ4" s="96"/>
+      <c r="BA4" s="97"/>
+      <c r="BB4" s="94" t="s">
         <v>126</v>
       </c>
-      <c r="AY3" s="94"/>
-      <c r="AZ3" s="94"/>
-      <c r="BA3" s="94"/>
-      <c r="BB3" s="94"/>
-      <c r="BC3" s="94"/>
-      <c r="BD3" s="94"/>
-      <c r="BE3" s="94"/>
-    </row>
-    <row r="4" spans="2:57">
-      <c r="B4" s="146" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="147"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="99" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
-      <c r="T4" s="101"/>
-      <c r="U4" s="95" t="s">
-        <v>82</v>
-      </c>
-      <c r="V4" s="95"/>
-      <c r="W4" s="95"/>
-      <c r="X4" s="95"/>
-      <c r="Y4" s="95"/>
-      <c r="Z4" s="95"/>
-      <c r="AA4" s="95"/>
-      <c r="AB4" s="95"/>
-      <c r="AC4" s="95"/>
-      <c r="AD4" s="95"/>
-      <c r="AE4" s="95"/>
-      <c r="AF4" s="95"/>
-      <c r="AG4" s="95"/>
-      <c r="AH4" s="95"/>
-      <c r="AI4" s="95"/>
-      <c r="AJ4" s="95"/>
-      <c r="AK4" s="95"/>
-      <c r="AL4" s="95"/>
-      <c r="AM4" s="95"/>
-      <c r="AN4" s="95"/>
-      <c r="AO4" s="95"/>
-      <c r="AP4" s="95"/>
-      <c r="AQ4" s="96" t="s">
+      <c r="BC4" s="94"/>
+      <c r="BD4" s="94"/>
+      <c r="BE4" s="94"/>
+    </row>
+    <row r="5" spans="2:57">
+      <c r="B5" s="99" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="98" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="99"/>
+      <c r="Q5" s="99"/>
+      <c r="R5" s="99"/>
+      <c r="S5" s="99"/>
+      <c r="T5" s="100"/>
+      <c r="U5" s="94"/>
+      <c r="V5" s="94"/>
+      <c r="W5" s="94"/>
+      <c r="X5" s="94"/>
+      <c r="Y5" s="94"/>
+      <c r="Z5" s="94"/>
+      <c r="AA5" s="94"/>
+      <c r="AB5" s="94"/>
+      <c r="AC5" s="94"/>
+      <c r="AD5" s="94"/>
+      <c r="AE5" s="94"/>
+      <c r="AF5" s="94"/>
+      <c r="AG5" s="94"/>
+      <c r="AH5" s="94"/>
+      <c r="AI5" s="94"/>
+      <c r="AJ5" s="94"/>
+      <c r="AK5" s="94"/>
+      <c r="AL5" s="94"/>
+      <c r="AM5" s="94"/>
+      <c r="AN5" s="94"/>
+      <c r="AO5" s="94"/>
+      <c r="AP5" s="94"/>
+      <c r="AQ5" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="AR4" s="97"/>
-      <c r="AS4" s="98"/>
-      <c r="AT4" s="95" t="s">
+      <c r="AR5" s="154"/>
+      <c r="AS5" s="100"/>
+      <c r="AT5" s="94" t="s">
         <v>83</v>
       </c>
-      <c r="AU4" s="95"/>
-      <c r="AV4" s="95"/>
-      <c r="AW4" s="95"/>
-      <c r="AX4" s="96" t="s">
+      <c r="AU5" s="94"/>
+      <c r="AV5" s="94"/>
+      <c r="AW5" s="94"/>
+      <c r="AX5" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="AY4" s="97"/>
-      <c r="AZ4" s="97"/>
-      <c r="BA4" s="98"/>
-      <c r="BB4" s="95" t="s">
-        <v>127</v>
-      </c>
-      <c r="BC4" s="95"/>
-      <c r="BD4" s="95"/>
-      <c r="BE4" s="95"/>
-    </row>
-    <row r="5" spans="2:57">
-      <c r="B5" s="100" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="95"/>
-      <c r="L5" s="95"/>
-      <c r="M5" s="95"/>
-      <c r="N5" s="95"/>
-      <c r="O5" s="99" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
-      <c r="S5" s="100"/>
-      <c r="T5" s="101"/>
-      <c r="U5" s="95"/>
-      <c r="V5" s="95"/>
-      <c r="W5" s="95"/>
-      <c r="X5" s="95"/>
-      <c r="Y5" s="95"/>
-      <c r="Z5" s="95"/>
-      <c r="AA5" s="95"/>
-      <c r="AB5" s="95"/>
-      <c r="AC5" s="95"/>
-      <c r="AD5" s="95"/>
-      <c r="AE5" s="95"/>
-      <c r="AF5" s="95"/>
-      <c r="AG5" s="95"/>
-      <c r="AH5" s="95"/>
-      <c r="AI5" s="95"/>
-      <c r="AJ5" s="95"/>
-      <c r="AK5" s="95"/>
-      <c r="AL5" s="95"/>
-      <c r="AM5" s="95"/>
-      <c r="AN5" s="95"/>
-      <c r="AO5" s="95"/>
-      <c r="AP5" s="95"/>
-      <c r="AQ5" s="99" t="s">
-        <v>23</v>
-      </c>
-      <c r="AR5" s="148"/>
-      <c r="AS5" s="101"/>
-      <c r="AT5" s="95" t="s">
-        <v>83</v>
-      </c>
-      <c r="AU5" s="95"/>
-      <c r="AV5" s="95"/>
-      <c r="AW5" s="95"/>
-      <c r="AX5" s="99" t="s">
-        <v>24</v>
-      </c>
-      <c r="AY5" s="100"/>
-      <c r="AZ5" s="100"/>
-      <c r="BA5" s="101"/>
-      <c r="BB5" s="95" t="s">
-        <v>129</v>
-      </c>
-      <c r="BC5" s="95"/>
-      <c r="BD5" s="95"/>
-      <c r="BE5" s="95"/>
+      <c r="AY5" s="99"/>
+      <c r="AZ5" s="99"/>
+      <c r="BA5" s="100"/>
+      <c r="BB5" s="94" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC5" s="94"/>
+      <c r="BD5" s="94"/>
+      <c r="BE5" s="94"/>
     </row>
     <row r="7" spans="2:57">
-      <c r="C7" s="144" t="s">
+      <c r="C7" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="144"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
     </row>
     <row r="9" spans="2:57" ht="13.5" thickBot="1">
       <c r="C9" s="32"/>
     </row>
     <row r="10" spans="2:57" ht="15" customHeight="1">
-      <c r="D10" s="110" t="s">
+      <c r="D10" s="120" t="s">
         <v>86</v>
       </c>
-      <c r="E10" s="111"/>
-      <c r="F10" s="111"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="128" t="s">
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="122"/>
+      <c r="H10" s="149" t="s">
         <v>87</v>
       </c>
-      <c r="I10" s="128"/>
-      <c r="J10" s="128"/>
-      <c r="K10" s="128"/>
-      <c r="L10" s="128"/>
-      <c r="M10" s="128"/>
-      <c r="N10" s="128"/>
-      <c r="O10" s="128"/>
-      <c r="P10" s="128"/>
-      <c r="Q10" s="128"/>
-      <c r="R10" s="128"/>
-      <c r="S10" s="128"/>
-      <c r="T10" s="128"/>
-      <c r="U10" s="128"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="149"/>
+      <c r="L10" s="149"/>
+      <c r="M10" s="149"/>
+      <c r="N10" s="149"/>
+      <c r="O10" s="149"/>
+      <c r="P10" s="149"/>
+      <c r="Q10" s="149"/>
+      <c r="R10" s="149"/>
+      <c r="S10" s="149"/>
+      <c r="T10" s="149"/>
+      <c r="U10" s="149"/>
       <c r="V10" s="70"/>
       <c r="W10" s="70"/>
       <c r="X10" s="70"/>
@@ -4019,24 +4064,24 @@
       <c r="BC10" s="71"/>
     </row>
     <row r="11" spans="2:57" ht="13.5" thickBot="1">
-      <c r="D11" s="125"/>
-      <c r="E11" s="126"/>
-      <c r="F11" s="126"/>
-      <c r="G11" s="127"/>
-      <c r="H11" s="129"/>
-      <c r="I11" s="129"/>
-      <c r="J11" s="129"/>
-      <c r="K11" s="129"/>
-      <c r="L11" s="129"/>
-      <c r="M11" s="129"/>
-      <c r="N11" s="129"/>
-      <c r="O11" s="129"/>
-      <c r="P11" s="129"/>
-      <c r="Q11" s="129"/>
-      <c r="R11" s="129"/>
-      <c r="S11" s="129"/>
-      <c r="T11" s="129"/>
-      <c r="U11" s="129"/>
+      <c r="D11" s="146"/>
+      <c r="E11" s="147"/>
+      <c r="F11" s="147"/>
+      <c r="G11" s="148"/>
+      <c r="H11" s="150"/>
+      <c r="I11" s="150"/>
+      <c r="J11" s="150"/>
+      <c r="K11" s="150"/>
+      <c r="L11" s="150"/>
+      <c r="M11" s="150"/>
+      <c r="N11" s="150"/>
+      <c r="O11" s="150"/>
+      <c r="P11" s="150"/>
+      <c r="Q11" s="150"/>
+      <c r="R11" s="150"/>
+      <c r="S11" s="150"/>
+      <c r="T11" s="150"/>
+      <c r="U11" s="150"/>
       <c r="V11" s="72"/>
       <c r="W11" s="72"/>
       <c r="X11" s="72"/>
@@ -4073,24 +4118,24 @@
       <c r="BC11" s="73"/>
     </row>
     <row r="12" spans="2:57" ht="15" customHeight="1">
-      <c r="D12" s="125"/>
-      <c r="E12" s="126"/>
-      <c r="F12" s="126"/>
-      <c r="G12" s="127"/>
-      <c r="H12" s="129"/>
-      <c r="I12" s="129"/>
-      <c r="J12" s="129"/>
-      <c r="K12" s="129"/>
-      <c r="L12" s="129"/>
-      <c r="M12" s="129"/>
-      <c r="N12" s="129"/>
-      <c r="O12" s="129"/>
-      <c r="P12" s="129"/>
-      <c r="Q12" s="129"/>
-      <c r="R12" s="129"/>
-      <c r="S12" s="129"/>
-      <c r="T12" s="129"/>
-      <c r="U12" s="129"/>
+      <c r="D12" s="146"/>
+      <c r="E12" s="147"/>
+      <c r="F12" s="147"/>
+      <c r="G12" s="148"/>
+      <c r="H12" s="150"/>
+      <c r="I12" s="150"/>
+      <c r="J12" s="150"/>
+      <c r="K12" s="150"/>
+      <c r="L12" s="150"/>
+      <c r="M12" s="150"/>
+      <c r="N12" s="150"/>
+      <c r="O12" s="150"/>
+      <c r="P12" s="150"/>
+      <c r="Q12" s="150"/>
+      <c r="R12" s="150"/>
+      <c r="S12" s="150"/>
+      <c r="T12" s="150"/>
+      <c r="U12" s="150"/>
       <c r="V12" s="72"/>
       <c r="W12" s="72"/>
       <c r="X12" s="72"/>
@@ -4102,59 +4147,59 @@
       <c r="AD12" s="72"/>
       <c r="AE12" s="72"/>
       <c r="AF12" s="72"/>
-      <c r="AG12" s="149" t="s">
+      <c r="AG12" s="134" t="s">
         <v>88</v>
       </c>
-      <c r="AH12" s="150"/>
-      <c r="AI12" s="150"/>
-      <c r="AJ12" s="151"/>
+      <c r="AH12" s="135"/>
+      <c r="AI12" s="135"/>
+      <c r="AJ12" s="136"/>
       <c r="AK12" s="72"/>
-      <c r="AL12" s="110" t="s">
+      <c r="AL12" s="120" t="s">
         <v>89</v>
       </c>
-      <c r="AM12" s="111"/>
-      <c r="AN12" s="112"/>
+      <c r="AM12" s="121"/>
+      <c r="AN12" s="122"/>
       <c r="AO12" s="72"/>
-      <c r="AP12" s="110" t="s">
+      <c r="AP12" s="120" t="s">
         <v>90</v>
       </c>
-      <c r="AQ12" s="111"/>
-      <c r="AR12" s="112"/>
+      <c r="AQ12" s="121"/>
+      <c r="AR12" s="122"/>
       <c r="AS12" s="72"/>
-      <c r="AT12" s="110" t="s">
+      <c r="AT12" s="120" t="s">
         <v>91</v>
       </c>
-      <c r="AU12" s="111"/>
-      <c r="AV12" s="112"/>
+      <c r="AU12" s="121"/>
+      <c r="AV12" s="122"/>
       <c r="AW12" s="75"/>
-      <c r="AX12" s="110" t="s">
+      <c r="AX12" s="120" t="s">
         <v>92</v>
       </c>
-      <c r="AY12" s="111"/>
-      <c r="AZ12" s="112"/>
+      <c r="AY12" s="121"/>
+      <c r="AZ12" s="122"/>
       <c r="BA12" s="72"/>
       <c r="BB12" s="72"/>
       <c r="BC12" s="73"/>
     </row>
     <row r="13" spans="2:57" ht="15.75" customHeight="1" thickBot="1">
-      <c r="D13" s="125"/>
-      <c r="E13" s="126"/>
-      <c r="F13" s="126"/>
-      <c r="G13" s="127"/>
-      <c r="H13" s="129"/>
-      <c r="I13" s="129"/>
-      <c r="J13" s="129"/>
-      <c r="K13" s="129"/>
-      <c r="L13" s="129"/>
-      <c r="M13" s="129"/>
-      <c r="N13" s="129"/>
-      <c r="O13" s="129"/>
-      <c r="P13" s="129"/>
-      <c r="Q13" s="129"/>
-      <c r="R13" s="129"/>
-      <c r="S13" s="129"/>
-      <c r="T13" s="129"/>
-      <c r="U13" s="129"/>
+      <c r="D13" s="146"/>
+      <c r="E13" s="147"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="148"/>
+      <c r="H13" s="150"/>
+      <c r="I13" s="150"/>
+      <c r="J13" s="150"/>
+      <c r="K13" s="150"/>
+      <c r="L13" s="150"/>
+      <c r="M13" s="150"/>
+      <c r="N13" s="150"/>
+      <c r="O13" s="150"/>
+      <c r="P13" s="150"/>
+      <c r="Q13" s="150"/>
+      <c r="R13" s="150"/>
+      <c r="S13" s="150"/>
+      <c r="T13" s="150"/>
+      <c r="U13" s="150"/>
       <c r="V13" s="72"/>
       <c r="W13" s="72"/>
       <c r="X13" s="72"/>
@@ -4166,49 +4211,49 @@
       <c r="AD13" s="72"/>
       <c r="AE13" s="72"/>
       <c r="AF13" s="72"/>
-      <c r="AG13" s="152"/>
-      <c r="AH13" s="153"/>
-      <c r="AI13" s="153"/>
-      <c r="AJ13" s="154"/>
+      <c r="AG13" s="137"/>
+      <c r="AH13" s="138"/>
+      <c r="AI13" s="138"/>
+      <c r="AJ13" s="139"/>
       <c r="AK13" s="72"/>
-      <c r="AL13" s="113"/>
-      <c r="AM13" s="114"/>
-      <c r="AN13" s="115"/>
+      <c r="AL13" s="123"/>
+      <c r="AM13" s="124"/>
+      <c r="AN13" s="125"/>
       <c r="AO13" s="72"/>
-      <c r="AP13" s="113"/>
-      <c r="AQ13" s="114"/>
-      <c r="AR13" s="115"/>
+      <c r="AP13" s="123"/>
+      <c r="AQ13" s="124"/>
+      <c r="AR13" s="125"/>
       <c r="AS13" s="72"/>
-      <c r="AT13" s="113"/>
-      <c r="AU13" s="114"/>
-      <c r="AV13" s="115"/>
+      <c r="AT13" s="123"/>
+      <c r="AU13" s="124"/>
+      <c r="AV13" s="125"/>
       <c r="AW13" s="75"/>
-      <c r="AX13" s="113"/>
-      <c r="AY13" s="114"/>
-      <c r="AZ13" s="115"/>
+      <c r="AX13" s="123"/>
+      <c r="AY13" s="124"/>
+      <c r="AZ13" s="125"/>
       <c r="BA13" s="72"/>
       <c r="BB13" s="72"/>
       <c r="BC13" s="73"/>
     </row>
     <row r="14" spans="2:57">
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="127"/>
-      <c r="H14" s="129"/>
-      <c r="I14" s="129"/>
-      <c r="J14" s="129"/>
-      <c r="K14" s="129"/>
-      <c r="L14" s="129"/>
-      <c r="M14" s="129"/>
-      <c r="N14" s="129"/>
-      <c r="O14" s="129"/>
-      <c r="P14" s="129"/>
-      <c r="Q14" s="129"/>
-      <c r="R14" s="129"/>
-      <c r="S14" s="129"/>
-      <c r="T14" s="129"/>
-      <c r="U14" s="129"/>
+      <c r="D14" s="146"/>
+      <c r="E14" s="147"/>
+      <c r="F14" s="147"/>
+      <c r="G14" s="148"/>
+      <c r="H14" s="150"/>
+      <c r="I14" s="150"/>
+      <c r="J14" s="150"/>
+      <c r="K14" s="150"/>
+      <c r="L14" s="150"/>
+      <c r="M14" s="150"/>
+      <c r="N14" s="150"/>
+      <c r="O14" s="150"/>
+      <c r="P14" s="150"/>
+      <c r="Q14" s="150"/>
+      <c r="R14" s="150"/>
+      <c r="S14" s="150"/>
+      <c r="T14" s="150"/>
+      <c r="U14" s="150"/>
       <c r="V14" s="72"/>
       <c r="W14" s="72"/>
       <c r="X14" s="72"/>
@@ -4245,24 +4290,24 @@
       <c r="BC14" s="73"/>
     </row>
     <row r="15" spans="2:57">
-      <c r="D15" s="125"/>
-      <c r="E15" s="126"/>
-      <c r="F15" s="126"/>
-      <c r="G15" s="127"/>
-      <c r="H15" s="129"/>
-      <c r="I15" s="129"/>
-      <c r="J15" s="129"/>
-      <c r="K15" s="129"/>
-      <c r="L15" s="129"/>
-      <c r="M15" s="129"/>
-      <c r="N15" s="129"/>
-      <c r="O15" s="129"/>
-      <c r="P15" s="129"/>
-      <c r="Q15" s="129"/>
-      <c r="R15" s="129"/>
-      <c r="S15" s="129"/>
-      <c r="T15" s="129"/>
-      <c r="U15" s="129"/>
+      <c r="D15" s="146"/>
+      <c r="E15" s="147"/>
+      <c r="F15" s="147"/>
+      <c r="G15" s="148"/>
+      <c r="H15" s="150"/>
+      <c r="I15" s="150"/>
+      <c r="J15" s="150"/>
+      <c r="K15" s="150"/>
+      <c r="L15" s="150"/>
+      <c r="M15" s="150"/>
+      <c r="N15" s="150"/>
+      <c r="O15" s="150"/>
+      <c r="P15" s="150"/>
+      <c r="Q15" s="150"/>
+      <c r="R15" s="150"/>
+      <c r="S15" s="150"/>
+      <c r="T15" s="150"/>
+      <c r="U15" s="150"/>
       <c r="V15" s="72"/>
       <c r="W15" s="72"/>
       <c r="X15" s="72"/>
@@ -4521,19 +4566,19 @@
         <v>93</v>
       </c>
       <c r="G20" s="44"/>
-      <c r="H20" s="116"/>
-      <c r="I20" s="117"/>
-      <c r="J20" s="118"/>
+      <c r="H20" s="126"/>
+      <c r="I20" s="127"/>
+      <c r="J20" s="128"/>
       <c r="K20" s="44"/>
-      <c r="L20" s="116" t="s">
+      <c r="L20" s="126" t="s">
         <v>94</v>
       </c>
-      <c r="M20" s="118"/>
+      <c r="M20" s="128"/>
       <c r="N20" s="44"/>
-      <c r="O20" s="116" t="s">
+      <c r="O20" s="126" t="s">
         <v>95</v>
       </c>
-      <c r="P20" s="118"/>
+      <c r="P20" s="128"/>
       <c r="Q20" s="44"/>
       <c r="R20" s="44"/>
       <c r="S20" s="44"/>
@@ -4557,25 +4602,25 @@
       <c r="AK20" s="44"/>
       <c r="AL20" s="44"/>
       <c r="AM20" s="44"/>
-      <c r="AN20" s="116" t="s">
+      <c r="AN20" s="126" t="s">
         <v>96</v>
       </c>
-      <c r="AO20" s="117"/>
-      <c r="AP20" s="117"/>
-      <c r="AQ20" s="117"/>
-      <c r="AR20" s="118"/>
+      <c r="AO20" s="127"/>
+      <c r="AP20" s="127"/>
+      <c r="AQ20" s="127"/>
+      <c r="AR20" s="128"/>
       <c r="AS20" s="78" t="s">
         <v>85</v>
       </c>
       <c r="AT20" s="44"/>
       <c r="AU20" s="44"/>
-      <c r="AV20" s="116" t="s">
+      <c r="AV20" s="126" t="s">
         <v>97</v>
       </c>
-      <c r="AW20" s="117"/>
-      <c r="AX20" s="117"/>
-      <c r="AY20" s="117"/>
-      <c r="AZ20" s="118"/>
+      <c r="AW20" s="127"/>
+      <c r="AX20" s="127"/>
+      <c r="AY20" s="127"/>
+      <c r="AZ20" s="128"/>
       <c r="BA20" s="78" t="s">
         <v>85</v>
       </c>
@@ -4641,13 +4686,13 @@
       <c r="E22" s="60"/>
       <c r="F22" s="44"/>
       <c r="G22" s="44"/>
-      <c r="H22" s="137" t="s">
+      <c r="H22" s="151" t="s">
         <v>79</v>
       </c>
-      <c r="I22" s="137"/>
-      <c r="J22" s="137"/>
-      <c r="K22" s="137"/>
-      <c r="L22" s="137"/>
+      <c r="I22" s="151"/>
+      <c r="J22" s="151"/>
+      <c r="K22" s="151"/>
+      <c r="L22" s="151"/>
       <c r="M22" s="44"/>
       <c r="N22" s="44"/>
       <c r="O22" s="44"/>
@@ -4695,71 +4740,71 @@
     <row r="23" spans="4:55">
       <c r="D23" s="65"/>
       <c r="E23" s="60"/>
-      <c r="F23" s="138" t="s">
+      <c r="F23" s="161" t="s">
         <v>98</v>
       </c>
-      <c r="G23" s="133"/>
-      <c r="H23" s="140" t="s">
+      <c r="G23" s="142"/>
+      <c r="H23" s="163" t="s">
         <v>99</v>
       </c>
-      <c r="I23" s="141"/>
-      <c r="J23" s="134" t="s">
+      <c r="I23" s="164"/>
+      <c r="J23" s="143" t="s">
         <v>100</v>
       </c>
-      <c r="K23" s="135"/>
-      <c r="L23" s="135"/>
-      <c r="M23" s="135"/>
-      <c r="N23" s="135"/>
-      <c r="O23" s="135"/>
-      <c r="P23" s="136"/>
-      <c r="Q23" s="131" t="s">
+      <c r="K23" s="144"/>
+      <c r="L23" s="144"/>
+      <c r="M23" s="144"/>
+      <c r="N23" s="144"/>
+      <c r="O23" s="144"/>
+      <c r="P23" s="145"/>
+      <c r="Q23" s="140" t="s">
         <v>101</v>
       </c>
-      <c r="R23" s="132"/>
-      <c r="S23" s="132"/>
-      <c r="T23" s="132"/>
-      <c r="U23" s="132"/>
-      <c r="V23" s="132"/>
-      <c r="W23" s="133"/>
-      <c r="X23" s="131" t="s">
+      <c r="R23" s="141"/>
+      <c r="S23" s="141"/>
+      <c r="T23" s="141"/>
+      <c r="U23" s="141"/>
+      <c r="V23" s="141"/>
+      <c r="W23" s="142"/>
+      <c r="X23" s="140" t="s">
         <v>102</v>
       </c>
-      <c r="Y23" s="132"/>
-      <c r="Z23" s="132"/>
-      <c r="AA23" s="133"/>
-      <c r="AB23" s="131" t="s">
+      <c r="Y23" s="141"/>
+      <c r="Z23" s="141"/>
+      <c r="AA23" s="142"/>
+      <c r="AB23" s="140" t="s">
         <v>103</v>
       </c>
-      <c r="AC23" s="132"/>
-      <c r="AD23" s="132"/>
-      <c r="AE23" s="133"/>
-      <c r="AF23" s="131" t="s">
+      <c r="AC23" s="141"/>
+      <c r="AD23" s="141"/>
+      <c r="AE23" s="142"/>
+      <c r="AF23" s="140" t="s">
         <v>104</v>
       </c>
-      <c r="AG23" s="132"/>
-      <c r="AH23" s="132"/>
-      <c r="AI23" s="132"/>
-      <c r="AJ23" s="132"/>
-      <c r="AK23" s="132"/>
-      <c r="AL23" s="132"/>
+      <c r="AG23" s="141"/>
+      <c r="AH23" s="141"/>
+      <c r="AI23" s="141"/>
+      <c r="AJ23" s="141"/>
+      <c r="AK23" s="141"/>
+      <c r="AL23" s="141"/>
       <c r="AM23" s="79"/>
-      <c r="AN23" s="131" t="s">
+      <c r="AN23" s="140" t="s">
         <v>105</v>
       </c>
-      <c r="AO23" s="132"/>
-      <c r="AP23" s="132"/>
-      <c r="AQ23" s="132"/>
-      <c r="AR23" s="132"/>
-      <c r="AS23" s="132"/>
-      <c r="AT23" s="133"/>
-      <c r="AU23" s="131" t="s">
+      <c r="AO23" s="141"/>
+      <c r="AP23" s="141"/>
+      <c r="AQ23" s="141"/>
+      <c r="AR23" s="141"/>
+      <c r="AS23" s="141"/>
+      <c r="AT23" s="142"/>
+      <c r="AU23" s="140" t="s">
         <v>107</v>
       </c>
-      <c r="AV23" s="132"/>
-      <c r="AW23" s="132"/>
-      <c r="AX23" s="132"/>
-      <c r="AY23" s="132"/>
-      <c r="AZ23" s="133"/>
+      <c r="AV23" s="141"/>
+      <c r="AW23" s="141"/>
+      <c r="AX23" s="141"/>
+      <c r="AY23" s="141"/>
+      <c r="AZ23" s="142"/>
       <c r="BA23" s="155" t="s">
         <v>106</v>
       </c>
@@ -4769,53 +4814,53 @@
     <row r="24" spans="4:55">
       <c r="D24" s="65"/>
       <c r="E24" s="60"/>
-      <c r="F24" s="139"/>
-      <c r="G24" s="136"/>
-      <c r="H24" s="142"/>
-      <c r="I24" s="143"/>
-      <c r="J24" s="134"/>
-      <c r="K24" s="135"/>
-      <c r="L24" s="135"/>
-      <c r="M24" s="135"/>
-      <c r="N24" s="135"/>
-      <c r="O24" s="135"/>
-      <c r="P24" s="136"/>
-      <c r="Q24" s="134"/>
-      <c r="R24" s="135"/>
-      <c r="S24" s="135"/>
-      <c r="T24" s="135"/>
-      <c r="U24" s="135"/>
-      <c r="V24" s="135"/>
-      <c r="W24" s="136"/>
-      <c r="X24" s="134"/>
-      <c r="Y24" s="135"/>
-      <c r="Z24" s="135"/>
-      <c r="AA24" s="136"/>
-      <c r="AB24" s="134"/>
-      <c r="AC24" s="135"/>
-      <c r="AD24" s="135"/>
-      <c r="AE24" s="136"/>
-      <c r="AF24" s="134"/>
-      <c r="AG24" s="135"/>
-      <c r="AH24" s="135"/>
-      <c r="AI24" s="135"/>
-      <c r="AJ24" s="135"/>
-      <c r="AK24" s="135"/>
-      <c r="AL24" s="135"/>
+      <c r="F24" s="162"/>
+      <c r="G24" s="145"/>
+      <c r="H24" s="165"/>
+      <c r="I24" s="166"/>
+      <c r="J24" s="143"/>
+      <c r="K24" s="144"/>
+      <c r="L24" s="144"/>
+      <c r="M24" s="144"/>
+      <c r="N24" s="144"/>
+      <c r="O24" s="144"/>
+      <c r="P24" s="145"/>
+      <c r="Q24" s="143"/>
+      <c r="R24" s="144"/>
+      <c r="S24" s="144"/>
+      <c r="T24" s="144"/>
+      <c r="U24" s="144"/>
+      <c r="V24" s="144"/>
+      <c r="W24" s="145"/>
+      <c r="X24" s="143"/>
+      <c r="Y24" s="144"/>
+      <c r="Z24" s="144"/>
+      <c r="AA24" s="145"/>
+      <c r="AB24" s="143"/>
+      <c r="AC24" s="144"/>
+      <c r="AD24" s="144"/>
+      <c r="AE24" s="145"/>
+      <c r="AF24" s="143"/>
+      <c r="AG24" s="144"/>
+      <c r="AH24" s="144"/>
+      <c r="AI24" s="144"/>
+      <c r="AJ24" s="144"/>
+      <c r="AK24" s="144"/>
+      <c r="AL24" s="144"/>
       <c r="AM24" s="72"/>
-      <c r="AN24" s="134"/>
-      <c r="AO24" s="135"/>
-      <c r="AP24" s="135"/>
-      <c r="AQ24" s="135"/>
-      <c r="AR24" s="135"/>
-      <c r="AS24" s="135"/>
-      <c r="AT24" s="136"/>
-      <c r="AU24" s="134"/>
-      <c r="AV24" s="135"/>
-      <c r="AW24" s="135"/>
-      <c r="AX24" s="135"/>
-      <c r="AY24" s="135"/>
-      <c r="AZ24" s="136"/>
+      <c r="AN24" s="143"/>
+      <c r="AO24" s="144"/>
+      <c r="AP24" s="144"/>
+      <c r="AQ24" s="144"/>
+      <c r="AR24" s="144"/>
+      <c r="AS24" s="144"/>
+      <c r="AT24" s="145"/>
+      <c r="AU24" s="143"/>
+      <c r="AV24" s="144"/>
+      <c r="AW24" s="144"/>
+      <c r="AX24" s="144"/>
+      <c r="AY24" s="144"/>
+      <c r="AZ24" s="145"/>
       <c r="BA24" s="156"/>
       <c r="BB24" s="61"/>
       <c r="BC24" s="66"/>
@@ -5581,94 +5626,94 @@
       <c r="BC38" s="69"/>
     </row>
     <row r="41" spans="3:56">
-      <c r="C41" s="145" t="s">
+      <c r="C41" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="D41" s="145"/>
-      <c r="E41" s="145"/>
-      <c r="F41" s="145"/>
-      <c r="G41" s="145"/>
+      <c r="D41" s="133"/>
+      <c r="E41" s="133"/>
+      <c r="F41" s="133"/>
+      <c r="G41" s="133"/>
     </row>
     <row r="42" spans="3:56">
       <c r="C42" s="31"/>
     </row>
     <row r="43" spans="3:56" ht="15">
-      <c r="C43" s="119" t="s">
+      <c r="C43" s="129" t="s">
         <v>34</v>
       </c>
-      <c r="D43" s="120"/>
-      <c r="E43" s="120" t="s">
+      <c r="D43" s="130"/>
+      <c r="E43" s="130" t="s">
         <v>35</v>
       </c>
-      <c r="F43" s="120"/>
-      <c r="G43" s="120"/>
-      <c r="H43" s="120"/>
-      <c r="I43" s="120"/>
-      <c r="J43" s="120"/>
-      <c r="K43" s="120"/>
-      <c r="L43" s="120"/>
-      <c r="M43" s="120"/>
-      <c r="N43" s="120" t="s">
+      <c r="F43" s="130"/>
+      <c r="G43" s="130"/>
+      <c r="H43" s="130"/>
+      <c r="I43" s="130"/>
+      <c r="J43" s="130"/>
+      <c r="K43" s="130"/>
+      <c r="L43" s="130"/>
+      <c r="M43" s="130"/>
+      <c r="N43" s="130" t="s">
         <v>36</v>
       </c>
-      <c r="O43" s="120"/>
-      <c r="P43" s="120"/>
-      <c r="Q43" s="120"/>
-      <c r="R43" s="120" t="s">
+      <c r="O43" s="130"/>
+      <c r="P43" s="130"/>
+      <c r="Q43" s="130"/>
+      <c r="R43" s="130" t="s">
         <v>37</v>
       </c>
-      <c r="S43" s="120"/>
-      <c r="T43" s="120"/>
-      <c r="U43" s="120" t="s">
+      <c r="S43" s="130"/>
+      <c r="T43" s="130"/>
+      <c r="U43" s="130" t="s">
         <v>38</v>
       </c>
-      <c r="V43" s="120"/>
-      <c r="W43" s="120"/>
-      <c r="X43" s="120" t="s">
+      <c r="V43" s="130"/>
+      <c r="W43" s="130"/>
+      <c r="X43" s="130" t="s">
         <v>39</v>
       </c>
-      <c r="Y43" s="120"/>
-      <c r="Z43" s="120"/>
-      <c r="AA43" s="120"/>
-      <c r="AB43" s="120"/>
-      <c r="AC43" s="120"/>
-      <c r="AD43" s="120"/>
-      <c r="AE43" s="120" t="s">
+      <c r="Y43" s="130"/>
+      <c r="Z43" s="130"/>
+      <c r="AA43" s="130"/>
+      <c r="AB43" s="130"/>
+      <c r="AC43" s="130"/>
+      <c r="AD43" s="130"/>
+      <c r="AE43" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="AF43" s="120"/>
-      <c r="AG43" s="120"/>
-      <c r="AH43" s="120"/>
-      <c r="AI43" s="120"/>
-      <c r="AJ43" s="120" t="s">
+      <c r="AF43" s="130"/>
+      <c r="AG43" s="130"/>
+      <c r="AH43" s="130"/>
+      <c r="AI43" s="130"/>
+      <c r="AJ43" s="130" t="s">
         <v>41</v>
       </c>
-      <c r="AK43" s="120"/>
-      <c r="AL43" s="120"/>
-      <c r="AM43" s="120"/>
-      <c r="AN43" s="120" t="s">
+      <c r="AK43" s="130"/>
+      <c r="AL43" s="130"/>
+      <c r="AM43" s="130"/>
+      <c r="AN43" s="130" t="s">
         <v>42</v>
       </c>
-      <c r="AO43" s="120"/>
-      <c r="AP43" s="120"/>
-      <c r="AQ43" s="120" t="s">
+      <c r="AO43" s="130"/>
+      <c r="AP43" s="130"/>
+      <c r="AQ43" s="130" t="s">
         <v>43</v>
       </c>
-      <c r="AR43" s="120"/>
-      <c r="AS43" s="120"/>
-      <c r="AT43" s="120"/>
-      <c r="AU43" s="120"/>
-      <c r="AV43" s="120"/>
-      <c r="AW43" s="120" t="s">
+      <c r="AR43" s="130"/>
+      <c r="AS43" s="130"/>
+      <c r="AT43" s="130"/>
+      <c r="AU43" s="130"/>
+      <c r="AV43" s="130"/>
+      <c r="AW43" s="130" t="s">
         <v>44</v>
       </c>
-      <c r="AX43" s="120"/>
-      <c r="AY43" s="120"/>
-      <c r="AZ43" s="120"/>
-      <c r="BA43" s="120"/>
-      <c r="BB43" s="120"/>
-      <c r="BC43" s="120"/>
-      <c r="BD43" s="130"/>
+      <c r="AX43" s="130"/>
+      <c r="AY43" s="130"/>
+      <c r="AZ43" s="130"/>
+      <c r="BA43" s="130"/>
+      <c r="BB43" s="130"/>
+      <c r="BC43" s="130"/>
+      <c r="BD43" s="160"/>
     </row>
     <row r="44" spans="3:56">
       <c r="C44" s="33"/>
@@ -5879,14 +5924,14 @@
         <v>53</v>
       </c>
       <c r="AP46" s="38"/>
-      <c r="AQ46" s="122" t="s">
+      <c r="AQ46" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="AR46" s="123"/>
-      <c r="AS46" s="123"/>
-      <c r="AT46" s="123"/>
-      <c r="AU46" s="123"/>
-      <c r="AV46" s="124"/>
+      <c r="AR46" s="115"/>
+      <c r="AS46" s="115"/>
+      <c r="AT46" s="115"/>
+      <c r="AU46" s="115"/>
+      <c r="AV46" s="116"/>
       <c r="AW46" s="39" t="s">
         <v>58</v>
       </c>
@@ -7215,104 +7260,104 @@
       <c r="BD66" s="44"/>
     </row>
     <row r="67" spans="3:56">
-      <c r="C67" s="145" t="s">
+      <c r="C67" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="D67" s="145"/>
-      <c r="E67" s="145"/>
-      <c r="F67" s="145"/>
-      <c r="G67" s="145"/>
-      <c r="H67" s="145"/>
-      <c r="I67" s="145"/>
-      <c r="J67" s="145"/>
+      <c r="D67" s="133"/>
+      <c r="E67" s="133"/>
+      <c r="F67" s="133"/>
+      <c r="G67" s="133"/>
+      <c r="H67" s="133"/>
+      <c r="I67" s="133"/>
+      <c r="J67" s="133"/>
     </row>
     <row r="68" spans="3:56">
       <c r="C68" s="31"/>
     </row>
     <row r="69" spans="3:56" ht="15">
-      <c r="C69" s="102" t="s">
+      <c r="C69" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="D69" s="103"/>
-      <c r="E69" s="103" t="s">
+      <c r="D69" s="102"/>
+      <c r="E69" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="F69" s="103"/>
-      <c r="G69" s="103"/>
-      <c r="H69" s="103"/>
-      <c r="I69" s="103"/>
-      <c r="J69" s="103"/>
-      <c r="K69" s="103"/>
-      <c r="L69" s="103"/>
-      <c r="M69" s="103"/>
-      <c r="N69" s="103"/>
-      <c r="O69" s="103"/>
-      <c r="P69" s="103"/>
-      <c r="Q69" s="103"/>
-      <c r="R69" s="103" t="s">
+      <c r="F69" s="102"/>
+      <c r="G69" s="102"/>
+      <c r="H69" s="102"/>
+      <c r="I69" s="102"/>
+      <c r="J69" s="102"/>
+      <c r="K69" s="102"/>
+      <c r="L69" s="102"/>
+      <c r="M69" s="102"/>
+      <c r="N69" s="102"/>
+      <c r="O69" s="102"/>
+      <c r="P69" s="102"/>
+      <c r="Q69" s="102"/>
+      <c r="R69" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="S69" s="103"/>
-      <c r="T69" s="103"/>
-      <c r="U69" s="103"/>
-      <c r="V69" s="103"/>
-      <c r="W69" s="103"/>
-      <c r="X69" s="103" t="s">
+      <c r="S69" s="102"/>
+      <c r="T69" s="102"/>
+      <c r="U69" s="102"/>
+      <c r="V69" s="102"/>
+      <c r="W69" s="102"/>
+      <c r="X69" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="Y69" s="103"/>
-      <c r="Z69" s="103"/>
-      <c r="AA69" s="103"/>
-      <c r="AB69" s="103"/>
-      <c r="AC69" s="103"/>
-      <c r="AD69" s="103"/>
-      <c r="AE69" s="103" t="s">
+      <c r="Y69" s="102"/>
+      <c r="Z69" s="102"/>
+      <c r="AA69" s="102"/>
+      <c r="AB69" s="102"/>
+      <c r="AC69" s="102"/>
+      <c r="AD69" s="102"/>
+      <c r="AE69" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="AF69" s="103"/>
-      <c r="AG69" s="103"/>
-      <c r="AH69" s="103"/>
-      <c r="AI69" s="103"/>
-      <c r="AJ69" s="103"/>
-      <c r="AK69" s="103"/>
-      <c r="AL69" s="103" t="s">
+      <c r="AF69" s="102"/>
+      <c r="AG69" s="102"/>
+      <c r="AH69" s="102"/>
+      <c r="AI69" s="102"/>
+      <c r="AJ69" s="102"/>
+      <c r="AK69" s="102"/>
+      <c r="AL69" s="102" t="s">
         <v>44</v>
       </c>
-      <c r="AM69" s="103"/>
-      <c r="AN69" s="103"/>
-      <c r="AO69" s="103"/>
-      <c r="AP69" s="103"/>
-      <c r="AQ69" s="103"/>
-      <c r="AR69" s="103"/>
-      <c r="AS69" s="103"/>
-      <c r="AT69" s="103"/>
-      <c r="AU69" s="103"/>
-      <c r="AV69" s="103"/>
-      <c r="AW69" s="103"/>
-      <c r="AX69" s="103"/>
-      <c r="AY69" s="103"/>
-      <c r="AZ69" s="103"/>
-      <c r="BA69" s="103"/>
-      <c r="BB69" s="103"/>
-      <c r="BC69" s="103"/>
-      <c r="BD69" s="121"/>
+      <c r="AM69" s="102"/>
+      <c r="AN69" s="102"/>
+      <c r="AO69" s="102"/>
+      <c r="AP69" s="102"/>
+      <c r="AQ69" s="102"/>
+      <c r="AR69" s="102"/>
+      <c r="AS69" s="102"/>
+      <c r="AT69" s="102"/>
+      <c r="AU69" s="102"/>
+      <c r="AV69" s="102"/>
+      <c r="AW69" s="102"/>
+      <c r="AX69" s="102"/>
+      <c r="AY69" s="102"/>
+      <c r="AZ69" s="102"/>
+      <c r="BA69" s="102"/>
+      <c r="BB69" s="102"/>
+      <c r="BC69" s="102"/>
+      <c r="BD69" s="131"/>
     </row>
     <row r="70" spans="3:56" ht="15" customHeight="1">
       <c r="C70" s="45"/>
       <c r="D70" s="37"/>
-      <c r="E70" s="104"/>
-      <c r="F70" s="105"/>
-      <c r="G70" s="105"/>
-      <c r="H70" s="105"/>
-      <c r="I70" s="105"/>
-      <c r="J70" s="105"/>
-      <c r="K70" s="105"/>
-      <c r="L70" s="105"/>
-      <c r="M70" s="105"/>
-      <c r="N70" s="105"/>
-      <c r="O70" s="105"/>
-      <c r="P70" s="105"/>
-      <c r="Q70" s="106"/>
+      <c r="E70" s="103"/>
+      <c r="F70" s="104"/>
+      <c r="G70" s="104"/>
+      <c r="H70" s="104"/>
+      <c r="I70" s="104"/>
+      <c r="J70" s="104"/>
+      <c r="K70" s="104"/>
+      <c r="L70" s="104"/>
+      <c r="M70" s="104"/>
+      <c r="N70" s="104"/>
+      <c r="O70" s="104"/>
+      <c r="P70" s="104"/>
+      <c r="Q70" s="105"/>
       <c r="R70" s="34"/>
       <c r="S70" s="34"/>
       <c r="T70" s="34"/>
@@ -7326,13 +7371,13 @@
       <c r="AB70" s="158"/>
       <c r="AC70" s="158"/>
       <c r="AD70" s="159"/>
-      <c r="AE70" s="104"/>
-      <c r="AF70" s="105"/>
-      <c r="AG70" s="105"/>
-      <c r="AH70" s="105"/>
-      <c r="AI70" s="105"/>
-      <c r="AJ70" s="105"/>
-      <c r="AK70" s="106"/>
+      <c r="AE70" s="103"/>
+      <c r="AF70" s="104"/>
+      <c r="AG70" s="104"/>
+      <c r="AH70" s="104"/>
+      <c r="AI70" s="104"/>
+      <c r="AJ70" s="104"/>
+      <c r="AK70" s="105"/>
       <c r="AL70" s="34"/>
       <c r="AM70" s="34"/>
       <c r="AN70" s="34"/>
@@ -7358,45 +7403,45 @@
       <c r="D71" s="40">
         <v>1</v>
       </c>
-      <c r="E71" s="107" t="s">
+      <c r="E71" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="F71" s="108"/>
-      <c r="G71" s="108"/>
-      <c r="H71" s="108"/>
-      <c r="I71" s="108"/>
-      <c r="J71" s="108"/>
-      <c r="K71" s="108"/>
-      <c r="L71" s="108"/>
-      <c r="M71" s="108"/>
-      <c r="N71" s="108"/>
-      <c r="O71" s="108"/>
-      <c r="P71" s="108"/>
-      <c r="Q71" s="109"/>
+      <c r="F71" s="107"/>
+      <c r="G71" s="107"/>
+      <c r="H71" s="107"/>
+      <c r="I71" s="107"/>
+      <c r="J71" s="107"/>
+      <c r="K71" s="107"/>
+      <c r="L71" s="107"/>
+      <c r="M71" s="107"/>
+      <c r="N71" s="107"/>
+      <c r="O71" s="107"/>
+      <c r="P71" s="107"/>
+      <c r="Q71" s="108"/>
       <c r="R71" s="38"/>
       <c r="S71" s="38"/>
       <c r="T71" s="38"/>
       <c r="U71" s="38"/>
       <c r="V71" s="38"/>
       <c r="W71" s="40"/>
-      <c r="X71" s="122" t="s">
+      <c r="X71" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="Y71" s="123"/>
-      <c r="Z71" s="123"/>
-      <c r="AA71" s="123"/>
-      <c r="AB71" s="123"/>
-      <c r="AC71" s="123"/>
-      <c r="AD71" s="124"/>
-      <c r="AE71" s="107" t="s">
+      <c r="Y71" s="115"/>
+      <c r="Z71" s="115"/>
+      <c r="AA71" s="115"/>
+      <c r="AB71" s="115"/>
+      <c r="AC71" s="115"/>
+      <c r="AD71" s="116"/>
+      <c r="AE71" s="106" t="s">
         <v>104</v>
       </c>
-      <c r="AF71" s="108"/>
-      <c r="AG71" s="108"/>
-      <c r="AH71" s="108"/>
-      <c r="AI71" s="108"/>
-      <c r="AJ71" s="108"/>
-      <c r="AK71" s="109"/>
+      <c r="AF71" s="107"/>
+      <c r="AG71" s="107"/>
+      <c r="AH71" s="107"/>
+      <c r="AI71" s="107"/>
+      <c r="AJ71" s="107"/>
+      <c r="AK71" s="108"/>
       <c r="AL71" s="38"/>
       <c r="AM71" s="38"/>
       <c r="AN71" s="38"/>
@@ -7422,45 +7467,45 @@
       <c r="D72" s="40">
         <v>2</v>
       </c>
-      <c r="E72" s="107" t="s">
+      <c r="E72" s="106" t="s">
         <v>111</v>
       </c>
-      <c r="F72" s="108"/>
-      <c r="G72" s="108"/>
-      <c r="H72" s="108"/>
-      <c r="I72" s="108"/>
-      <c r="J72" s="108"/>
-      <c r="K72" s="108"/>
-      <c r="L72" s="108"/>
-      <c r="M72" s="108"/>
-      <c r="N72" s="108"/>
-      <c r="O72" s="108"/>
-      <c r="P72" s="108"/>
-      <c r="Q72" s="109"/>
+      <c r="F72" s="107"/>
+      <c r="G72" s="107"/>
+      <c r="H72" s="107"/>
+      <c r="I72" s="107"/>
+      <c r="J72" s="107"/>
+      <c r="K72" s="107"/>
+      <c r="L72" s="107"/>
+      <c r="M72" s="107"/>
+      <c r="N72" s="107"/>
+      <c r="O72" s="107"/>
+      <c r="P72" s="107"/>
+      <c r="Q72" s="108"/>
       <c r="R72" s="38"/>
       <c r="S72" s="38"/>
       <c r="T72" s="38"/>
       <c r="U72" s="38"/>
       <c r="V72" s="38"/>
       <c r="W72" s="40"/>
-      <c r="X72" s="122" t="s">
+      <c r="X72" s="114" t="s">
         <v>109</v>
       </c>
-      <c r="Y72" s="123"/>
-      <c r="Z72" s="123"/>
-      <c r="AA72" s="123"/>
-      <c r="AB72" s="123"/>
-      <c r="AC72" s="123"/>
-      <c r="AD72" s="124"/>
-      <c r="AE72" s="107" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF72" s="108"/>
-      <c r="AG72" s="108"/>
-      <c r="AH72" s="108"/>
-      <c r="AI72" s="108"/>
-      <c r="AJ72" s="108"/>
-      <c r="AK72" s="109"/>
+      <c r="Y72" s="115"/>
+      <c r="Z72" s="115"/>
+      <c r="AA72" s="115"/>
+      <c r="AB72" s="115"/>
+      <c r="AC72" s="115"/>
+      <c r="AD72" s="116"/>
+      <c r="AE72" s="106" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF72" s="107"/>
+      <c r="AG72" s="107"/>
+      <c r="AH72" s="107"/>
+      <c r="AI72" s="107"/>
+      <c r="AJ72" s="107"/>
+      <c r="AK72" s="108"/>
       <c r="AL72" s="38"/>
       <c r="AM72" s="38"/>
       <c r="AN72" s="38"/>
@@ -7481,42 +7526,50 @@
       <c r="BC72" s="38"/>
       <c r="BD72" s="40"/>
     </row>
-    <row r="73" spans="3:56">
+    <row r="73" spans="3:56" ht="15" customHeight="1">
       <c r="C73" s="86"/>
-      <c r="D73" s="53"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="50"/>
-      <c r="H73" s="50"/>
-      <c r="I73" s="50"/>
-      <c r="J73" s="50"/>
-      <c r="K73" s="50"/>
-      <c r="L73" s="50"/>
-      <c r="M73" s="50"/>
-      <c r="N73" s="50"/>
-      <c r="O73" s="50"/>
-      <c r="P73" s="50"/>
-      <c r="Q73" s="53"/>
+      <c r="D73" s="53">
+        <v>3</v>
+      </c>
+      <c r="E73" s="109" t="s">
+        <v>129</v>
+      </c>
+      <c r="F73" s="110"/>
+      <c r="G73" s="110"/>
+      <c r="H73" s="110"/>
+      <c r="I73" s="110"/>
+      <c r="J73" s="110"/>
+      <c r="K73" s="110"/>
+      <c r="L73" s="110"/>
+      <c r="M73" s="110"/>
+      <c r="N73" s="110"/>
+      <c r="O73" s="110"/>
+      <c r="P73" s="110"/>
+      <c r="Q73" s="111"/>
       <c r="R73" s="50"/>
       <c r="S73" s="50"/>
       <c r="T73" s="50"/>
       <c r="U73" s="50"/>
       <c r="V73" s="50"/>
       <c r="W73" s="53"/>
-      <c r="X73" s="50"/>
-      <c r="Y73" s="50"/>
-      <c r="Z73" s="50"/>
-      <c r="AA73" s="50"/>
-      <c r="AB73" s="50"/>
-      <c r="AC73" s="50"/>
-      <c r="AD73" s="53"/>
-      <c r="AE73" s="50"/>
-      <c r="AF73" s="50"/>
-      <c r="AG73" s="50"/>
-      <c r="AH73" s="50"/>
-      <c r="AI73" s="50"/>
-      <c r="AJ73" s="50"/>
-      <c r="AK73" s="53"/>
+      <c r="X73" s="170" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y73" s="171"/>
+      <c r="Z73" s="171"/>
+      <c r="AA73" s="171"/>
+      <c r="AB73" s="171"/>
+      <c r="AC73" s="171"/>
+      <c r="AD73" s="172"/>
+      <c r="AE73" s="109" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF73" s="110"/>
+      <c r="AG73" s="110"/>
+      <c r="AH73" s="110"/>
+      <c r="AI73" s="110"/>
+      <c r="AJ73" s="110"/>
+      <c r="AK73" s="111"/>
       <c r="AL73" s="50"/>
       <c r="AM73" s="50"/>
       <c r="AN73" s="50"/>
@@ -7537,120 +7590,128 @@
       <c r="BC73" s="50"/>
       <c r="BD73" s="53"/>
     </row>
-    <row r="74" spans="3:56">
-      <c r="C74" s="87"/>
-      <c r="D74" s="54"/>
-      <c r="E74" s="54"/>
-      <c r="F74" s="54"/>
-      <c r="G74" s="54"/>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
-      <c r="J74" s="54"/>
-      <c r="K74" s="54"/>
-      <c r="L74" s="54"/>
-      <c r="M74" s="54"/>
-      <c r="N74" s="54"/>
-      <c r="O74" s="54"/>
-      <c r="P74" s="54"/>
-      <c r="Q74" s="54"/>
-      <c r="R74" s="54"/>
-      <c r="S74" s="54"/>
-      <c r="T74" s="54"/>
-      <c r="U74" s="54"/>
-      <c r="V74" s="54"/>
-      <c r="W74" s="54"/>
-      <c r="X74" s="54"/>
-      <c r="Y74" s="54"/>
-      <c r="Z74" s="54"/>
-      <c r="AA74" s="54"/>
-      <c r="AB74" s="54"/>
-      <c r="AC74" s="54"/>
-      <c r="AD74" s="54"/>
-      <c r="AE74" s="54"/>
-      <c r="AF74" s="54"/>
-      <c r="AG74" s="54"/>
-      <c r="AH74" s="54"/>
-      <c r="AI74" s="54"/>
-      <c r="AJ74" s="54"/>
-      <c r="AK74" s="54"/>
-      <c r="AL74" s="54"/>
-      <c r="AM74" s="54"/>
-      <c r="AN74" s="54"/>
-      <c r="AO74" s="54"/>
-      <c r="AP74" s="54"/>
-      <c r="AQ74" s="54"/>
-      <c r="AR74" s="54"/>
-      <c r="AS74" s="54"/>
-      <c r="AT74" s="54"/>
-      <c r="AU74" s="54"/>
-      <c r="AV74" s="54"/>
-      <c r="AW74" s="54"/>
-      <c r="AX74" s="54"/>
-      <c r="AY74" s="54"/>
-      <c r="AZ74" s="54"/>
-      <c r="BA74" s="54"/>
-      <c r="BB74" s="54"/>
-      <c r="BC74" s="54"/>
-      <c r="BD74" s="54"/>
-    </row>
-    <row r="75" spans="3:56">
-      <c r="C75" s="88"/>
-      <c r="D75" s="44"/>
-      <c r="E75" s="44"/>
-      <c r="F75" s="44"/>
-      <c r="G75" s="44"/>
-      <c r="H75" s="44"/>
-      <c r="I75" s="44"/>
-      <c r="J75" s="44"/>
-      <c r="K75" s="44"/>
-      <c r="L75" s="44"/>
-      <c r="M75" s="44"/>
-      <c r="N75" s="44"/>
-      <c r="O75" s="44"/>
-      <c r="P75" s="44"/>
-      <c r="Q75" s="44"/>
-      <c r="R75" s="44"/>
-      <c r="S75" s="44"/>
-      <c r="T75" s="44"/>
-      <c r="U75" s="44"/>
-      <c r="V75" s="44"/>
-      <c r="W75" s="44"/>
-      <c r="X75" s="44"/>
-      <c r="Y75" s="44"/>
-      <c r="Z75" s="44"/>
-      <c r="AA75" s="44"/>
-      <c r="AB75" s="44"/>
-      <c r="AC75" s="44"/>
-      <c r="AD75" s="44"/>
-      <c r="AE75" s="44"/>
-      <c r="AF75" s="44"/>
-      <c r="AG75" s="44"/>
-      <c r="AH75" s="44"/>
-      <c r="AI75" s="44"/>
-      <c r="AJ75" s="44"/>
-      <c r="AK75" s="44"/>
-      <c r="AL75" s="44"/>
-      <c r="AM75" s="44"/>
-      <c r="AN75" s="44"/>
-      <c r="AO75" s="44"/>
-      <c r="AP75" s="44"/>
-      <c r="AQ75" s="44"/>
-      <c r="AR75" s="44"/>
-      <c r="AS75" s="44"/>
-      <c r="AT75" s="44"/>
-      <c r="AU75" s="44"/>
-      <c r="AV75" s="44"/>
-      <c r="AW75" s="44"/>
-      <c r="AX75" s="44"/>
-      <c r="AY75" s="44"/>
-      <c r="AZ75" s="44"/>
-      <c r="BA75" s="44"/>
-      <c r="BB75" s="44"/>
-      <c r="BC75" s="44"/>
-      <c r="BD75" s="44"/>
+    <row r="74" spans="3:56" ht="15" customHeight="1">
+      <c r="C74" s="173">
+        <v>4</v>
+      </c>
+      <c r="D74" s="174"/>
+      <c r="E74" s="106" t="s">
+        <v>131</v>
+      </c>
+      <c r="F74" s="107"/>
+      <c r="G74" s="107"/>
+      <c r="H74" s="107"/>
+      <c r="I74" s="107"/>
+      <c r="J74" s="107"/>
+      <c r="K74" s="107"/>
+      <c r="L74" s="107"/>
+      <c r="M74" s="107"/>
+      <c r="N74" s="107"/>
+      <c r="O74" s="107"/>
+      <c r="P74" s="107"/>
+      <c r="Q74" s="108"/>
+      <c r="R74" s="114"/>
+      <c r="S74" s="115"/>
+      <c r="T74" s="115"/>
+      <c r="U74" s="115"/>
+      <c r="V74" s="115"/>
+      <c r="W74" s="116"/>
+      <c r="X74" s="114" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y74" s="115"/>
+      <c r="Z74" s="115"/>
+      <c r="AA74" s="115"/>
+      <c r="AB74" s="115"/>
+      <c r="AC74" s="115"/>
+      <c r="AD74" s="116"/>
+      <c r="AE74" s="167" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF74" s="168"/>
+      <c r="AG74" s="168"/>
+      <c r="AH74" s="168"/>
+      <c r="AI74" s="168"/>
+      <c r="AJ74" s="168"/>
+      <c r="AK74" s="169"/>
+      <c r="AL74" s="114"/>
+      <c r="AM74" s="115"/>
+      <c r="AN74" s="115"/>
+      <c r="AO74" s="115"/>
+      <c r="AP74" s="115"/>
+      <c r="AQ74" s="115"/>
+      <c r="AR74" s="115"/>
+      <c r="AS74" s="115"/>
+      <c r="AT74" s="115"/>
+      <c r="AU74" s="115"/>
+      <c r="AV74" s="115"/>
+      <c r="AW74" s="115"/>
+      <c r="AX74" s="115"/>
+      <c r="AY74" s="115"/>
+      <c r="AZ74" s="115"/>
+      <c r="BA74" s="115"/>
+      <c r="BB74" s="115"/>
+      <c r="BC74" s="115"/>
+      <c r="BD74" s="116"/>
+    </row>
+    <row r="75" spans="3:56" ht="15" customHeight="1">
+      <c r="C75" s="112"/>
+      <c r="D75" s="113"/>
+      <c r="E75" s="117"/>
+      <c r="F75" s="118"/>
+      <c r="G75" s="118"/>
+      <c r="H75" s="118"/>
+      <c r="I75" s="118"/>
+      <c r="J75" s="118"/>
+      <c r="K75" s="118"/>
+      <c r="L75" s="118"/>
+      <c r="M75" s="118"/>
+      <c r="N75" s="118"/>
+      <c r="O75" s="118"/>
+      <c r="P75" s="118"/>
+      <c r="Q75" s="119"/>
+      <c r="R75" s="117"/>
+      <c r="S75" s="118"/>
+      <c r="T75" s="118"/>
+      <c r="U75" s="118"/>
+      <c r="V75" s="118"/>
+      <c r="W75" s="119"/>
+      <c r="X75" s="117"/>
+      <c r="Y75" s="118"/>
+      <c r="Z75" s="118"/>
+      <c r="AA75" s="118"/>
+      <c r="AB75" s="118"/>
+      <c r="AC75" s="118"/>
+      <c r="AD75" s="119"/>
+      <c r="AE75" s="117"/>
+      <c r="AF75" s="118"/>
+      <c r="AG75" s="118"/>
+      <c r="AH75" s="118"/>
+      <c r="AI75" s="118"/>
+      <c r="AJ75" s="118"/>
+      <c r="AK75" s="119"/>
+      <c r="AL75" s="117"/>
+      <c r="AM75" s="118"/>
+      <c r="AN75" s="118"/>
+      <c r="AO75" s="118"/>
+      <c r="AP75" s="118"/>
+      <c r="AQ75" s="118"/>
+      <c r="AR75" s="118"/>
+      <c r="AS75" s="118"/>
+      <c r="AT75" s="118"/>
+      <c r="AU75" s="118"/>
+      <c r="AV75" s="118"/>
+      <c r="AW75" s="118"/>
+      <c r="AX75" s="118"/>
+      <c r="AY75" s="118"/>
+      <c r="AZ75" s="118"/>
+      <c r="BA75" s="118"/>
+      <c r="BB75" s="118"/>
+      <c r="BC75" s="118"/>
+      <c r="BD75" s="119"/>
     </row>
     <row r="76" spans="3:56">
-      <c r="C76" s="88"/>
+      <c r="C76" s="87"/>
       <c r="D76" s="44"/>
       <c r="E76" s="44"/>
       <c r="F76" s="44"/>
@@ -8159,68 +8220,68 @@
       </c>
     </row>
     <row r="88" spans="3:56" ht="15">
-      <c r="C88" s="102" t="s">
+      <c r="C88" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="D88" s="103"/>
-      <c r="E88" s="103" t="s">
+      <c r="D88" s="102"/>
+      <c r="E88" s="102" t="s">
         <v>47</v>
       </c>
-      <c r="F88" s="103"/>
-      <c r="G88" s="103"/>
-      <c r="H88" s="103"/>
-      <c r="I88" s="103"/>
-      <c r="J88" s="103"/>
-      <c r="K88" s="103"/>
-      <c r="L88" s="103"/>
-      <c r="M88" s="103"/>
-      <c r="N88" s="103"/>
-      <c r="O88" s="103"/>
-      <c r="P88" s="103"/>
-      <c r="Q88" s="103"/>
-      <c r="R88" s="103" t="s">
+      <c r="F88" s="102"/>
+      <c r="G88" s="102"/>
+      <c r="H88" s="102"/>
+      <c r="I88" s="102"/>
+      <c r="J88" s="102"/>
+      <c r="K88" s="102"/>
+      <c r="L88" s="102"/>
+      <c r="M88" s="102"/>
+      <c r="N88" s="102"/>
+      <c r="O88" s="102"/>
+      <c r="P88" s="102"/>
+      <c r="Q88" s="102"/>
+      <c r="R88" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="S88" s="103"/>
-      <c r="T88" s="103"/>
-      <c r="U88" s="103"/>
-      <c r="V88" s="103"/>
-      <c r="W88" s="103"/>
-      <c r="X88" s="103" t="s">
+      <c r="S88" s="102"/>
+      <c r="T88" s="102"/>
+      <c r="U88" s="102"/>
+      <c r="V88" s="102"/>
+      <c r="W88" s="102"/>
+      <c r="X88" s="102" t="s">
         <v>49</v>
       </c>
-      <c r="Y88" s="103"/>
-      <c r="Z88" s="103"/>
-      <c r="AA88" s="103"/>
-      <c r="AB88" s="103"/>
-      <c r="AC88" s="103"/>
-      <c r="AD88" s="103"/>
-      <c r="AE88" s="103"/>
-      <c r="AF88" s="103"/>
-      <c r="AG88" s="103"/>
-      <c r="AH88" s="103"/>
-      <c r="AI88" s="103"/>
-      <c r="AJ88" s="103"/>
-      <c r="AK88" s="103"/>
-      <c r="AL88" s="103"/>
-      <c r="AM88" s="103"/>
-      <c r="AN88" s="103"/>
-      <c r="AO88" s="103"/>
-      <c r="AP88" s="103"/>
-      <c r="AQ88" s="103"/>
-      <c r="AR88" s="103"/>
-      <c r="AS88" s="103"/>
-      <c r="AT88" s="103"/>
-      <c r="AU88" s="103"/>
-      <c r="AV88" s="103"/>
-      <c r="AW88" s="103"/>
-      <c r="AX88" s="103"/>
-      <c r="AY88" s="103"/>
-      <c r="AZ88" s="103"/>
-      <c r="BA88" s="103"/>
-      <c r="BB88" s="103"/>
-      <c r="BC88" s="103"/>
-      <c r="BD88" s="121"/>
+      <c r="Y88" s="102"/>
+      <c r="Z88" s="102"/>
+      <c r="AA88" s="102"/>
+      <c r="AB88" s="102"/>
+      <c r="AC88" s="102"/>
+      <c r="AD88" s="102"/>
+      <c r="AE88" s="102"/>
+      <c r="AF88" s="102"/>
+      <c r="AG88" s="102"/>
+      <c r="AH88" s="102"/>
+      <c r="AI88" s="102"/>
+      <c r="AJ88" s="102"/>
+      <c r="AK88" s="102"/>
+      <c r="AL88" s="102"/>
+      <c r="AM88" s="102"/>
+      <c r="AN88" s="102"/>
+      <c r="AO88" s="102"/>
+      <c r="AP88" s="102"/>
+      <c r="AQ88" s="102"/>
+      <c r="AR88" s="102"/>
+      <c r="AS88" s="102"/>
+      <c r="AT88" s="102"/>
+      <c r="AU88" s="102"/>
+      <c r="AV88" s="102"/>
+      <c r="AW88" s="102"/>
+      <c r="AX88" s="102"/>
+      <c r="AY88" s="102"/>
+      <c r="AZ88" s="102"/>
+      <c r="BA88" s="102"/>
+      <c r="BB88" s="102"/>
+      <c r="BC88" s="102"/>
+      <c r="BD88" s="131"/>
     </row>
     <row r="89" spans="3:56" ht="15" customHeight="1">
       <c r="C89" s="33"/>
@@ -8245,46 +8306,46 @@
       <c r="R89" s="34"/>
       <c r="S89" s="34"/>
       <c r="T89" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U89" s="34"/>
       <c r="V89" s="34"/>
       <c r="W89" s="37"/>
-      <c r="X89" s="104" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y89" s="105"/>
-      <c r="Z89" s="105"/>
-      <c r="AA89" s="105"/>
-      <c r="AB89" s="105"/>
-      <c r="AC89" s="105"/>
-      <c r="AD89" s="105"/>
-      <c r="AE89" s="105"/>
-      <c r="AF89" s="105"/>
-      <c r="AG89" s="105"/>
-      <c r="AH89" s="105"/>
-      <c r="AI89" s="105"/>
-      <c r="AJ89" s="105"/>
-      <c r="AK89" s="105"/>
-      <c r="AL89" s="105"/>
-      <c r="AM89" s="105"/>
-      <c r="AN89" s="105"/>
-      <c r="AO89" s="105"/>
-      <c r="AP89" s="105"/>
-      <c r="AQ89" s="105"/>
-      <c r="AR89" s="105"/>
-      <c r="AS89" s="105"/>
-      <c r="AT89" s="105"/>
-      <c r="AU89" s="105"/>
-      <c r="AV89" s="105"/>
-      <c r="AW89" s="105"/>
-      <c r="AX89" s="105"/>
-      <c r="AY89" s="105"/>
-      <c r="AZ89" s="105"/>
-      <c r="BA89" s="105"/>
-      <c r="BB89" s="105"/>
-      <c r="BC89" s="105"/>
-      <c r="BD89" s="106"/>
+      <c r="X89" s="103" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y89" s="104"/>
+      <c r="Z89" s="104"/>
+      <c r="AA89" s="104"/>
+      <c r="AB89" s="104"/>
+      <c r="AC89" s="104"/>
+      <c r="AD89" s="104"/>
+      <c r="AE89" s="104"/>
+      <c r="AF89" s="104"/>
+      <c r="AG89" s="104"/>
+      <c r="AH89" s="104"/>
+      <c r="AI89" s="104"/>
+      <c r="AJ89" s="104"/>
+      <c r="AK89" s="104"/>
+      <c r="AL89" s="104"/>
+      <c r="AM89" s="104"/>
+      <c r="AN89" s="104"/>
+      <c r="AO89" s="104"/>
+      <c r="AP89" s="104"/>
+      <c r="AQ89" s="104"/>
+      <c r="AR89" s="104"/>
+      <c r="AS89" s="104"/>
+      <c r="AT89" s="104"/>
+      <c r="AU89" s="104"/>
+      <c r="AV89" s="104"/>
+      <c r="AW89" s="104"/>
+      <c r="AX89" s="104"/>
+      <c r="AY89" s="104"/>
+      <c r="AZ89" s="104"/>
+      <c r="BA89" s="104"/>
+      <c r="BB89" s="104"/>
+      <c r="BC89" s="104"/>
+      <c r="BD89" s="105"/>
     </row>
     <row r="90" spans="3:56" ht="15" customHeight="1">
       <c r="C90" s="39"/>
@@ -8309,46 +8370,46 @@
       <c r="R90" s="38"/>
       <c r="S90" s="38"/>
       <c r="T90" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U90" s="38"/>
       <c r="V90" s="38"/>
       <c r="W90" s="40"/>
-      <c r="X90" s="107" t="s">
-        <v>117</v>
-      </c>
-      <c r="Y90" s="108"/>
-      <c r="Z90" s="108"/>
-      <c r="AA90" s="108"/>
-      <c r="AB90" s="108"/>
-      <c r="AC90" s="108"/>
-      <c r="AD90" s="108"/>
-      <c r="AE90" s="108"/>
-      <c r="AF90" s="108"/>
-      <c r="AG90" s="108"/>
-      <c r="AH90" s="108"/>
-      <c r="AI90" s="108"/>
-      <c r="AJ90" s="108"/>
-      <c r="AK90" s="108"/>
-      <c r="AL90" s="108"/>
-      <c r="AM90" s="108"/>
-      <c r="AN90" s="108"/>
-      <c r="AO90" s="108"/>
-      <c r="AP90" s="108"/>
-      <c r="AQ90" s="108"/>
-      <c r="AR90" s="108"/>
-      <c r="AS90" s="108"/>
-      <c r="AT90" s="108"/>
-      <c r="AU90" s="108"/>
-      <c r="AV90" s="108"/>
-      <c r="AW90" s="108"/>
-      <c r="AX90" s="108"/>
-      <c r="AY90" s="108"/>
-      <c r="AZ90" s="108"/>
-      <c r="BA90" s="108"/>
-      <c r="BB90" s="108"/>
-      <c r="BC90" s="108"/>
-      <c r="BD90" s="109"/>
+      <c r="X90" s="106" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y90" s="107"/>
+      <c r="Z90" s="107"/>
+      <c r="AA90" s="107"/>
+      <c r="AB90" s="107"/>
+      <c r="AC90" s="107"/>
+      <c r="AD90" s="107"/>
+      <c r="AE90" s="107"/>
+      <c r="AF90" s="107"/>
+      <c r="AG90" s="107"/>
+      <c r="AH90" s="107"/>
+      <c r="AI90" s="107"/>
+      <c r="AJ90" s="107"/>
+      <c r="AK90" s="107"/>
+      <c r="AL90" s="107"/>
+      <c r="AM90" s="107"/>
+      <c r="AN90" s="107"/>
+      <c r="AO90" s="107"/>
+      <c r="AP90" s="107"/>
+      <c r="AQ90" s="107"/>
+      <c r="AR90" s="107"/>
+      <c r="AS90" s="107"/>
+      <c r="AT90" s="107"/>
+      <c r="AU90" s="107"/>
+      <c r="AV90" s="107"/>
+      <c r="AW90" s="107"/>
+      <c r="AX90" s="107"/>
+      <c r="AY90" s="107"/>
+      <c r="AZ90" s="107"/>
+      <c r="BA90" s="107"/>
+      <c r="BB90" s="107"/>
+      <c r="BC90" s="107"/>
+      <c r="BD90" s="108"/>
     </row>
     <row r="91" spans="3:56" ht="15" customHeight="1">
       <c r="C91" s="39"/>
@@ -8373,46 +8434,46 @@
       <c r="R91" s="38"/>
       <c r="S91" s="38"/>
       <c r="T91" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U91" s="38"/>
       <c r="V91" s="38"/>
       <c r="W91" s="40"/>
-      <c r="X91" s="107" t="s">
-        <v>118</v>
-      </c>
-      <c r="Y91" s="108"/>
-      <c r="Z91" s="108"/>
-      <c r="AA91" s="108"/>
-      <c r="AB91" s="108"/>
-      <c r="AC91" s="108"/>
-      <c r="AD91" s="108"/>
-      <c r="AE91" s="108"/>
-      <c r="AF91" s="108"/>
-      <c r="AG91" s="108"/>
-      <c r="AH91" s="108"/>
-      <c r="AI91" s="108"/>
-      <c r="AJ91" s="108"/>
-      <c r="AK91" s="108"/>
-      <c r="AL91" s="108"/>
-      <c r="AM91" s="108"/>
-      <c r="AN91" s="108"/>
-      <c r="AO91" s="108"/>
-      <c r="AP91" s="108"/>
-      <c r="AQ91" s="108"/>
-      <c r="AR91" s="108"/>
-      <c r="AS91" s="108"/>
-      <c r="AT91" s="108"/>
-      <c r="AU91" s="108"/>
-      <c r="AV91" s="108"/>
-      <c r="AW91" s="108"/>
-      <c r="AX91" s="108"/>
-      <c r="AY91" s="108"/>
-      <c r="AZ91" s="108"/>
-      <c r="BA91" s="108"/>
-      <c r="BB91" s="108"/>
-      <c r="BC91" s="108"/>
-      <c r="BD91" s="109"/>
+      <c r="X91" s="106" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y91" s="107"/>
+      <c r="Z91" s="107"/>
+      <c r="AA91" s="107"/>
+      <c r="AB91" s="107"/>
+      <c r="AC91" s="107"/>
+      <c r="AD91" s="107"/>
+      <c r="AE91" s="107"/>
+      <c r="AF91" s="107"/>
+      <c r="AG91" s="107"/>
+      <c r="AH91" s="107"/>
+      <c r="AI91" s="107"/>
+      <c r="AJ91" s="107"/>
+      <c r="AK91" s="107"/>
+      <c r="AL91" s="107"/>
+      <c r="AM91" s="107"/>
+      <c r="AN91" s="107"/>
+      <c r="AO91" s="107"/>
+      <c r="AP91" s="107"/>
+      <c r="AQ91" s="107"/>
+      <c r="AR91" s="107"/>
+      <c r="AS91" s="107"/>
+      <c r="AT91" s="107"/>
+      <c r="AU91" s="107"/>
+      <c r="AV91" s="107"/>
+      <c r="AW91" s="107"/>
+      <c r="AX91" s="107"/>
+      <c r="AY91" s="107"/>
+      <c r="AZ91" s="107"/>
+      <c r="BA91" s="107"/>
+      <c r="BB91" s="107"/>
+      <c r="BC91" s="107"/>
+      <c r="BD91" s="108"/>
     </row>
     <row r="92" spans="3:56" ht="15" customHeight="1">
       <c r="C92" s="39"/>
@@ -8437,46 +8498,46 @@
       <c r="R92" s="38"/>
       <c r="S92" s="38"/>
       <c r="T92" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U92" s="38"/>
       <c r="V92" s="38"/>
       <c r="W92" s="40"/>
-      <c r="X92" s="107" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y92" s="108"/>
-      <c r="Z92" s="108"/>
-      <c r="AA92" s="108"/>
-      <c r="AB92" s="108"/>
-      <c r="AC92" s="108"/>
-      <c r="AD92" s="108"/>
-      <c r="AE92" s="108"/>
-      <c r="AF92" s="108"/>
-      <c r="AG92" s="108"/>
-      <c r="AH92" s="108"/>
-      <c r="AI92" s="108"/>
-      <c r="AJ92" s="108"/>
-      <c r="AK92" s="108"/>
-      <c r="AL92" s="108"/>
-      <c r="AM92" s="108"/>
-      <c r="AN92" s="108"/>
-      <c r="AO92" s="108"/>
-      <c r="AP92" s="108"/>
-      <c r="AQ92" s="108"/>
-      <c r="AR92" s="108"/>
-      <c r="AS92" s="108"/>
-      <c r="AT92" s="108"/>
-      <c r="AU92" s="108"/>
-      <c r="AV92" s="108"/>
-      <c r="AW92" s="108"/>
-      <c r="AX92" s="108"/>
-      <c r="AY92" s="108"/>
-      <c r="AZ92" s="108"/>
-      <c r="BA92" s="108"/>
-      <c r="BB92" s="108"/>
-      <c r="BC92" s="108"/>
-      <c r="BD92" s="109"/>
+      <c r="X92" s="106" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y92" s="107"/>
+      <c r="Z92" s="107"/>
+      <c r="AA92" s="107"/>
+      <c r="AB92" s="107"/>
+      <c r="AC92" s="107"/>
+      <c r="AD92" s="107"/>
+      <c r="AE92" s="107"/>
+      <c r="AF92" s="107"/>
+      <c r="AG92" s="107"/>
+      <c r="AH92" s="107"/>
+      <c r="AI92" s="107"/>
+      <c r="AJ92" s="107"/>
+      <c r="AK92" s="107"/>
+      <c r="AL92" s="107"/>
+      <c r="AM92" s="107"/>
+      <c r="AN92" s="107"/>
+      <c r="AO92" s="107"/>
+      <c r="AP92" s="107"/>
+      <c r="AQ92" s="107"/>
+      <c r="AR92" s="107"/>
+      <c r="AS92" s="107"/>
+      <c r="AT92" s="107"/>
+      <c r="AU92" s="107"/>
+      <c r="AV92" s="107"/>
+      <c r="AW92" s="107"/>
+      <c r="AX92" s="107"/>
+      <c r="AY92" s="107"/>
+      <c r="AZ92" s="107"/>
+      <c r="BA92" s="107"/>
+      <c r="BB92" s="107"/>
+      <c r="BC92" s="107"/>
+      <c r="BD92" s="108"/>
     </row>
     <row r="93" spans="3:56" ht="15" customHeight="1">
       <c r="C93" s="39"/>
@@ -8501,46 +8562,46 @@
       <c r="R93" s="38"/>
       <c r="S93" s="38"/>
       <c r="T93" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U93" s="38"/>
       <c r="V93" s="38"/>
       <c r="W93" s="40"/>
-      <c r="X93" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y93" s="161"/>
-      <c r="Z93" s="161"/>
-      <c r="AA93" s="161"/>
-      <c r="AB93" s="161"/>
-      <c r="AC93" s="161"/>
-      <c r="AD93" s="161"/>
-      <c r="AE93" s="161"/>
-      <c r="AF93" s="161"/>
-      <c r="AG93" s="161"/>
-      <c r="AH93" s="161"/>
-      <c r="AI93" s="161"/>
-      <c r="AJ93" s="161"/>
-      <c r="AK93" s="161"/>
-      <c r="AL93" s="161"/>
-      <c r="AM93" s="161"/>
-      <c r="AN93" s="161"/>
-      <c r="AO93" s="161"/>
-      <c r="AP93" s="161"/>
-      <c r="AQ93" s="161"/>
-      <c r="AR93" s="161"/>
-      <c r="AS93" s="161"/>
-      <c r="AT93" s="161"/>
-      <c r="AU93" s="161"/>
-      <c r="AV93" s="161"/>
-      <c r="AW93" s="161"/>
-      <c r="AX93" s="161"/>
-      <c r="AY93" s="161"/>
-      <c r="AZ93" s="161"/>
-      <c r="BA93" s="161"/>
-      <c r="BB93" s="161"/>
-      <c r="BC93" s="161"/>
-      <c r="BD93" s="162"/>
+      <c r="X93" s="167" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y93" s="168"/>
+      <c r="Z93" s="168"/>
+      <c r="AA93" s="168"/>
+      <c r="AB93" s="168"/>
+      <c r="AC93" s="168"/>
+      <c r="AD93" s="168"/>
+      <c r="AE93" s="168"/>
+      <c r="AF93" s="168"/>
+      <c r="AG93" s="168"/>
+      <c r="AH93" s="168"/>
+      <c r="AI93" s="168"/>
+      <c r="AJ93" s="168"/>
+      <c r="AK93" s="168"/>
+      <c r="AL93" s="168"/>
+      <c r="AM93" s="168"/>
+      <c r="AN93" s="168"/>
+      <c r="AO93" s="168"/>
+      <c r="AP93" s="168"/>
+      <c r="AQ93" s="168"/>
+      <c r="AR93" s="168"/>
+      <c r="AS93" s="168"/>
+      <c r="AT93" s="168"/>
+      <c r="AU93" s="168"/>
+      <c r="AV93" s="168"/>
+      <c r="AW93" s="168"/>
+      <c r="AX93" s="168"/>
+      <c r="AY93" s="168"/>
+      <c r="AZ93" s="168"/>
+      <c r="BA93" s="168"/>
+      <c r="BB93" s="168"/>
+      <c r="BC93" s="168"/>
+      <c r="BD93" s="169"/>
     </row>
     <row r="94" spans="3:56" ht="15" customHeight="1">
       <c r="C94" s="39"/>
@@ -8565,46 +8626,46 @@
       <c r="R94" s="38"/>
       <c r="S94" s="38"/>
       <c r="T94" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U94" s="38"/>
       <c r="V94" s="38"/>
       <c r="W94" s="40"/>
-      <c r="X94" s="160" t="s">
-        <v>121</v>
-      </c>
-      <c r="Y94" s="161"/>
-      <c r="Z94" s="161"/>
-      <c r="AA94" s="161"/>
-      <c r="AB94" s="161"/>
-      <c r="AC94" s="161"/>
-      <c r="AD94" s="161"/>
-      <c r="AE94" s="161"/>
-      <c r="AF94" s="161"/>
-      <c r="AG94" s="161"/>
-      <c r="AH94" s="161"/>
-      <c r="AI94" s="161"/>
-      <c r="AJ94" s="161"/>
-      <c r="AK94" s="161"/>
-      <c r="AL94" s="161"/>
-      <c r="AM94" s="161"/>
-      <c r="AN94" s="161"/>
-      <c r="AO94" s="161"/>
-      <c r="AP94" s="161"/>
-      <c r="AQ94" s="161"/>
-      <c r="AR94" s="161"/>
-      <c r="AS94" s="161"/>
-      <c r="AT94" s="161"/>
-      <c r="AU94" s="161"/>
-      <c r="AV94" s="161"/>
-      <c r="AW94" s="161"/>
-      <c r="AX94" s="161"/>
-      <c r="AY94" s="161"/>
-      <c r="AZ94" s="161"/>
-      <c r="BA94" s="161"/>
-      <c r="BB94" s="161"/>
-      <c r="BC94" s="161"/>
-      <c r="BD94" s="162"/>
+      <c r="X94" s="167" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y94" s="168"/>
+      <c r="Z94" s="168"/>
+      <c r="AA94" s="168"/>
+      <c r="AB94" s="168"/>
+      <c r="AC94" s="168"/>
+      <c r="AD94" s="168"/>
+      <c r="AE94" s="168"/>
+      <c r="AF94" s="168"/>
+      <c r="AG94" s="168"/>
+      <c r="AH94" s="168"/>
+      <c r="AI94" s="168"/>
+      <c r="AJ94" s="168"/>
+      <c r="AK94" s="168"/>
+      <c r="AL94" s="168"/>
+      <c r="AM94" s="168"/>
+      <c r="AN94" s="168"/>
+      <c r="AO94" s="168"/>
+      <c r="AP94" s="168"/>
+      <c r="AQ94" s="168"/>
+      <c r="AR94" s="168"/>
+      <c r="AS94" s="168"/>
+      <c r="AT94" s="168"/>
+      <c r="AU94" s="168"/>
+      <c r="AV94" s="168"/>
+      <c r="AW94" s="168"/>
+      <c r="AX94" s="168"/>
+      <c r="AY94" s="168"/>
+      <c r="AZ94" s="168"/>
+      <c r="BA94" s="168"/>
+      <c r="BB94" s="168"/>
+      <c r="BC94" s="168"/>
+      <c r="BD94" s="169"/>
     </row>
     <row r="95" spans="3:56" ht="15" customHeight="1">
       <c r="C95" s="39"/>
@@ -8629,46 +8690,46 @@
       <c r="R95" s="38"/>
       <c r="S95" s="38"/>
       <c r="T95" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U95" s="38"/>
       <c r="V95" s="38"/>
       <c r="W95" s="40"/>
-      <c r="X95" s="107" t="s">
-        <v>122</v>
-      </c>
-      <c r="Y95" s="108"/>
-      <c r="Z95" s="108"/>
-      <c r="AA95" s="108"/>
-      <c r="AB95" s="108"/>
-      <c r="AC95" s="108"/>
-      <c r="AD95" s="108"/>
-      <c r="AE95" s="108"/>
-      <c r="AF95" s="108"/>
-      <c r="AG95" s="108"/>
-      <c r="AH95" s="108"/>
-      <c r="AI95" s="108"/>
-      <c r="AJ95" s="108"/>
-      <c r="AK95" s="108"/>
-      <c r="AL95" s="108"/>
-      <c r="AM95" s="108"/>
-      <c r="AN95" s="108"/>
-      <c r="AO95" s="108"/>
-      <c r="AP95" s="108"/>
-      <c r="AQ95" s="108"/>
-      <c r="AR95" s="108"/>
-      <c r="AS95" s="108"/>
-      <c r="AT95" s="108"/>
-      <c r="AU95" s="108"/>
-      <c r="AV95" s="108"/>
-      <c r="AW95" s="108"/>
-      <c r="AX95" s="108"/>
-      <c r="AY95" s="108"/>
-      <c r="AZ95" s="108"/>
-      <c r="BA95" s="108"/>
-      <c r="BB95" s="108"/>
-      <c r="BC95" s="108"/>
-      <c r="BD95" s="109"/>
+      <c r="X95" s="106" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y95" s="107"/>
+      <c r="Z95" s="107"/>
+      <c r="AA95" s="107"/>
+      <c r="AB95" s="107"/>
+      <c r="AC95" s="107"/>
+      <c r="AD95" s="107"/>
+      <c r="AE95" s="107"/>
+      <c r="AF95" s="107"/>
+      <c r="AG95" s="107"/>
+      <c r="AH95" s="107"/>
+      <c r="AI95" s="107"/>
+      <c r="AJ95" s="107"/>
+      <c r="AK95" s="107"/>
+      <c r="AL95" s="107"/>
+      <c r="AM95" s="107"/>
+      <c r="AN95" s="107"/>
+      <c r="AO95" s="107"/>
+      <c r="AP95" s="107"/>
+      <c r="AQ95" s="107"/>
+      <c r="AR95" s="107"/>
+      <c r="AS95" s="107"/>
+      <c r="AT95" s="107"/>
+      <c r="AU95" s="107"/>
+      <c r="AV95" s="107"/>
+      <c r="AW95" s="107"/>
+      <c r="AX95" s="107"/>
+      <c r="AY95" s="107"/>
+      <c r="AZ95" s="107"/>
+      <c r="BA95" s="107"/>
+      <c r="BB95" s="107"/>
+      <c r="BC95" s="107"/>
+      <c r="BD95" s="108"/>
     </row>
     <row r="96" spans="3:56" ht="15" customHeight="1">
       <c r="C96" s="39"/>
@@ -8693,46 +8754,46 @@
       <c r="R96" s="38"/>
       <c r="S96" s="38"/>
       <c r="T96" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U96" s="38"/>
       <c r="V96" s="38"/>
       <c r="W96" s="40"/>
-      <c r="X96" s="160" t="s">
-        <v>124</v>
-      </c>
-      <c r="Y96" s="161"/>
-      <c r="Z96" s="161"/>
-      <c r="AA96" s="161"/>
-      <c r="AB96" s="161"/>
-      <c r="AC96" s="161"/>
-      <c r="AD96" s="161"/>
-      <c r="AE96" s="161"/>
-      <c r="AF96" s="161"/>
-      <c r="AG96" s="161"/>
-      <c r="AH96" s="161"/>
-      <c r="AI96" s="161"/>
-      <c r="AJ96" s="161"/>
-      <c r="AK96" s="161"/>
-      <c r="AL96" s="161"/>
-      <c r="AM96" s="161"/>
-      <c r="AN96" s="161"/>
-      <c r="AO96" s="161"/>
-      <c r="AP96" s="161"/>
-      <c r="AQ96" s="161"/>
-      <c r="AR96" s="161"/>
-      <c r="AS96" s="161"/>
-      <c r="AT96" s="161"/>
-      <c r="AU96" s="161"/>
-      <c r="AV96" s="161"/>
-      <c r="AW96" s="161"/>
-      <c r="AX96" s="161"/>
-      <c r="AY96" s="161"/>
-      <c r="AZ96" s="161"/>
-      <c r="BA96" s="161"/>
-      <c r="BB96" s="161"/>
-      <c r="BC96" s="161"/>
-      <c r="BD96" s="162"/>
+      <c r="X96" s="167" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y96" s="168"/>
+      <c r="Z96" s="168"/>
+      <c r="AA96" s="168"/>
+      <c r="AB96" s="168"/>
+      <c r="AC96" s="168"/>
+      <c r="AD96" s="168"/>
+      <c r="AE96" s="168"/>
+      <c r="AF96" s="168"/>
+      <c r="AG96" s="168"/>
+      <c r="AH96" s="168"/>
+      <c r="AI96" s="168"/>
+      <c r="AJ96" s="168"/>
+      <c r="AK96" s="168"/>
+      <c r="AL96" s="168"/>
+      <c r="AM96" s="168"/>
+      <c r="AN96" s="168"/>
+      <c r="AO96" s="168"/>
+      <c r="AP96" s="168"/>
+      <c r="AQ96" s="168"/>
+      <c r="AR96" s="168"/>
+      <c r="AS96" s="168"/>
+      <c r="AT96" s="168"/>
+      <c r="AU96" s="168"/>
+      <c r="AV96" s="168"/>
+      <c r="AW96" s="168"/>
+      <c r="AX96" s="168"/>
+      <c r="AY96" s="168"/>
+      <c r="AZ96" s="168"/>
+      <c r="BA96" s="168"/>
+      <c r="BB96" s="168"/>
+      <c r="BC96" s="168"/>
+      <c r="BD96" s="169"/>
     </row>
     <row r="97" spans="3:56" ht="15" customHeight="1">
       <c r="C97" s="39"/>
@@ -8757,46 +8818,46 @@
       <c r="R97" s="38"/>
       <c r="S97" s="38"/>
       <c r="T97" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U97" s="38"/>
       <c r="V97" s="38"/>
       <c r="W97" s="40"/>
-      <c r="X97" s="160" t="s">
-        <v>125</v>
-      </c>
-      <c r="Y97" s="161"/>
-      <c r="Z97" s="161"/>
-      <c r="AA97" s="161"/>
-      <c r="AB97" s="161"/>
-      <c r="AC97" s="161"/>
-      <c r="AD97" s="161"/>
-      <c r="AE97" s="161"/>
-      <c r="AF97" s="161"/>
-      <c r="AG97" s="161"/>
-      <c r="AH97" s="161"/>
-      <c r="AI97" s="161"/>
-      <c r="AJ97" s="161"/>
-      <c r="AK97" s="161"/>
-      <c r="AL97" s="161"/>
-      <c r="AM97" s="161"/>
-      <c r="AN97" s="161"/>
-      <c r="AO97" s="161"/>
-      <c r="AP97" s="161"/>
-      <c r="AQ97" s="161"/>
-      <c r="AR97" s="161"/>
-      <c r="AS97" s="161"/>
-      <c r="AT97" s="161"/>
-      <c r="AU97" s="161"/>
-      <c r="AV97" s="161"/>
-      <c r="AW97" s="161"/>
-      <c r="AX97" s="161"/>
-      <c r="AY97" s="161"/>
-      <c r="AZ97" s="161"/>
-      <c r="BA97" s="161"/>
-      <c r="BB97" s="161"/>
-      <c r="BC97" s="161"/>
-      <c r="BD97" s="162"/>
+      <c r="X97" s="167" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y97" s="168"/>
+      <c r="Z97" s="168"/>
+      <c r="AA97" s="168"/>
+      <c r="AB97" s="168"/>
+      <c r="AC97" s="168"/>
+      <c r="AD97" s="168"/>
+      <c r="AE97" s="168"/>
+      <c r="AF97" s="168"/>
+      <c r="AG97" s="168"/>
+      <c r="AH97" s="168"/>
+      <c r="AI97" s="168"/>
+      <c r="AJ97" s="168"/>
+      <c r="AK97" s="168"/>
+      <c r="AL97" s="168"/>
+      <c r="AM97" s="168"/>
+      <c r="AN97" s="168"/>
+      <c r="AO97" s="168"/>
+      <c r="AP97" s="168"/>
+      <c r="AQ97" s="168"/>
+      <c r="AR97" s="168"/>
+      <c r="AS97" s="168"/>
+      <c r="AT97" s="168"/>
+      <c r="AU97" s="168"/>
+      <c r="AV97" s="168"/>
+      <c r="AW97" s="168"/>
+      <c r="AX97" s="168"/>
+      <c r="AY97" s="168"/>
+      <c r="AZ97" s="168"/>
+      <c r="BA97" s="168"/>
+      <c r="BB97" s="168"/>
+      <c r="BC97" s="168"/>
+      <c r="BD97" s="169"/>
     </row>
     <row r="98" spans="3:56" ht="15" customHeight="1">
       <c r="C98" s="39"/>
@@ -8821,46 +8882,46 @@
       <c r="R98" s="38"/>
       <c r="S98" s="38"/>
       <c r="T98" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="U98" s="38"/>
       <c r="V98" s="38"/>
       <c r="W98" s="40"/>
-      <c r="X98" s="160" t="s">
-        <v>123</v>
-      </c>
-      <c r="Y98" s="161"/>
-      <c r="Z98" s="161"/>
-      <c r="AA98" s="161"/>
-      <c r="AB98" s="161"/>
-      <c r="AC98" s="161"/>
-      <c r="AD98" s="161"/>
-      <c r="AE98" s="161"/>
-      <c r="AF98" s="161"/>
-      <c r="AG98" s="161"/>
-      <c r="AH98" s="161"/>
-      <c r="AI98" s="161"/>
-      <c r="AJ98" s="161"/>
-      <c r="AK98" s="161"/>
-      <c r="AL98" s="161"/>
-      <c r="AM98" s="161"/>
-      <c r="AN98" s="161"/>
-      <c r="AO98" s="161"/>
-      <c r="AP98" s="161"/>
-      <c r="AQ98" s="161"/>
-      <c r="AR98" s="161"/>
-      <c r="AS98" s="161"/>
-      <c r="AT98" s="161"/>
-      <c r="AU98" s="161"/>
-      <c r="AV98" s="161"/>
-      <c r="AW98" s="161"/>
-      <c r="AX98" s="161"/>
-      <c r="AY98" s="161"/>
-      <c r="AZ98" s="161"/>
-      <c r="BA98" s="161"/>
-      <c r="BB98" s="161"/>
-      <c r="BC98" s="161"/>
-      <c r="BD98" s="162"/>
+      <c r="X98" s="167" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y98" s="168"/>
+      <c r="Z98" s="168"/>
+      <c r="AA98" s="168"/>
+      <c r="AB98" s="168"/>
+      <c r="AC98" s="168"/>
+      <c r="AD98" s="168"/>
+      <c r="AE98" s="168"/>
+      <c r="AF98" s="168"/>
+      <c r="AG98" s="168"/>
+      <c r="AH98" s="168"/>
+      <c r="AI98" s="168"/>
+      <c r="AJ98" s="168"/>
+      <c r="AK98" s="168"/>
+      <c r="AL98" s="168"/>
+      <c r="AM98" s="168"/>
+      <c r="AN98" s="168"/>
+      <c r="AO98" s="168"/>
+      <c r="AP98" s="168"/>
+      <c r="AQ98" s="168"/>
+      <c r="AR98" s="168"/>
+      <c r="AS98" s="168"/>
+      <c r="AT98" s="168"/>
+      <c r="AU98" s="168"/>
+      <c r="AV98" s="168"/>
+      <c r="AW98" s="168"/>
+      <c r="AX98" s="168"/>
+      <c r="AY98" s="168"/>
+      <c r="AZ98" s="168"/>
+      <c r="BA98" s="168"/>
+      <c r="BB98" s="168"/>
+      <c r="BC98" s="168"/>
+      <c r="BD98" s="169"/>
     </row>
     <row r="99" spans="3:56" ht="15" customHeight="1">
       <c r="C99" s="39"/>
@@ -8885,46 +8946,46 @@
       <c r="R99" s="38"/>
       <c r="S99" s="38"/>
       <c r="T99" s="38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="U99" s="38"/>
       <c r="V99" s="38"/>
       <c r="W99" s="40"/>
-      <c r="X99" s="160" t="s">
+      <c r="X99" s="167" t="s">
         <v>78</v>
       </c>
-      <c r="Y99" s="161"/>
-      <c r="Z99" s="161"/>
-      <c r="AA99" s="161"/>
-      <c r="AB99" s="161"/>
-      <c r="AC99" s="161"/>
-      <c r="AD99" s="161"/>
-      <c r="AE99" s="161"/>
-      <c r="AF99" s="161"/>
-      <c r="AG99" s="161"/>
-      <c r="AH99" s="161"/>
-      <c r="AI99" s="161"/>
-      <c r="AJ99" s="161"/>
-      <c r="AK99" s="161"/>
-      <c r="AL99" s="161"/>
-      <c r="AM99" s="161"/>
-      <c r="AN99" s="161"/>
-      <c r="AO99" s="161"/>
-      <c r="AP99" s="161"/>
-      <c r="AQ99" s="161"/>
-      <c r="AR99" s="161"/>
-      <c r="AS99" s="161"/>
-      <c r="AT99" s="161"/>
-      <c r="AU99" s="161"/>
-      <c r="AV99" s="161"/>
-      <c r="AW99" s="161"/>
-      <c r="AX99" s="161"/>
-      <c r="AY99" s="161"/>
-      <c r="AZ99" s="161"/>
-      <c r="BA99" s="161"/>
-      <c r="BB99" s="161"/>
-      <c r="BC99" s="161"/>
-      <c r="BD99" s="162"/>
+      <c r="Y99" s="168"/>
+      <c r="Z99" s="168"/>
+      <c r="AA99" s="168"/>
+      <c r="AB99" s="168"/>
+      <c r="AC99" s="168"/>
+      <c r="AD99" s="168"/>
+      <c r="AE99" s="168"/>
+      <c r="AF99" s="168"/>
+      <c r="AG99" s="168"/>
+      <c r="AH99" s="168"/>
+      <c r="AI99" s="168"/>
+      <c r="AJ99" s="168"/>
+      <c r="AK99" s="168"/>
+      <c r="AL99" s="168"/>
+      <c r="AM99" s="168"/>
+      <c r="AN99" s="168"/>
+      <c r="AO99" s="168"/>
+      <c r="AP99" s="168"/>
+      <c r="AQ99" s="168"/>
+      <c r="AR99" s="168"/>
+      <c r="AS99" s="168"/>
+      <c r="AT99" s="168"/>
+      <c r="AU99" s="168"/>
+      <c r="AV99" s="168"/>
+      <c r="AW99" s="168"/>
+      <c r="AX99" s="168"/>
+      <c r="AY99" s="168"/>
+      <c r="AZ99" s="168"/>
+      <c r="BA99" s="168"/>
+      <c r="BB99" s="168"/>
+      <c r="BC99" s="168"/>
+      <c r="BD99" s="169"/>
     </row>
     <row r="100" spans="3:56">
       <c r="C100" s="39"/>
@@ -9039,7 +9100,7 @@
       <c r="BD101" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="90">
+  <mergeCells count="105">
     <mergeCell ref="X97:BD97"/>
     <mergeCell ref="X98:BD98"/>
     <mergeCell ref="X99:BD99"/>
@@ -9054,21 +9115,24 @@
     <mergeCell ref="X90:BD90"/>
     <mergeCell ref="X96:BD96"/>
     <mergeCell ref="X88:BD88"/>
-    <mergeCell ref="AU23:AZ24"/>
-    <mergeCell ref="BA23:BA24"/>
+    <mergeCell ref="X73:AD73"/>
+    <mergeCell ref="AE73:AK73"/>
+    <mergeCell ref="X74:AD74"/>
+    <mergeCell ref="AE74:AK74"/>
+    <mergeCell ref="AL74:BD74"/>
+    <mergeCell ref="X75:AD75"/>
+    <mergeCell ref="AE75:AK75"/>
+    <mergeCell ref="AL75:BD75"/>
     <mergeCell ref="X70:AD70"/>
     <mergeCell ref="AE70:AK70"/>
     <mergeCell ref="E71:Q71"/>
     <mergeCell ref="X71:AD71"/>
     <mergeCell ref="AE71:AK71"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="O4:T4"/>
-    <mergeCell ref="O5:T5"/>
-    <mergeCell ref="AQ4:AS4"/>
-    <mergeCell ref="AQ5:AS5"/>
-    <mergeCell ref="F4:N4"/>
-    <mergeCell ref="U4:AP4"/>
+    <mergeCell ref="AW43:BD43"/>
+    <mergeCell ref="F23:G24"/>
+    <mergeCell ref="H23:I24"/>
+    <mergeCell ref="J23:P24"/>
+    <mergeCell ref="Q23:W24"/>
     <mergeCell ref="C7:H7"/>
     <mergeCell ref="C41:G41"/>
     <mergeCell ref="C67:J67"/>
@@ -9083,18 +9147,9 @@
     <mergeCell ref="D10:G15"/>
     <mergeCell ref="H10:U15"/>
     <mergeCell ref="AQ43:AV43"/>
-    <mergeCell ref="AW43:BD43"/>
     <mergeCell ref="X23:AA24"/>
     <mergeCell ref="H22:L22"/>
-    <mergeCell ref="F23:G24"/>
-    <mergeCell ref="H23:I24"/>
-    <mergeCell ref="J23:P24"/>
-    <mergeCell ref="Q23:W24"/>
-    <mergeCell ref="L20:M20"/>
-    <mergeCell ref="O20:P20"/>
-    <mergeCell ref="AN20:AR20"/>
-    <mergeCell ref="AV20:AZ20"/>
-    <mergeCell ref="AP12:AR13"/>
+    <mergeCell ref="AU23:AZ24"/>
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="E69:Q69"/>
     <mergeCell ref="AT12:AV13"/>
@@ -9111,11 +9166,30 @@
     <mergeCell ref="R69:W69"/>
     <mergeCell ref="X69:AD69"/>
     <mergeCell ref="AE69:AK69"/>
+    <mergeCell ref="L20:M20"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="AN20:AR20"/>
+    <mergeCell ref="AV20:AZ20"/>
+    <mergeCell ref="AP12:AR13"/>
+    <mergeCell ref="BA23:BA24"/>
     <mergeCell ref="C88:D88"/>
     <mergeCell ref="E88:Q88"/>
     <mergeCell ref="R88:W88"/>
     <mergeCell ref="E70:Q70"/>
     <mergeCell ref="E72:Q72"/>
+    <mergeCell ref="E73:Q73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="E74:Q74"/>
+    <mergeCell ref="R74:W74"/>
+    <mergeCell ref="E75:Q75"/>
+    <mergeCell ref="R75:W75"/>
+    <mergeCell ref="B2:D3"/>
+    <mergeCell ref="E2:AP3"/>
+    <mergeCell ref="AQ2:AW2"/>
+    <mergeCell ref="AX2:BE2"/>
+    <mergeCell ref="AQ3:AW3"/>
+    <mergeCell ref="AX3:BE3"/>
     <mergeCell ref="AT4:AW4"/>
     <mergeCell ref="BB4:BE4"/>
     <mergeCell ref="F5:N5"/>
@@ -9124,12 +9198,14 @@
     <mergeCell ref="BB5:BE5"/>
     <mergeCell ref="AX4:BA4"/>
     <mergeCell ref="AX5:BA5"/>
-    <mergeCell ref="B2:D3"/>
-    <mergeCell ref="E2:AP3"/>
-    <mergeCell ref="AQ2:AW2"/>
-    <mergeCell ref="AX2:BE2"/>
-    <mergeCell ref="AQ3:AW3"/>
-    <mergeCell ref="AX3:BE3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="O4:T4"/>
+    <mergeCell ref="O5:T5"/>
+    <mergeCell ref="AQ4:AS4"/>
+    <mergeCell ref="AQ5:AS5"/>
+    <mergeCell ref="F4:N4"/>
+    <mergeCell ref="U4:AP4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="87" orientation="portrait" r:id="rId1"/>

</xml_diff>